<commit_message>
Added try catch to fix failed runs, new output version
</commit_message>
<xml_diff>
--- a/data/final/v3output.xlsx
+++ b/data/final/v3output.xlsx
@@ -481,7 +481,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>so I think we are fine to get started and the first thing on the agenda is the first thing on our agenda is a message from Dr Philip ormondsey I should have used this slide I'm just realizing that sorry I hear that thing I've said all of that all right thanks yeah thank you very much and thank you for hosting this Market engagement event welcome everyone to this event we're really delighted to have you here it's great to see that CCS Crown commercial service and hmrc a collaborating on such an important activity not just for hmrc but for the oil of government Legacy migration Legacy encapsulation Legacy remediation is quite topical right now most of what we spend in government you know goes to where is managing our Legacy estate so it's really good to see us working collaboratively with hmrc to</t>
+          <t>So, I think we are fine to get started and the first thing on the agenda is a message from Dr. Philip Ormondsey. I should have used this slide, I'm just realizing that. Sorry, I hear that thing I've said all of that. All right, thanks. Yeah, thank you very much and thank you for hosting this Market Engagement Event. Welcome everyone to this event. We're really delighted to have you here. It's great to see that CCS (Crown Commercial Service) and HMRC are collaborating on such an important activity, not just for HMRC but for the whole of government. Legacy migration, Legacy encapsulation, Legacy remediation is quite topical right now. Most of what we spend in government, you know, goes to managing our Legacy estate. So, it's really good to see us working collaboratively with HMRC to do this.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -491,17 +491,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['CCS', 'HMRC', 'Legacy', 'Remediation', 'Encapsulation']</t>
+          <t>['Legacy', 'Migration', 'HMRC', 'CCS', 'Government']</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="H2" t="n">
         <v>0.2</v>
@@ -513,7 +513,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>launch this this framework ccs and Andrew tomasi through the creation of our Dallas agreement supports the public sector strategic approach to migrating from Legacy applications and we're hoping that our partners will support us again in this in this in this venture to ensure that we do this right but do it at a cost effective and valid delivery process Dallas will offer an easy approach to assist in the provision of more cost effective and innovative solutions again not just for HMR see but for the oil of government so my team and the team at the hmrc are looking forward to hearing from you all on this approach and on how we can ensure the success of yet another CCS agreement please listening to the conversations that our teams are going to be having with you this morning and continue the</t>
+          <t>Launch this framework, CCS and Andrew Tomasi, through the creation of our Dallas agreement, supports the public sector's strategic approach to migrating from Legacy applications. We're hoping that our partners will support us again in this venture to ensure that we do this right, but do it at a cost effective and valid delivery process. Dallas will offer an easy approach to assist in the provision of more cost effective and innovative solutions, again not just for HMR see but for the whole of government. So, my team and the team at the HMRC are looking forward to hearing from you all on this approach and on how we can ensure the success of yet another CCS agreement. Please listen to the conversations that our teams are going to be having with you this morning and continue the discussion.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -523,20 +523,20 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['launch', 'framework', 'CCS', 'Andrew', 'Tomasi', 'Legacy', 'applications', 'HMR', 'government', 'CCS agreement']</t>
+          <t>['CCS', 'Legacy Applications', 'HMRC', 'Cost Effective', 'Innovative Solutions']</t>
         </is>
       </c>
       <c r="E3" t="n">
         <v>0.5</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H3" t="n">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="4">
@@ -545,7 +545,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>dialogue and the engagement and I wish I wish you know all participants in this engagement are very successful event thank you very much for attending and hopefully hope to see or speak or interact with you all pretty soon thank you right thank you Philip and well thanks to everybody for coming I'd like to make a welcome from hmrc to everybody both in the room and online it's still a still a bit of a novelty as they're seeing everybody back face to face and it is it's absolutely great to see so thank you very much for that and I'm going to give an introduction to why why we're doing this why is hmrc with our friends in CTS building this framework and what's the purpose so this is really the vehicle for the next stage in the technology sourcing program tsp hopefully most of you in the room will have heard of tsp we'll have a knowledge of of tsp but what effectively tsp is is bringing the brain back in to</t>
+          <t>Dialogue and the engagement, and I wish, I wish you know all participants in this engagement are very successful event. Thank you very much for attending and hopefully hope to see or speak or interact with you all pretty soon. Thank you right. Thank you Philip and well thanks to everybody for coming. I'd like to make a welcome from HMRC to everybody both in the room and online. It's still a still a bit of a novelty as they're seeing everybody back face to face and it is it's absolutely great to see so thank you very much for that. And I'm going to give an introduction to why why we're doing this, why is HMRC with our friends in CTS building this framework and what's the purpose? So this is really the vehicle for the next stage in the technology sourcing program TSP. Hopefully most of you in the room will have heard of TSP, we'll have a knowledge of of TSP, but what effectively TSP is is bringing the brain back in to.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -555,17 +555,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['dialogue', 'engagement', 'HMRC', 'CTS', 'framework']</t>
+          <t>['HMRC', 'CTS', 'TSP', 'Dialogue', 'Engagement']</t>
         </is>
       </c>
       <c r="E4" t="n">
         <v>0.7</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="H4" t="n">
         <v>0.2</v>
@@ -577,17 +577,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>hmrc we've been outsourced for a long long time and a lot of the knowledge has sat with third-party suppliers tsp is all about bringing the brain back in and so far what have we done we've done the disaggregation of the contracts but that's very much the start of tsp it is not what tsp is about so the disaggregation so far has been taking those big monolithic outsourced contracts and breaking them up into smaller contracts but what we've done is we've taken one of Monopoly contracts easy for me to say and we've broken them down into much smaller Monopoly contracts and we've done that for a couple of reasons the mature of hmrc didn't enable us to go from where we were to where we want to be in one jump and also we had time constraints to get us to where we needed to be so Dallas is going to provide us that next level of contract vehicle to get the maturity of hmrc to help build that intelligent client to help us take the</t>
+          <t>HMRC has been outsourced for a long time and a lot of the knowledge has sat with third-party suppliers. TSP is all about bringing the brain back in and so far, what have we done? We've done the disaggregation of the contracts, but that's very much the start of TSP. It is not what TSP is about. So, the disaggregation so far has been taking those big monolithic outsourced contracts and breaking them up into smaller contracts. But what we've done is we've taken one of Monopoly contracts and we've broken them down into much smaller Monopoly contracts. And we've done that for a couple of reasons: the maturity of HMRC didn't enable us to go from where we were to where we want to be in one jump, and also we had time constraints to get us to where we needed to be. So, Dallas is going to provide us that next level of contract vehicle to get the maturity of HMRC to help build that intelligent client to help us take the next step.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>HMRC Outsourcing</t>
+          <t>Outsourcing Knowledge</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>['HMRC', 'Outsourcing', 'TSP', 'Disaggregation', 'Monopoly', 'Contracts']</t>
+          <t>['HMRC', 'TSP', 'Monopoly', 'Disaggregation', 'Dallas']</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -597,10 +597,10 @@
         <v>0.7</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="H5" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="6">
@@ -609,27 +609,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>applications and our services to the next level so there's three main aims of Dallas they all begin with C which makes it nice and easy to remember capability its capacity and its competition what Dallas aims to do is down select a smaller group of suppliers who will have the confidence that they are going to get significant work from hmrc so they are able to invest in hmrc really getting to know hmrc and provide the best quality of service to hmrc having multiple providers though gives us the best capacity I don't think I've ever known such squeeze on capacity as we have right now so relying on two smaller number of suppliers puts it at risk and I think we've just seen across lots of areas over the last 12 24 months how important diversity in the supply chain is and this will help us with that as well and then finally competition</t>
+          <t>Applications and our services to the next level, so there's three main aims of Dallas: they all begin with C, which makes it nice and easy to remember - capability, capacity, and competition. What Dallas aims to do is down select a smaller group of suppliers who will have the confidence that they are going to get significant work from HMRC, so they are able to invest in HMRC, really getting to know HMRC and provide the best quality of service to HMRC. Having multiple providers though gives us the best capacity. I don't think I've ever known such squeeze on capacity as we have right now, so relying on two smaller number of suppliers puts it at risk, and I think we've just seen across lots of areas over the last 12-24 months how important diversity in the supply chain is, and this will help us with that as well. Finally, competition.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Dallas Aims</t>
+          <t>Supply Chain</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>['applications', 'services', 'suppliers', 'capacity', 'competition']</t>
+          <t>['HMRC', 'Capacity', 'Competition', 'Diversity', 'Investment']</t>
         </is>
       </c>
       <c r="E6" t="n">
         <v>0.5</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="H6" t="n">
         <v>0.2</v>
@@ -641,7 +641,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>small number of suppliers that are pre-down selected means that we can keep competition helps Drive value for money or we can also do it quicker so instead of having to run procurements it takes months through the Dallas framework we should be able to turn things around in a matter of weeks so they're the three main drivers you'll get some more detail today and this is the first of of a whole string of of Market engagement so we really do want to hear your thoughts as well at the end of it we've got some questions but we also have follow-up sessions so I'm now going to hand over to Mike thank you Lee good morning all my name is Mike Hannan I'm the category lead within CCS for technology Services cyber and Technology transport and our my team will be looking after the Dallas framework and making sure that goes live yeah and we're really pleased to be working with hmrc as Philip said to get this off the road because we think it's a good good idea a good way of bringing</t>
+          <t>A small number of suppliers that are pre-down selected means that we can keep competition, which helps drive value for money. Or, we can also do it quicker. So, instead of having to run procurements that take months through the Dallas framework, we should be able to turn things around in a matter of weeks. These are the three main drivers. You'll get some more detail today and this is the first of a whole string of market engagement. We really do want to hear your thoughts as well. At the end of it, we've got some questions, but we also have follow-up sessions. I'm now going to hand over to Mike. Thank you, Lee. Good morning, all. My name is Mike Hannan. I'm the category lead within CCS for technology services, cyber and technology transport, and my team will be looking after the Dallas framework and making sure that goes live. Yeah, and we're really pleased to be working with HMRC, as Philip said, to get this off the road because we think it's a good idea, a good way of bringing things together.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -651,20 +651,20 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>['suppliers', 'value', 'money', 'procurements', 'Market engagement', 'Mike Hannan', 'CCS', 'Technology Services', 'cyber', 'Technology transport']</t>
+          <t>['suppliers', 'procurements', 'market engagement', 'HMRC', 'Mike Hannan']</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="G7" t="n">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="H7" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8">
@@ -673,17 +673,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>in and changing the way the the Legacy services are developed and maintained okay just Sean to the next slide so this is what we think the the lighting structure looks like we're pretty sure this is about how we're going to look forward against a little bit more detail of the lot names and what goes through and and Phil we'll go through more of those in the level of detail why they're there for supported hmrc and clearly this is we've been talking to other government departments as well and they are looking to do something very similar to this so we're trying to build this so it's a capability that's available for all government departments okay so as as Lee said we're trying to look at the rationalize the number of suppliers across each of the lots to ensure that we got the the right suppliers in there the right competition the right capabilities to align those so you know we will go into further detail around that ecosystem it this more or less aligns</t>
+          <t>In and changing the way the Legacy services are developed and maintained. Okay, just Sean to the next slide. So, this is what we think the lighting structure looks like. We're pretty sure this is about how we're going to look forward against a little bit more detail of the lot names and what goes through and and Phil we'll go through more of those in the level of detail why they're there for supported hmrc. And, clearly this is we've been talking to other government departments as well and they are looking to do something very similar to this. So, we're trying to build this so it's a capability that's available for all government departments. Okay, so as Lee said, we're trying to look at the rationalize the number of suppliers across each of the lots to ensure that we got the right suppliers in there, the right competition, the right capabilities to align those. So, you know we will go into further detail around that ecosystem it this more or less aligns.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Lighting Structure</t>
+          <t>Government services</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>['Legacy services', 'government departments', 'suppliers', 'competition', 'capabilities']</t>
+          <t>['Legacy services', 'lighting structure', 'lot names', 'hmrc', 'government departments', 'suppliers', 'competition', 'capabilities', 'ecosystem']</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -705,30 +705,30 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>to what are the type of suppliers we're looking for within those areas and and Phil again we'll go into more detail around what they look like and why we've got them there we just flip onto the next slide so I'm not going to go through all the level of details within there's a lot of detail on there but but effectively this is a design service aspect for lot one we're looking at the support and the delivery aspects for that design design activity okay until okay and this is the larger scale integration and development services so we're looking for large-scale organizations to support this these were very larger values across the the programs of activity hmrc will be putting out and we move on to 2B and these are the for the smaller SME level suppliers with this lower level lower value but you know still great capability that need to support hmrc and other Supply and other customers on okay lot three is integration and run</t>
+          <t>To what are the type of suppliers we're looking for within those areas? And Phil again, we'll go into more detail around what they look like and why we've got them there. We just flip onto the next slide, so I'm not going to go through all the level of details within. There's a lot of detail on there, but effectively this is a design service aspect for Lot One. We're looking at the support and the delivery aspects for that design design activity. Okay, until okay. And this is the larger scale integration and development services. So, we're looking for large-scale organizations to support this. These were very larger values across the programs of activity HMRC will be putting out. And we move on to 2B and these are the for the smaller SME level suppliers with this lower level lower value, but you know still great capability that need to support HMRC and other Supply and other customers on. Okay, Lot Three is integration and run.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Supplier Types</t>
+          <t>Supplier selection</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>['Suppliers', 'Design', 'Integration', 'Development', 'SME']</t>
+          <t>['HMRC', 'SME', 'Integration', 'Development', 'Design']</t>
         </is>
       </c>
       <c r="E9" t="n">
         <v>0.5</v>
       </c>
       <c r="F9" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G9" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="H9" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="10">
@@ -737,7 +737,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Services you know there's nothing new there the these These are still required again large-scale suppliers they are big platforms big activities they're going through that will need supporting configuration Services again lot 4A is the larger scale Prime aspects with ecosystems of suppliers supporting this this service again lots of the the normal activities that you'd expect within the configuration service and and until up 4B and 4B we talk about the The Specialist so we're back into an SME environment of how that and what that helps deliver in smaller programs smaller projects activities and again it would all be aligned through as one one activity for for hmrc so they can manage all of the supply base and we look at the other customers are looking for that as well yeah if we move on to five and this is a capability pipeline for Academy trading as Lee said you've lost lost</t>
+          <t>Services you know there's nothing new there. The these These are still required again large-scale suppliers they are big platforms big activities they're going through that will need supporting configuration Services again. Lot 4A is the larger scale Prime aspects with ecosystems of suppliers supporting this this service again. Lots of the the normal activities that you'd expect within the configuration service and and until up 4B and 4B we talk about the The Specialist so we're back into an SME environment of how that and what that helps deliver in smaller programs smaller projects activities and again it would all be aligned through as one one activity for for hmrc so they can manage all of the supply base and we look at the other customers are looking for that as well. Yeah if we move on to five and this is a capability pipeline for Academy trading as Lee said you've lost lost.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -747,7 +747,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>['Services', 'configuration', 'SME', 'supply base', 'Academy']</t>
+          <t>['Services', 'Configuration', 'Suppliers', 'SME', 'hmrc']</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -769,7 +769,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>knowledge lost a capabilities within the organization and this is then building up and putting back in that knowledge within hmrc and we know this from lots of other government partners that are this is also required it's something that is missing and they want to bring back from all their years of Outsourcing I'm going to head over to Phil now to just go into what the next aspects looks like in terms of what they think the value is going through the the framework at this level for hmrc good morning I'm Phil desbrie associate director for it commercial my particular focus is as the commercial lead for hmrc for the Dallas project delivering that alongside our colleagues in CCS if we can move on to the next slide you'll see an expanded view here of the last instructor that Mike's already shown you so just to explain this in a bit more detail so when we were conceptualizing this model we started to look at some of the challenges and problems that hmrc faced</t>
+          <t>Knowledge was lost in capabilities within the organization, and this was then building up and putting back in that knowledge within HMRC. We know this from lots of other government partners that this is also required; it's something that is missing, and they want to bring back from all their years of Outsourcing. I'm going to head over to Phil now to just go into what the next aspects looks like in terms of what they think the value is going through the framework at this level for HMRC. Good morning, I'm Phil Desbrie, associate director for IT Commercial. My particular focus is as the commercial lead for HMRC for the Dallas project, delivering that alongside our colleagues in CCS. If we can move on to the next slide, you'll see an expanded view here of the last instructor that Mike's already shown you. So, just to explain this in a bit more detail, when we were conceptualizing this model, we started to look at some of the challenges and problems that HMRC faced.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -779,7 +779,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>['knowledge', 'capabilities', 'Outsourcing', 'value', 'framework', 'commercial']</t>
+          <t>['Knowledge', 'Outsourcing', 'HMRC', 'Dallas Project', 'CCS']</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -789,10 +789,10 @@
         <v>0.7</v>
       </c>
       <c r="G11" t="n">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="H11" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="12">
@@ -801,7 +801,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>so in the digital space for example digital development we had a situation where we had a very small number of suppliers who had to be assigned to do one particular piece of activity so we didn't have ongoing competitive tension and we struggled to adopt the GDs approach to Rainbow teams where you would have individuals from multiple suppliers working together to deliver the same types of things and when we have been able to do that with an hmrc what that's tended to mean is that you've had a hmrc person looking after that rainbow team and therefore the risk for delivery all stays with hmrc rather than being transferred into the market so we started off with that as a strategic problem and then started to build around this as to what the loss instructor should look like so as Mike's already pointed out we have some large-scale suppliers operating in the digital space today what we want to do is bolster that capability by bringing in opportunities for smaller suppliers smes of course but</t>
+          <t>So, in the digital space, for example digital development, we had a situation where we had a very small number of suppliers who had to be assigned to do one particular piece of activity, so we didn't have ongoing competitive tension and we struggled to adopt the GDs approach to Rainbow teams, where you would have individuals from multiple suppliers working together to deliver the same types of things. And when we have been able to do that with an HMRC, what that's tended to mean is that you've had an HMRC person looking after that Rainbow team and therefore the risk for delivery all stays with HMRC rather than being transferred into the market. So, we started off with that as a strategic problem and then started to build around this as to what the loss instructor should look like. So, as Mike's already pointed out, we have some large-scale suppliers operating in the digital space today. What we want to do is bolster that capability by bringing in opportunities for smaller suppliers, SMEs of course, but...</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -811,7 +811,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>['Digital', 'Suppliers', 'Rainbow Teams', 'HMRC', 'Loss Instructor', 'Large-Scale Suppliers', 'SMEs']</t>
+          <t>['Digital', 'HMRC', 'Rainbow Teams', 'Suppliers', 'SMEs']</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -833,27 +833,27 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>we're not being restrictive about that and in lap 2A and 2B one of the restrictions we are going to make is that if for the suppliers that bid they cannot be on both Lots so that will give us the opportunity to have a nice mix of both larger suppliers and smaller suppliers lot 3 which will also be delivered as part of the first wave of competition activity as Mike said is largely based on the Legacy run services that exist today so you will you will already know from TSP we've competed things like corporation tax we've competed things like child Benefit services and real-time information those services are going to be ultimately within that lot but you'll also see services that currently exist in borders and trade in that lot the services that we have retained with some incumbent suppliers that cover things like self-assessment that cover paye that cover banking services over time they will start to exit those contracts and will also drop into this framework as a means of procuring those</t>
+          <t>We're not being restrictive about that and in Lap 2A and 2B one of the restrictions we are going to make is that if for the suppliers that bid they cannot be on both Lots so that will give us the opportunity to have a nice mix of both larger suppliers and smaller suppliers. Lot 3, which will also be delivered as part of the first wave of competition activity as Mike said, is largely based on the Legacy run services that exist today. So, you will already know from TSP, we've competed things like Corporation Tax, we've competed things like Child Benefit services and Real-Time Information. Those services are going to be ultimately within that Lot, but you'll also see services that currently exist in Borders and Trade in that Lot. The services that we have retained with some incumbent suppliers that cover things like Self-Assessment, that cover PAYE, that cover Banking services, over time they will start to exit those contracts and will also drop into this framework as a means of procuring those.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Government Services</t>
+          <t>Procurement Framework</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>['Legacy', 'TSP', 'Corporation Tax', 'Child Benefit', 'Real-Time Information', 'Borders', 'Trade', 'Self-Assessment', 'PAYE', 'Banking']</t>
+          <t>['Suppliers', 'Lots', 'Legacy', 'TSP', 'Corporation Tax', 'Child Benefit', 'Real-Time Information', 'Borders', 'Trade', 'Self-Assessment', 'PAYE', 'Banking']</t>
         </is>
       </c>
       <c r="E13" t="n">
         <v>0.5</v>
       </c>
       <c r="F13" t="n">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="G13" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="H13" t="n">
         <v>0.2</v>
@@ -865,27 +865,27 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>services and when you think about the number of suppliers that we've we've put here as our aspiration that's very much focused on the point that Lee made about very rapid competition so what you can expect to see as we go through this process and we'll describe it in a bit more detail later in the presentation is to take steps to robustly pre-qualify the suppliers that we appoint on the basis of their capacity their capability their ability to work together with other suppliers and the reason we need that is because when we have a trusted supplier group we are then able to share much more information with that trusted supplier group with the best will in the world and for all of the wonderful things that CCS has done with their Frameworks it's impossible for us to be able to share the level of information that we have with 150 suppliers on tech services three or three thousand suppliers on dos if we have a smaller group of suppliers we can be much more open about our pipelines we could be much more open about our architecture about our</t>
+          <t>Services, and when you think about the number of suppliers that we've we've put here as our aspiration, that's very much focused on the point that Lee made about very rapid competition. So, what you can expect to see as we go through this process, and we'll describe it in a bit more detail later in the presentation, is to take steps to robustly pre-qualify the suppliers that we appoint on the basis of their capacity, their capability, their ability to work together with other suppliers. And the reason we need that is because when we have a trusted supplier group, we are then able to share much more information with that trusted supplier group. With the best will in the world, and for all of the wonderful things that CCS has done with their Frameworks, it's impossible for us to be able to share the level of information that we have with 150 suppliers on tech services three or three thousand suppliers on dos, if we have a smaller group of suppliers we can be much more open about our pipelines, we could be much more open about our architecture about our.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Tech Services</t>
+          <t>Supplier Qualification</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>['services', 'suppliers', 'CCS', 'Frameworks', 'pipelines', 'architecture']</t>
+          <t>['Suppliers', 'CCS', 'Frameworks', 'Pipelines', 'Architecture']</t>
         </is>
       </c>
       <c r="E14" t="n">
         <v>0.5</v>
       </c>
       <c r="F14" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G14" t="n">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="H14" t="n">
         <v>0.2</v>
@@ -897,24 +897,24 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Journeys about what's happening a year in advance when the plans crystallize what's happening three months in advance and that information sharing will enable suppliers to be better placed to respond toward a rapid competition approach so we're anticipating that once this lands we'll be able in a lot of cases particularly in Lots two and four to turn competitions around and around about four to six weeks so it's quite a move from where we are now where we average about 14 weeks for a Dos competition in about five months for a competition through tech services three so quite a difference to what we see today so those suppliers you'll see from the the screen will be required in some cases to have an SME ecosystem with them so that will be in the lot where we are not specifically targeting smes so in Lots 2B and 4B we're giving smes the opportunities to bid there and to try to remove the barriers to entry and as a consequence of that they won't be required to bring an SME ecosystem with them because</t>
+          <t>Journeys about what's happening a year in advance when the plans crystallize what's happening three months in advance and that information sharing will enable suppliers to be better placed to respond toward a rapid competition approach so we're anticipating that once this lands we'll be able in a lot of cases particularly in Lots two and four to turn competitions around and around about four to six weeks so it's quite a move from where we are now where we average about 14 weeks for a Dos competition in about five months for a competition through tech services three so quite a difference to what we see today so those suppliers you'll see from the screen will be required in some cases to have an SME ecosystem with them so that will be in the lot where we are not specifically targeting SMEs so in Lots 2B and 4B we're giving SMEs the opportunities to bid there and to try to remove the barriers to entry and as a consequence of that they won't be required to bring an SME ecosystem with them because</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Information Sharing</t>
+          <t>Competition Plans</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>['Journeys', 'Plans', 'Competition', 'SMEs']</t>
+          <t>['Journeys', 'Plans', 'Suppliers', 'Competitions', 'SMEs']</t>
         </is>
       </c>
       <c r="E15" t="n">
         <v>0.5</v>
       </c>
       <c r="F15" t="n">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="G15" t="n">
         <v>0.7</v>
@@ -929,7 +929,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>that's quite an overhead for an SME anyway to front that for other smes in the lots that aren't specifically targeted at smes there will be some requirements there but we're going to make some changes to what was done within tsp so in tsp we had a requirement of a pass-through of at least 30 percent of revenues to an ecosystem of at least five suppliers in most of the cases what we're going to do in Dallas because we've got the equator SME consideration with those lots is reduce the revenue pass through to 20 to a minimum of three smes so that's perhaps a little bit more different and a little bit more attractive perhaps to some of the bidders the annual values that you see quoted that's a forecast value roughly based on our spend today so it's not a Target and it's not a commitment as such so we just need to position that correctly but that's what we anticipate spending each year over the course of the framework and the total value we've calculated over five years because as with all Frameworks there are certain contracts that you can let up to seven years be on</t>
+          <t>That's quite an overhead for an SME anyway to front that for other SMEs in the lots that aren't specifically targeted at SMEs. There will be some requirements there, but we're going to make some changes to what was done within TSP. So, in TSP, we had a requirement of a pass-through of at least 30 percent of revenues to an ecosystem of at least five suppliers. In most of the cases, what we're going to do in Dallas, because we've got the Equator SME consideration with those lots, is reduce the revenue pass-through to 20 to a minimum of three SMEs. So, that's perhaps a little bit more different and a little bit more attractive perhaps to some of the bidders. The annual values that you see quoted, that's a forecast value roughly based on our spend today. So, it's not a target and it's not a commitment as such. We just need to position that correctly, but that's what we anticipate spending each year over the course of the framework and the total value we've calculated over five years, because as with all frameworks, there are certain contracts that you can let up to seven years be on.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -939,7 +939,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>['SME', 'Revenue', 'Suppliers', 'Bidders', 'Framework']</t>
+          <t>['SME', 'Pass-Through', 'Revenues', 'Ecosystem', 'Suppliers']</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -961,7 +961,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>the expiry of the framework so we're anticipating from a total value point of view that hmrcs spend alone will be in the order of about two billion pounds over the next five years now huge numbers as you can imagine and as Lee said huge pie to be able to go around a number of suppliers that will exist within this framework but thinking about it more broadly and Mike touched on this before and Philip are on Wednesday indeed about the fact that this is a CCS framework the overall value you'll have seen in the pin that was released to the market is four and a half billion which enables access from other government departments to be able to use some of the mechanisms and methods that we'll be using as part of setting this framework up so do we have another slide I'm handing over now to Tom skalach who's going to it's a video message because he can't be here in person today but I hope you'll enjoy this presentation</t>
+          <t>The expiry of the framework, so we're anticipating from a total value point of view that HMRC's spend alone will be in the order of about two billion pounds over the next five years. Now, huge numbers, as you can imagine, and as Lee said, huge pie to be able to go around a number of suppliers that will exist within this framework. But thinking about it more broadly, and Mike touched on this before and Philip are on Wednesday indeed about the fact that this is a CCS framework. The overall value you'll have seen in the PIN that was released to the market is four and a half billion, which enables access from other government departments to be able to use some of the mechanisms and methods that we'll be using as part of setting this framework up. So, do we have another slide? I'm handing over now to Tom Skalach, who's going to it's a video message because he can't be here in person today, but I hope you'll enjoy this presentation.</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -971,17 +971,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>['expiry', 'value', 'suppliers', 'CCS', 'government departments', 'mechanisms']</t>
+          <t>['HMRC', 'CCS', 'Government', 'PIN', 'Tom Skalach']</t>
         </is>
       </c>
       <c r="E17" t="n">
         <v>0.5</v>
       </c>
       <c r="F17" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="H17" t="n">
         <v>0.2</v>
@@ -993,7 +993,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>hi I'm Tom skalach this is me talking about IIT strategy and the relevance to the Dallas framework what are the key principles of the hmrc technology strategy over the next four to five years the next four to five years ultimately we want increased agility reduced risk and a faster time to Market our systems are currently constraining us too much taking us a long time to produce Solutions and we have a lot of risk from Legacy applications and solutions we want to ultimately reduce the amount of applications we've got motor more platform and product based architecture set of platforms and products are produced on top of those we want strategically adopt the use of cloud ideally with as much as as a service as possible ideally software as a service if not platform as a service and below that</t>
+          <t>Hi, I'm Tom Skalach. This is me talking about IIT strategy and the relevance to the Dallas framework. What are the key principles of the HMRC technology strategy over the next four to five years? The next four to five years, ultimately we want increased agility, reduced risk, and a faster time to market. Our systems are currently constraining us too much, taking us a long time to produce solutions, and we have a lot of risk from legacy applications and solutions. We want to ultimately reduce the amount of applications we've got, move towards more platform and product based architecture. A set of platforms and products are produced on top of those. We want to strategically adopt the use of cloud, ideally with as much as as a service as possible, ideally software as a service if not platform as a service, and below that.</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>['HMRC', 'Technology', 'Agility', 'Risk', 'Time to Market']</t>
+          <t>['HMRC', 'Agility', 'Risk', 'Cloud']</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -1013,10 +1013,10 @@
         <v>0.7</v>
       </c>
       <c r="G18" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="H18" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="19">
@@ -1025,27 +1025,27 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>infrastructure as a service ultimately where a vendor can provide a solution to us as a service and we can consume that and we can add the value add for hmrc can deliver on top of that for the products which are most fitting to our business needs and our customers needs we want to remove a lot of those Legacy systems and things that hold us back and things that cause a great deal of technical debts overall as a business we're moving to a more digital business we want to reduce the amount of contact that we've got and we want to have people self-serve and so we want solutions that can enable that and provide those customer facing systems for our customers to to consume the services and interact without taking expensive back office human interaction yeah ultimately we want to simplify we want less customizations ideally the only configurations and ideally not too many of those we want to be working to the systems and of the systems State this is what is common and it's only the particular things that are</t>
+          <t>Infrastructure as a service is ultimately where a vendor can provide a solution to us as a service and we can consume that and we can add the value add for HMRC to deliver on top of that for the products which are most fitting to our business needs and our customers' needs. We want to remove a lot of those legacy systems and things that hold us back and things that cause a great deal of technical debt overall. As a business, we're moving to a more digital business. We want to reduce the amount of contact that we've got and we want to have people self-serve and so we want solutions that can enable that and provide those customer-facing systems for our customers to consume the services and interact without taking expensive back office human interaction. Yeah, ultimately we want to simplify. We want less customizations, ideally the only configurations, and ideally not too many of those. We want to be working to the systems' state; this is what is common and it's only the particular things that are different.</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Digital Business</t>
+          <t>Digital Transformation</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>['infrastructure', 'vendor', 'Legacy', 'systems', 'customizations']</t>
+          <t>['Infrastructure', 'Legacy Systems', 'HMRC', 'Self-Serve', 'Simplify', 'Customizations']</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F19" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="G19" t="n">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="H19" t="n">
         <v>0.2</v>
@@ -1057,7 +1057,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>unique to hmrc that we add on top of those we see low code and no code as a big part of our future both enabling Business Development to be done inside the business and application development to be done there too so they can take power of Their Own Destiny and not be hindered from a core set of people that only know specific Technologies in specific areas we within that we also want the faster time to Market so we can quickly prototype and prove the concept and test out the things that we want to have in the future and see them as a reality rather than just through documents in a long-lived waterfall style development time frame But ultimately really want to be moving away from code and it's just those configurations we want a service-based architecture so we can consume services and data from the applications where it's needed and</t>
+          <t>Unique to HMRC, we add on top of those we see. Low code and no code are a big part of our future, both enabling Business Development to be done inside the business and application development to be done there too, so they can take power of their own destiny and not be hindered from a core set of people that only know specific technologies in specific areas. We also want a faster time to market, so we can quickly prototype and prove the concept and test out the things that we want to have in the future and see them as a reality, rather than just through documents in a long-lived waterfall style development time frame. But ultimately, we really want to be moving away from code and it's just those configurations. We want a service-based architecture, so we can consume services and data from the applications where it's needed.</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>['low code', 'no code', 'Business Development', 'application development', 'time to Market', 'configurations', 'service-based architecture']</t>
+          <t>['HMRC', 'Low Code', 'No Code', 'Business Development', 'Time to Market', 'Service-Based Architecture']</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -1077,10 +1077,10 @@
         <v>0.7</v>
       </c>
       <c r="G20" t="n">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="H20" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="21">
@@ -1089,7 +1089,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>overall together we have an integrated ecosystem that delivers to our customers and business funds so with all this together we get increased agility reduced risk at a faster time to Market what are the key technologies that will enable this journey there are many technologies that fit those characteristics of what I'm described in this as a service World be that software as a service platform as a service or even if they're living on top of an infrastructure as a service and can also offer these kind of low code no code faster time to Market style Solutions examples of these are sap within both the Erp space and also in our tax collection and tax revenue Management Solutions service now a nice and power platforms or be that through service now with its itsm capabilities or other applications</t>
+          <t>Overall, together we have an integrated ecosystem that delivers to our customers and business funds. So, with all this together, we get increased agility, reduced risk, and a faster time to Market. What are the key technologies that will enable this journey? There are many technologies that fit those characteristics of what I'm described in this as a service World, be that software as a service, platform as a service, or even if they're living on top of an infrastructure as a service and can also offer these kind of low code, no code, faster time to Market style Solutions. Examples of these are SAP within both the ERP space and also in our tax collection and tax revenue Management Solutions, ServiceNow, a nice and power platforms, or be that through ServiceNow with its ITSM capabilities or other applications.</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1099,20 +1099,20 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>['agility', 'risk', 'time to Market', 'SaaS', 'PaaS', 'IaaS', 'low code', 'no code', 'SAP', 'Erp', 'tax collection', 'tax revenue Management', 'ServiceNow', 'itsm', 'applications']</t>
+          <t>['SAP', 'ERP', 'ServiceNow', 'ITSM', 'Low Code']</t>
         </is>
       </c>
       <c r="E21" t="n">
         <v>0.5</v>
       </c>
       <c r="F21" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G21" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H21" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="22">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>like nice and power where we can develop on top of those to find to automate in particular areas that are a little bit Niche to us we've got documentum and Pega for managing our documents and our workflow processes as well as also advisor uis and simplified user experiences to both our customer and our internal user we've got AI Services as well making best use of our data Microsoft Dynamics for CRM and other case management cases and uses and products like Kong for our API management which is a key part of our integration moving forward these are just some examples and there are many more thank you what are the key characteristics that we are looking for from the supplier on this framework on supplies on this framework we're</t>
+          <t>Like nice and power, where we can develop on top of those to find to automate in particular areas that are a little bit niche to us. We've got Documentum and Pega for managing our documents and our workflow processes, as well as also advisor UIs and simplified user experiences to both our customer and our internal user. We've got AI Services as well, making best use of our data. Microsoft Dynamics for CRM and other case management cases and uses, and products like Kong for our API management, which is a key part of our integration moving forward. These are just some examples, and there are many more. Thank you. What are the key characteristics that we are looking for from the supplier on this framework? On supplies on this framework, we're</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1131,7 +1131,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>['documentum', 'Pega', 'AI Services', 'Microsoft Dynamics', 'Kong', 'API Management']</t>
+          <t>['Supplier', 'Framework', 'AI Services', 'Microsoft Dynamics', 'Kong']</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1144,7 +1144,7 @@
         <v>0.7</v>
       </c>
       <c r="H22" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="23">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>looking with for suppliers that collaborate with us work really closely be open to be flexible and agile but come with their deep expertise and deep knowledge what they've got in both their product but also where their products being applied within other government departments and in the outside world with one vendors and and suppliers who can continue to learn and learn with us and learn how best to apply these Technologies ultimately we want people who can be outcome based delivered to an outcome that that we set that our business and our customers need and the vendors and system integrators are prepared to take some skin on the game and deliver to the outcome not just the times the materials that could potentially go on forever we want people who want to who can understand hmrc both as an organization and as the systems and ecosystems that we've got in place right now we can't quickly just move to a green field and forget the old we've got we've</t>
+          <t>Looking for suppliers that collaborate with us, work really closely, be open to be flexible and agile, but come with their deep expertise and deep knowledge of what they've got in both their product but also where their products being applied within other government departments and in the outside world. With one vendors and and suppliers who can continue to learn and learn with us and learn how best to apply these Technologies. Ultimately, we want people who can be outcome based, delivered to an outcome that that we set that our business and our customers need. And the vendors and system integrators are prepared to take some skin on the game and deliver to the outcome, not just the times the materials that could potentially go on forever. We want people who want to who can understand HMRC both as an organization and as the systems and ecosystems that we've got in place right now. We can't quickly just move to a green field and forget the old we've got we've.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>['suppliers', 'flexible', 'agile', 'expertise', 'knowledge', 'outcome based']</t>
+          <t>['Suppliers', 'Vendors', 'System Integrators', 'Outcome Based', 'HMRC']</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -1185,12 +1185,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>got to on a journey to coexist both the Legacy and the new and ultimately we want people who can take opportunities from the rest of their ecosystem and bring to us all the knowledge from the other vendors and other suppliers that they work with and other customers and ultimately help hmrc do things faster and better what else are we looking for from suppliers to help us achieve our vision for it the framework is set up to allow suppliers to bring their broad knowledge and experience and learning from other government departments and industries into hmrc that's what we want we want to find a way to implement the best Solutions the fastest time the reduced cost and the reduced risk we want innovators who can help us bring an external perspective see the art of the possible and show us what we're potentially missing out on or what the next stage will be and potentially miss</t>
+          <t>Got to on a journey to coexist both the Legacy and the new and ultimately we want people who can take opportunities from the rest of their ecosystem and bring to us all the knowledge from the other vendors and other suppliers that they work with and other customers and ultimately help HMRC do things faster and better. What else are we looking for from suppliers to help us achieve our vision for it? The framework is set up to allow suppliers to bring their broad knowledge and experience and learning from other government departments and industries into HMRC. That's what we want. We want to find a way to implement the best Solutions the fastest time, the reduced cost and the reduced risk. We want innovators who can help us bring an external perspective, see the art of the possible and show us what we're potentially missing out on or what the next stage will be and potentially miss out on.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>HMRC Vision</t>
+          <t>Innovation &amp; HMRC</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1202,13 +1202,13 @@
         <v>0.5</v>
       </c>
       <c r="F24" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="G24" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="H24" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="25">
@@ -1217,17 +1217,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>a few stages out and find intuitive ways to solving problems not just technology in certain areas okay thank you I'd like to now invite Jillian Bates to give her presentation she's joining online Jillian good morning good morning morning everyone sorry I can't be in the room I couldn't get it's hard as to be in Newcastle and in London at the same time today so you've got me on camera and I'm Julian Bates I'm the deputy director of the digital platform teams within hmrc cdio let me go to the next slide please so a digital platform so what do we do in the digital platform team here in hmrc we basically run all of the customer face and services that we have in the department and we also run the multi-digital tax platform which is the platform in which the services sit on so</t>
+          <t>A few stages out and find intuitive ways to solving problems, not just technology in certain areas. Okay, thank you. I'd like to now invite Jillian Bates to give her presentation. She's joining online. Jillian, good morning! Good morning, everyone. Sorry, I can't be in the room. I couldn't get it's hard as to be in Newcastle and in London at the same time today, so you've got me on camera and I'm Julian Bates. I'm the deputy director of the digital platform teams within HMRC CDIO. Let me go to the next slide please. So, a digital platform. What do we do in the digital platform team here in HMRC? We basically run all of the customer face and services that we have in the department and we also run the multi-digital tax platform, which is the platform in which the services sit on.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Digital Platforms</t>
+          <t>Digital Platform</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>['hmrc', 'customer', 'services', 'digital', 'tax']</t>
+          <t>['HMRC', 'CDIO', 'Digital Platform', 'Tax Platform', 'Customer Services']</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -1249,17 +1249,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>we have the digital channel the digital channels we also have the intelligent Automation and Robotics platform sitting in the digital platform team we have the government Gateway platform we have the customer Insight platform and many others as well and the services that we have are built and run within the digital platform teams they are customer Centric they follow the gdf standards and we built they've built it once ethos through identification of common components across all of the digital channels we have a portfolio of Digital Services as well as the platforms we've got things like the mobile app we've got the G forms we've got iPhones and many many other services including a payment service and the hmrc digital is a brand that gives hmrc the parity with other government departments such as DWP digital and NHS digital as well and the team has been in operation since the beginning of hmrc's digital transformation Journey which was back in 2014 and we have worked with</t>
+          <t>We have the digital channel, the digital channels. We also have the intelligent Automation and Robotics platform sitting in the digital platform team. We have the government Gateway platform, we have the customer Insight platform and many others as well. And the services that we have are built and run within the digital platform teams. They are customer Centric, they follow the GDF standards and we built they've built it once ethos through identification of common components across all of the digital channels. We have a portfolio of Digital Services as well as the platforms. We've got things like the mobile app, we've got the G forms, we've got iPhones and many many other services including a payment service. And the HMRC digital is a brand that gives HMRC the parity with other government departments such as DWP digital and NHS digital as well. And the team has been in operation since the beginning of HMRC's digital transformation Journey which was back in 2014 and we have worked with.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>HMRC Digital</t>
+          <t>Digital Transformation</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>['Digital', 'Automation', 'Robotics', 'Government', 'Customer']</t>
+          <t>['digital', 'HMRC', 'GDF', 'mobile', 'payment']</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1281,27 +1281,27 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>multiple suppliers throughout that journey to get to where we are today to increase our own capability and knowledge and expertise around hmrc's digital Vision next slide please what do we do so we enable the hmrc customer to file serve the tax Affairs through designing and building the cloud hosted hmrc services so like say we started back in 2014 with the first service being the tax credit renewal service and some of the most recent successes that we've had were the corvid schemes for the job retention scheme the self-employment scheme and then more recently this year the new plastic packaging tax scheme as well we designed the digital services for the customers so that they are easy to use and like we say to try and help the customer solve through the tax Affairs as much as possible try and promote the digital take up across the department enhance the systems that we provide support on our digital service by operating the multi-channel digital tax</t>
+          <t>Multiple suppliers throughout that journey to get to where we are today to increase our own capability and knowledge and expertise around HMRC's digital vision. Next slide please. What do we do? So, we enable the HMRC customer to file serve the tax affairs through designing and building the cloud hosted HMRC services. So, like say we started back in 2014 with the first service being the tax credit renewal service and some of the most recent successes that we've had were the Corvid schemes for the job retention scheme, the self-employment scheme and then more recently this year the new plastic packaging tax scheme as well. We designed the digital services for the customers so that they are easy to use and, like we say, to try and help the customer solve through the tax affairs as much as possible, try and promote the digital take up across the department, enhance the systems that we provide support on our digital service by operating the multi-channel digital tax.</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>HMRC Digital Vision</t>
+          <t>HMRC services</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>['hmrc', 'tax', 'digital', 'services', 'customers']</t>
+          <t>['HMRC', 'tax affairs', 'digital services', 'Corvid schemes', 'plastic packaging tax']</t>
         </is>
       </c>
       <c r="E27" t="n">
         <v>0.5</v>
       </c>
       <c r="F27" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G27" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H27" t="n">
         <v>0.2</v>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>platform like I say all services that we build sit on that at the moment connecting with the current head of Duty estate they existing estate the Legacy estate that Tom referred to and our front-end Services connect in there to bring the data in and allow the transactions to proceed through managing customer authentication and agent authentication through the government Gateway and services as well give people the skills to make the most of digital tools and services we work together to support each other in multi-disciplinary teams we work in an agile way and we use scrum and we use kanban across the digital platform teams we improve the quality of the data to make management policy operational and intervention decisions or within the customer inside platform we've got a lot of risk and built in there which helps our customer compliance colleagues and then the culture of continuous Improvement of the services and processes so in the Run side Water Services built and handed over to our run operation in a devops model we continue to iterate all</t>
+          <t>Platform, like I say, all services that we build sit on that at the moment. Connecting with the current head of Duty estate, they existing estate, the Legacy estate that Tom referred to, and our front-end Services connect in there to bring the data in and allow the transactions to proceed through. Managing customer authentication and agent authentication through the government Gateway and services as well, give people the skills to make the most of digital tools and services. We work together to support each other in multi-disciplinary teams. We work in an agile way and we use scrum and we use kanban across the digital platform teams. We improve the quality of the data to make management policy operational and intervention decisions or within the customer inside platform. We've got a lot of risk and built in there which helps our customer compliance colleagues. And then the culture of continuous Improvement of the services and processes. So, in the Run side Water Services built and handed over to our run operation in a devops model. We continue to iterate all.</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1323,7 +1323,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>['services', 'data', 'customer', 'agent', 'government', 'skills', 'multi-disciplinary', 'agile', 'scrum', 'kanban', 'quality']</t>
+          <t>['Platform', 'Services', 'Legacy', 'Government Gateway', 'Skills', 'Multi-disciplinary', 'Agile', 'Scrum', 'Kanban', 'Data']</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -1345,7 +1345,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>services and keep them as up to date as required and also transform internally through intelligent automation like I said we've got the automation delivery Center which is the robotics platform at the moment where we are also headed more towards Ai and we've got quite a large RPA presence on the estate at the moment and we are moving forward again to try and increase the amount of automation that we have in the department to use as many new technologies as possible next slide this is just a picture of the organization within the digital platform teams just to give you some context around the size and scale of what we do and we've got the five digital platform centers which are Edinburgh Newcastle leads tell certain Worthen we've also got the multi-digit tax platform team which is braced in Bristol and at the moment we've got about 250 permanent</t>
+          <t>Services and keep them as up to date as required and also transform internally through intelligent automation. Like I said, we've got the Automation Delivery Center, which is the robotics platform at the moment, where we are also headed more towards AI and we've got quite a large RPA presence on the estate at the moment. We are moving forward again to try and increase the amount of automation that we have in the department to use as many new technologies as possible. Next slide, this is just a picture of the organization within the Digital Platform Teams, just to give you some context around the size and scale of what we do. We've got the five Digital Platform Centers which are Edinburgh, Newcastle, Leeds, Telford, and Worthen. We've also got the Multi-Digit Tax Platform Team which is based in Bristol. At the moment, we've got about 250 permanent employees.</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1355,7 +1355,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>['services', 'automation', 'AI', 'RPA', 'organization']</t>
+          <t>['services', 'automation', 'AI', 'RPA', 'Digital Platforms']</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1377,27 +1377,27 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>hmrc staff and 790 contract supplier staff which are provided through a multiple contract and scheme that we've got on at the moment through tech services two tech services three and through dos five and we currently have around 70 scrum teams delivering a substantial pipeline of projects which includes the EU exit Services the making tax Digital Services and a single customer account services and obviously we had a change in government of change in prime minister sorry yesterday so we are expecting some work to come out of that as well but I say this is just to give you some sort of context of the size of the digital platform team next slide please for our requirements and the future is that Dallas will allow hmrc to procure the suitable skilled supplies to support all aspects of the digital platforms work will be defined based on statements of work which is obviously the work packages Define and set outcomes and</t>
+          <t>HMRC staff and 790 contract supplier staff, which are provided through a multiple contract and scheme that we've got on at the moment through Tech Services 2, Tech Services 3, and through DOS 5, and we currently have around 70 Scrum teams delivering a substantial pipeline of projects which includes the EU Exit Services, the Making Tax Digital Services, and a Single Customer Account Services. And obviously, we had a change in government of change in Prime Minister sorry yesterday, so we are expecting some work to come out of that as well. But I say this is just to give you some sort of context of the size of the Digital Platform Team. Next slide please. For our requirements and the future, Dallas will allow HMRC to procure the suitable skilled supplies to support all aspects of the Digital Platforms work. Will be defined based on statements of work, which is obviously the work packages define and set outcomes and set.</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>HMRC Digital Platform</t>
+          <t>Digital Platforms</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>['HMRC', 'Contract Supplier', 'EU Exit Services', 'Making Tax Digital Services', 'Single Customer Account Services']</t>
+          <t>['HMRC', 'EU Exit', 'Making Tax Digital', 'Single Customer Account']</t>
         </is>
       </c>
       <c r="E30" t="n">
         <v>0.5</v>
       </c>
       <c r="F30" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G30" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H30" t="n">
         <v>0.2</v>
@@ -1409,7 +1409,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>detailed delivery expectations as an example hmrc will expect the supply that demonstrates significant experience of all capability in the following so that includes the Technologies in the tool sets at the moment we use Scala to build our Digital Services we use play and Frameworks mongodb and many others within mdtp within the automation delivery Center at the moment we use nice for our RPA and we've recently brought hyperscience under the estate for intelligent character recognition as well from Aurora's point of view the resources we have aligned to the ddac profession framework which include things like delivery managers product managers user researchers designers and many others and practices and competencies like I said Agile development we use scrum and kanban across the centers at the moment devops and Trust driven development design and user research to develop the</t>
+          <t>HMRC will expect the supply that demonstrates significant experience of all capability in the following, so that includes the Technologies in the tool sets at the moment. We use Scala to build our Digital Services, we use Play and Frameworks, MongoDB and many others within MDTP. Within the Automation Delivery Center at the moment, we use NICE for our RPA and we've recently brought Hyperscience under the estate for Intelligent Character Recognition as well. From Aurora's point of view, the resources we have aligned to the DDAC profession framework which include things like Delivery Managers, Product Managers, User Researchers, Designers and many others. And practices and competencies like Agile Development, we use Scrum and Kanban across the Centers at the moment, DevOps and Trust Driven Development, Design and User Research to develop the.</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>['HMRC', 'Scala', 'Play', 'Frameworks', 'Mongodb']</t>
+          <t>['HMRC', 'Scala', 'Play', 'MongoDB', 'NICE']</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -1441,17 +1441,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>services in line with the UK government service standards complete and user research working with seldom heard groups for example people with access needs all or digital literacy work and line and support and continuous Improvement of our services in language slas and upskill and the internal teams and collaborative work and one of the big things for us in the digital platform team is that when we work with our supplier colleagues is that when you walk into the digital platform team you put your digital platform badge on so for me it should be really difficult to try and work out who was a supplier member starting who was an hmrc permanent member of Staff because of the way we collaborate and the good work and practices we have across the teams and that's a real importance to us next slide Financial approach bring in the requirements looking to cover the following key elements create a diverse and Innovative Supply base looking for suppliers to really</t>
+          <t>Services in line with the UK government service standards, complete and user research working with seldom heard groups (for example, people with access needs, all or digital literacy work, and line and support and continuous improvement of our services in language SLAs and upskill and the internal teams and collaborative work). And one of the big things for us in the Digital Platform Team is that when we work with our supplier colleagues, is that when you walk into the Digital Platform Team, you put your Digital Platform badge on. So, for me, it should be really difficult to try and work out who was a supplier member starting who was an HMRC permanent member of staff, because of the way we collaborate and the good work and practices we have across the teams, and that's a real importance to us. Next slide: Financial approach, bring in the requirements, looking to cover the following key elements: create a diverse and innovative supply base, looking for suppliers to really.</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Digital Platform Team</t>
+          <t>Digital Platform</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>['services', 'user research', 'seldom heard groups', 'access needs', 'digital literacy', 'continuous Improvement', 'language slas', 'upskill', 'internal teams', 'collaborative work', 'Financial approach', 'diverse Supply base', 'Innovative Supply base']</t>
+          <t>['services', 'research', 'suppliers', 'HMRC', 'collaboration', 'financial']</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1473,7 +1473,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>demonstrate how they achieve social value in work pass through in local sourceful impact looking for supply chain transparency that implies supply chain Partnerships in Supply chains to chmrc as an honest broker when Elite suppliers to give their ecosystem supplies the freedom to join multiple Supply chains encourage collaboration and also see a contract management step change that will operate on the basis of openness and honesty and hope that is okay for everybody and that gives you a flavor of what we do in the digital platform teams and I'll be around for any questions in the question and answer session thank you thanks Jillian Richard are you there are you online I am thank you yes yes we can hear you thank you fantastic hi everybody so I'm Richard Aldrich I head up the Enterprise Integration Services team could we move to the next slide please thank you so the Enterprise Integration team develops all the internal and</t>
+          <t>Demonstrate how they achieve social value in work pass through in local sourceful impact looking for supply chain transparency that implies supply chain Partnerships in Supply chains to CHMRC as an honest broker when Elite suppliers to give their ecosystem supplies the freedom to join multiple Supply chains encourage collaboration and also see a contract management step change that will operate on the basis of openness and honesty and hope that is okay for everybody and that gives you a flavor of what we do in the digital platform teams and I'll be around for any questions in the question and answer session. Thank you. Thanks Jillian. Richard, are you there? Are you online? I am, thank you. Yes, yes we can hear you. Thank you, fantastic. Hi everybody, so I'm Richard Aldrich. I head up the Enterprise Integration Services team. Could we move to the next slide please? Thank you.</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1483,17 +1483,17 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>['Supply Chains', 'Supply Chain Partnerships', 'Contract Management', 'Digital Platforms', 'Ecosystem Supplies']</t>
+          <t>['social value', 'supply chain', 'CHMRC', 'Elite suppliers', 'ecosystem supplies', 'contract management', 'digital platform']</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F33" t="n">
         <v>0.3</v>
       </c>
       <c r="G33" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="H33" t="n">
         <v>0.2</v>
@@ -1505,17 +1505,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>external integration within hmrc we we effectively enable internal systems to connect to each other as well as managing externally facing apis and file transfers we utilize on-prem Legacy integration as well as cloud-based services so we're predominantly moving to cloud-based Services now we manage large and complex integration services that support all the tax submissions like things like self-assessment corporation tax and also we support all the core customer services and within the team we do Platform and development support operations management as well as service support we also help and manage the relationship with third-party software companies that build products you utilize our external facing apis and also other government departments that are seeking to exchange data with</t>
+          <t>External integration within HMRC enables internal systems to connect to each other, as well as managing externally facing APIs and file transfers. We utilize on-prem Legacy integration as well as cloud-based services, and are predominantly moving to cloud-based services now. We manage large and complex integration services that support all the tax submissions, like self-assessment and corporation tax. We also support all the core customer services. Within the team, we do Platform and development support, operations management, as well as service support. We also help and manage the relationship with third-party software companies that build products, and utilize our external facing APIs. We also exchange data with other government departments.</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>External Integration</t>
+          <t>Integration Services</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>['HMRC', 'Legacy', 'Cloud-based', 'Tax Submissions', 'Platform', 'Development', 'Operations', 'Service Support', 'Third-Party Software']</t>
+          <t>['HMRC', 'APIs', 'Legacy', 'Cloud', 'Tax', 'Customer Services']</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1537,24 +1537,24 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>hmrc as I said we we own the Strategic relationship with the software industry that build at the third party tax products and we help set up the process of design influenced by policy Eis also enable million billions of pounds of transactions to connect through and be processed by hmrc and we use a a multitude of Technologies most importantly or most recently Open Source Products using and we use agile techniques to do our development okay could we move to the next slide please so we're currently based over four different locations which are leads Telford Bristol and south end we have 140 permanent staff which build which is our intelligent client function so we want to use that to retain our expertise and knowledge within the organization</t>
+          <t>HMRC, as I said, we own the Strategic relationship with the software industry that build at the third party tax products and we help set up the process of design influenced by policy. EIS also enable million billions of pounds of transactions to connect through and be processed by HMRC and we use a multitude of Technologies, most importantly or most recently Open Source Products, using and we use agile techniques to do our development. Okay, could we move to the next slide please? So, we're currently based over four different locations which are Leeds, Telford, Bristol and South End. We have 140 permanent staff which build which is our intelligent client function, so we want to use that to retain our expertise and knowledge within the organization.</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>HMRC Software</t>
+          <t>HMRC Development</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>['HMRC', 'Software', 'Open Source', 'Agile', 'Intelligent Client']</t>
+          <t>['HMRC', 'Software Industry', 'Tax Products', 'Open Source', 'Agile Techniques', 'Intelligent Client']</t>
         </is>
       </c>
       <c r="E35" t="n">
         <v>0.5</v>
       </c>
       <c r="F35" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="G35" t="n">
         <v>0.7</v>
@@ -1569,17 +1569,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>and we're currently also utilize around roughly around about 360 supplier-based staff to do mostly in development and platform support work okay if you come over to the next slide please thank you so how will we utilize the Dallas framework well we require strategic Partners to help us transform our Legacy Services we also need suppliers or the partners to provide platform support to integrate with our existing teams in some cases and provide expertise and also to provide development teams to enable us to increase our pipeline of work we're also looking for a mixed economy of of our contracts of outcomes so some will be fixed price some will be outcome based but essentially what we're trying to do is utilize the skills and expertise from suppliers to help augment</t>
+          <t>And we're currently also utilizing around roughly around about 360 supplier-based staff to do mostly in development and platform support work. Okay, if you come over to the next slide please. Thank you. So, how will we utilize the Dallas framework? Well, we require strategic partners to help us transform our legacy services. We also need suppliers or the partners to provide platform support to integrate with our existing teams in some cases and provide expertise and also to provide development teams to enable us to increase our pipeline of work. We're also looking for a mixed economy of our contracts of outcomes, so some will be fixed price, some will be outcome based, but essentially what we're trying to do is utilize the skills and expertise from suppliers to help augment.</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Dallas Framework</t>
+          <t>Partner Utilization</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>['strategic Partners', 'Legacy Services', 'platform support', 'development teams', 'contracts']</t>
+          <t>['Dallas Framework', 'Legacy Services', 'Platform Support', 'Development Teams', 'Mixed Economy']</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -1601,7 +1601,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>our existing team to help us deliver what we need to do say we're keen to utilize skills and experience so we do have an intelligent client function as I said that is trying to retain the skills and expertise within hmrc but we want to utilize suppliers where they've got additional expertise and knowledge and and help us augment our skills and essentially we want to use the Dallas framework to reduce the number of resources overhead within within the team and also to help with the the burst capability within the team so when we have large demand or a greater demand we want to be able to flex with the suppliers that were brought in via the contracts and we move to the next Sub-Q okay so what are our strategic imperatives well we want to provide more flexible integration services to support future business needs and requirements</t>
+          <t>Our existing team will help us deliver what we need to do. We're keen to utilize skills and experience, so we do have an intelligent client function. As I said, that is trying to retain the skills and expertise within HMRC, but we want to utilize suppliers where they've got additional expertise and knowledge and help us augment our skills. We want to use the Dallas framework to reduce the number of resources overhead within the team and also to help with the burst capability within the team. So, when we have large demand or a greater demand, we want to be able to flex with the suppliers that were brought in via the contracts and we move to the next Sub-Q. Okay, so what are our strategic imperatives? Well, we want to provide more flexible integration services to support future business needs and requirements.</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1611,17 +1611,17 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>['team', 'suppliers', 'Dallas framework', 'resources', 'flexible', 'integration']</t>
+          <t>['flexible', 'suppliers', 'HMRC', 'Dallas', 'Sub-Q']</t>
         </is>
       </c>
       <c r="E37" t="n">
         <v>0.5</v>
       </c>
       <c r="F37" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="G37" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="H37" t="n">
         <v>0.2</v>
@@ -1633,7 +1633,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>and support innovation we want to migrate off of Legacy services that are inflexible expensive to run and don't scale we want to deliver integration faster and more effectively and cheaper and that will be done through API reuse and also through self-serve capabilities so one of the things that we're trying to do at the moment is build a platform that utilizes or creates a self-discovery mechanism and a self-serve Discovery a self self-serve mechanisms that essentially helps us to Federate out delivery so that it's not all confined within the one team within Eis so that we give projects the ability to deliver some of this stuff themselves and also we want to make sure that the products that we did develop and deliver</t>
+          <t>We want to migrate off of legacy services that are inflexible, expensive to run, and don't scale. We want to deliver integration faster, more effectively, and cheaper, and that will be done through API reuse and also through self-serve capabilities. So, one of the things that we're trying to do at the moment is build a platform that utilizes or creates a self-discovery mechanism and a self-serve discovery mechanism that essentially helps us to federate out delivery so that it's not all confined within the one team within EIS. We also want to make sure that the products that we develop and deliver are of high quality.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1643,14 +1643,14 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>['Legacy services', 'Integration', 'Self-serve', 'Federate', 'Delivery']</t>
+          <t>['API', 'Reuse', 'Integration', 'Delivery', 'Self-serve']</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F38" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="G38" t="n">
         <v>0.5</v>
@@ -1665,24 +1665,24 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ensure that we're secure that we meet gdpr and secure customer record standards so the benefits of that as I've described is to provide a self-serve for an internal and external customers we want to be highly scalable and resilient and have a stable set of products we want to simplify our integration footprint so we've got lots of Legacy services that we want to reduce and have much more flexible systems that are cloud-based and we also want to make them more efficient so we want to automate where possible use Auto scaling so that we're cost effective and only utilize resources when we need them and we want to a coherent set of integration patterns that are easily accessible through self-serve and self-discovery that hopefully reduce time to Market and also the amount of development work that we need to do</t>
+          <t>Ensure that we're secure, that we meet GDPR and secure customer record standards. So, the benefits of that, as I've described, is to provide a self-serve for internal and external customers. We want to be highly scalable and resilient, and have a stable set of products. We want to simplify our integration footprint, so we've got lots of legacy services that we want to reduce and have much more flexible systems that are cloud-based. We also want to make them more efficient, so we want to automate where possible, use auto scaling so that we're cost effective and only utilize resources when we need them. And we want to have a coherent set of integration patterns that are easily accessible through self-serve and self-discovery, that hopefully reduce time to market and also the amount of development work that we need to do.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Secure customer records</t>
+          <t>Cloud Automation</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>['GDPR', 'self-serve', 'scalable', 'resilient', 'Legacy services', 'cloud-based', 'automate', 'Auto scaling', 'integration patterns', 'self-discovery', 'time to Market']</t>
+          <t>['security', 'GDPR', 'scalability', 'resilience', 'integration', 'automation', 'cost-effectiveness']</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F39" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="G39" t="n">
         <v>0.8</v>
@@ -1697,7 +1697,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>thank you very much as Julian said I I will also be at the certain question session later on so thank you thanks so much I just want to say quite a few questions already going up on slido so please do stick around because Sarah lots of questions to be answered I'd like to do that great thanks so much is Dean there please Dean I certainly am I'm out okay thanks we can hear you yes okay good hopefully you can you can see see me as well well whether that's good or not I shall I shall leave you to work out okay so only one slide if we can move on to the next slide for only one slide for us I want to talk to you about what borders and trade is in five minutes there's nowhere near enough but I want to give you the flavor of what we do and I think the most important thing to take away is we're we're a CIO group so we Face the business yeah we we use we use riches richer team we</t>
+          <t>Thank you very much, as Julian said. I will also be at the certain question session later on, so thank you. Thanks so much. I just want to say, quite a few questions already going up on Slido, so please do stick around because Sarah has lots of questions to be answered. I'd like to do that. Great, thanks so much. Is Dean there? Please, Dean? I certainly am. I'm out. Okay, thanks. We can hear you. Yes, okay. Good. Hopefully, you can see me as well, well, whether that's good or not, I shall leave you to work out. Okay, so only one slide. If we can move on to the next slide for only one slide for us, I want to talk to you about what borders and trade is in five minutes. There's nowhere near enough, but I want to give you the flavor of what we do. And I think the most important thing to take away is, we're a CIO group, so we face the business. Yeah, we use Richer Team, we use Riches.</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1707,7 +1707,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>['CIO', 'richer team', 'business']</t>
+          <t>['CIO', 'Richer Team', 'Riches']</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1729,17 +1729,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>use we use Jillian's team we use all those other delivery groups to form the services but we build and we run and we Face policy so very much in that front line facing facing the business delivering the services running and building so a couple of things to to call out there are two lenses on us the change lens and they're both big okay I think that's the thing you need to take away with the largest portfolio of I.T change in hmrc now and ever so we do more delivery work than the cdio puts put together within our organization there is a there is a portfolio by the way who am I I'm the portfolio director for change so there's a single program in there which is the largest IT program that HR hmrc or its or its forerunners has ever done that's the biggest all right okay that's the Customs decoration service but everything facing borders and trade the exploitation of EU exit Northern</t>
+          <t>Use we use Jillian's team. We use all those other delivery groups to form the services, but we build and we run and we face policy so very much in that front line facing facing the business delivering the services, running and building. So, a couple of things to to call out there are two lenses on us: the change lens and they're both big. Okay, I think that's the thing you need to take away with the largest portfolio of I.T change in HMRC now and ever. So, we do more delivery work than the CDIO puts put together. Within our organization, there is a there is a portfolio. By the way, who am I? I'm the portfolio director for change. So, there's a single program in there which is the largest IT program that HR HMRC or its or its forerunners has ever done. That's the biggest. All right, okay. That's the Customs Decoration Service, but everything facing borders and trade, the exploitation of EU exit Northern.</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>HMRC Change</t>
+          <t>IT Change</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>["Jillian's team", 'delivery groups', 'change lens', 'largest portfolio', 'IT change', 'CDIO', 'Customs decoration service', 'borders and trade', 'EU exit']</t>
+          <t>['HMRC', 'CDIO', 'Customs Decoration Service', 'EU Exit', 'Northern']</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1749,7 +1749,7 @@
         <v>0.7</v>
       </c>
       <c r="G41" t="n">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="H41" t="n">
         <v>0.2</v>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Ireland protocol changes within our trade structure are us but the Run lens is also important we have Circa 150 160 live Services of a range of Services possibly in this this this might be a little bit flippant but using every tech tech technology over the last 30 40 years not far off Okay so we've got large Legacy estate and our Legacy estate or our our entire estate the new services have real world impacts so the pictures on the right hand side are there to just bring it real okay for an example and this is where we work with with suppliers to inside borders and freight and I will give you some I will give you some numbers now in a minute but we have real world impacts within hours so we can break Kent okay if one or two of our systems one major system goes down the roads in Kent fill up with lorries we Supply services that enables feel that</t>
+          <t>Ireland protocol changes within our trade structure are us, but the Run lens is also important. We have Circa 150-160 live Services of a range of Services, possibly in this. This might be a little bit flippant, but using every tech technology over the last 30-40 years, not far off. Okay, so we've got large Legacy estate and our Legacy estate or our entire estate. The new services have real world impacts, so the pictures on the right hand side are there to just bring it real. Okay, for an example, and this is where we work with suppliers to inside borders and freight, and I will give you some numbers now in a minute. But we have real world impacts within hours, so we can break Kent. Okay, if one or two of our systems, one major system goes down, the roads in Kent fill up with lorries. We Supply services that enables feel that due.</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1771,7 +1771,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>['Ireland', 'Run lens', 'Legacy estate', 'Suppliers', 'Kent']</t>
+          <t>['Ireland', 'Run lens', 'Legacy estate', 'real world impacts', 'Kent']</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -1781,7 +1781,7 @@
         <v>0.8</v>
       </c>
       <c r="G42" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="H42" t="n">
         <v>0.2</v>
@@ -1793,27 +1793,27 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>enables felixstow to work which is the largest container port in in in the UK they have more services than just us but if we get it wrong they seriously suffer and of course Heathrow yeah and ferries and that and that and that channel too tunnel so the scale of the work that that we're doing let me talk a little bit about that over the next three years between run and build it's about one billion pounds worth of of work roughly three quarters of that is in is in change we use over 1 300 staff internals and externals about 800 of those are external Circa the number goes up and down to deliver those services to deliver that change to deliver the live but not just that we use 700 resources Circa in areas such as jillians and Richards who you've just heard heard from and others we have so trying to get over in that five minutes about the opportunities</t>
+          <t>Enables Felixstow to work, which is the largest container port in the UK. They have more services than just us, but if we get it wrong, they seriously suffer - and of course Heathrow, yeah, and ferries and that, and that, and that Channel too tunnel. So, the scale of the work that we're doing - let me talk a little bit about that over the next three years. Between run and build, it's about one billion pounds worth of work, roughly three quarters of that is in change. We use over 1,300 staff, internals and externals - about 800 of those are external, circa. The number goes up and down to deliver those services, to deliver that change, to deliver the live, but not just that - we use 700 resources, circa, in areas such as Jillians and Richards, who you've just heard from, and others. We have, so trying to get over in that five minutes about the opportunities.</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Felixstow Work</t>
+          <t>Work Opportunities</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>['container port', 'Heathrow', 'ferries', 'channel tunnel', 'change', 'jillians', 'Richards']</t>
+          <t>['Felixstow', 'Heathrow', 'Change', 'Live', 'Opportunities']</t>
         </is>
       </c>
       <c r="E43" t="n">
         <v>0.5</v>
       </c>
       <c r="F43" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G43" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="H43" t="n">
         <v>0.2</v>
@@ -1825,7 +1825,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>that are here and and the way we are supported by our supplier partners and they are partners so whereas all our contracts are output based a lot of the services that we provide effectively we are the service integrators so we have rainbow we have rainbow teams of different suppliers performing different roles inside us we are ddat as professions we're PD professions in the main we are across 18 locations within the UK from Glasgow to Belfast to pretty much everywhere else mainly South End and London we as well we've heard a few times we're transforming to intelligent client as the rest of cdio but we need we also need Dallas to assist us not only to build an Iranian output based contracts like I said and burst capacity that not just burst capacity but as a firm partnership with our suppliers to do that build and run but making sure that we are intelligent client to make sure that whilst we use the skills you know</t>
+          <t>That are here, and the way we are supported by our supplier partners, and they are partners, so whereas all our contracts are output based, a lot of the services that we provide, effectively we are the service integrators. So we have rainbow teams of different suppliers performing different roles inside us. We are Ddat as professions, we're PD professions in the main. We are across 18 locations within the UK, from Glasgow to Belfast to pretty much everywhere else, mainly South End and London. We, as well, we've heard a few times, we're transforming to intelligent client as the rest of CDIO, but we need we also need Dallas to assist us, not only to build an Iranian output based contracts like I said, and burst capacity, that not just burst capacity, but as a firm partnership with our suppliers to do that build and run, but making sure that we are intelligent client to make sure that whilst we use the skills, you know.</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1835,7 +1835,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>['Rainbow Teams', 'PD Professions', 'Output Based Contracts', 'Burst Capacity', 'Firm Partnership', 'Build and Run']</t>
+          <t>['suppliers', 'contracts', 'services', 'professions', 'locations', 'CDIO']</t>
         </is>
       </c>
       <c r="E44" t="n">
@@ -1857,27 +1857,27 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>no other no external knows more about our services than we do but that's not simple in sourcing and Outsourcing it's it's not quite as simple as that lastly about the operating environment lens we we support multiple systems of critical National infrastructure so if you're not conversing with that term other examples are the West Coast main main line the M1 but we support the vat data Chief something called gvms which handles flow of lorries and can't go through ports Customs decoration service and Chief and other various custom services but they have they hold a special status within within the UK what we do we also run intelligence systems and services for UK Safety and Security and other ogds pulling that out trade alone is worth it's over this now at 800 billion to the UK our services</t>
+          <t>No other, external knows more about our services than we do, but that's not simple in sourcing and Outsourcing - it's not quite as simple as that. Lastly, about the operating environment lens, we support multiple systems of critical National infrastructure - so if you're not conversing with that term, other examples are the West Coast main line, the M1, but we support the VAT data, Chief, something called GVMS which handles flow of lorries and can't go through ports, Customs decoration service and Chief, and other various custom services, but they have they hold a special status within the UK. What we do, we also run intelligence systems and services for UK Safety and Security and other OGDs. Pulling that out, trade alone is worth over 800 billion to the UK - our services.</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>UK Services</t>
+          <t>UK services</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>['sourcing', 'outsourcing', 'National infrastructure', 'GVMS', 'Customs decoration service', 'UK Safety and Security']</t>
+          <t>['sourcing', 'Outsourcing', 'National infrastructure', 'VAT data', 'GVMS', 'Customs decoration service', 'UK Safety and Security', 'OGDs']</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F45" t="n">
         <v>0.3</v>
       </c>
       <c r="G45" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="H45" t="n">
         <v>0.2</v>
@@ -1889,27 +1889,27 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>collect using Jillian's jilliance teams using Richard's teams but our services as a whole collect over 150 billion in Revenue Dallas framework to us is really important it's the opportunity to continue using external suppliers in a sophisticated way it's a it's it's it's important to us to have those output based com contracts we've we are not only are we in the strange rate the newest CIO but we're also the oldest so we're quite mature in the way that we work with suppliers deeply and in that rainbow way and I will be here for questions I could bang on for days and I have and I have been known to so I shall be here for questions should any occur thank you thank you so much that was really really helpful David Cooper are you are</t>
+          <t>Collect using Jillian's Jilliance teams using Richard's teams, but our services as a whole collect over 150 billion in Revenue. Dallas framework to us is really important. It's the opportunity to continue using external suppliers in a sophisticated way. It's important to us to have those output based com contracts. We're not only in the strange rate, the newest CIO, but we're also the oldest, so we're quite mature in the way that we work with suppliers deeply and in that rainbow way. I will be here for questions. I could bang on for days and I have been known to, so I shall be here for questions should any occur. Thank you so much, that was really really helpful. David Cooper, are you are?</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>External Suppliers</t>
+          <t>Supplier Management</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>["Jillian's teams", "Richard's teams", '150 billion', 'Dallas framework', 'output based com contracts', 'strange rate', 'CIO', 'rainbow way']</t>
+          <t>['Suppliers', 'Contracts', 'CIO', 'Revenue', 'Dallas']</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F46" t="n">
         <v>0.3</v>
       </c>
       <c r="G46" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="H46" t="n">
         <v>0.2</v>
@@ -1921,7 +1921,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>you there yes I am okay everybody so if you could move to the next slide please so my name's Davey Cooper I run the case management delivery group so if we can move on please so who are we we're a group of I.T professionals who use devops ways of working to deliver Pega documentum and Office 365 solutions to our customers we Embrace agile ways of working and our product teams comprise of a mix of perm staff contingent labor and supplier resources we sit inside the hmrc cdio organization so if you could move on to the next slide what do we do so we build enhance and maintain case and content Management Solutions across hmrc used by around about 26 000 staff our products are used by hmrc colleagues in customer services customer compliance and as you just heard in borders and</t>
+          <t>You there? Yes, I am okay everybody. So, if you could move to the next slide please. So, my name's Davey Cooper. I run the case management delivery group. So, if we can move on please. So, who are we? We're a group of I.T professionals who use devops ways of working to deliver Pega documentum and Office 365 solutions to our customers. We embrace agile ways of working and our product teams comprise of a mix of perm staff, contingent labor and supplier resources. We sit inside the hmrc cdio organization. So, if you could move on to the next slide, what do we do? So, we build, enhance and maintain case and content management solutions across hmrc used by around about 26,000 staff. Our products are used by hmrc colleagues in customer services, customer compliance and, as you just heard, in borders and customs.</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1931,7 +1931,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>['devops', 'agile', 'Pega', 'documentum', 'Office 365']</t>
+          <t>['devops', 'agile', 'hmrc', 'Pega', 'documentum', 'Office 365']</t>
         </is>
       </c>
       <c r="E47" t="n">
@@ -1953,17 +1953,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>trade directorates our focus is to utilize the case and content Management Solutions to create a series of products which are built by our teams who are based in Telford Newcastle and Bristol and our teams are responsible for the whole life cycle for a product and we use the Mantra you build it you run it next slide this gives you a view a high level view of how we're organized and it's mainly within our product teams that we utilize supplier resources to help us build and maintain the products that we're responsible for so if you'd like to move on again so what I wanted to do here was just give you a little bit of a feel for the engagement types that we've used today so whilst I can't guarantee future commitments this slide gives you a view of the types of engagements we've undertaken with suppliers using our current agreement so you can see they go from very small short assignments through to quite</t>
+          <t>Trade directorates: Our focus is to utilize the case and content Management Solutions to create a series of products which are built by our teams who are based in Telford, Newcastle, and Bristol. Our teams are responsible for the whole life cycle for a product and we use the mantra: "You build it, you run it." Next slide, this gives you a view a high level view of how we're organized and it's mainly within our product teams that we utilize supplier resources to help us build and maintain the products that we're responsible for. So, if you'd like to move on again, so what I wanted to do here was just give you a little bit of a feel for the engagement types that we've used today. Whilst I can't guarantee future commitments, this slide gives you a view of the types of engagements we've undertaken with suppliers using our current agreement. So, you can see they go from very small short assignments through to quite.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Supplier Engagements</t>
+          <t>Supplier Engagement</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>['trade', 'case', 'content', 'Management', 'Solutions', 'Mantra']</t>
+          <t>['Supplier', 'Engagement', 'Product', 'Mantra', 'Agreement']</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -1985,17 +1985,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>long multi-million pound contract assignments next slide so what am I looking forward to so I'm looking forward to using the Dallas framework to help me meet the demand I have from my customers for new and enhanced case and content Management Solutions my experience today has shown me that by us working together and adopting a one-team approach we're able to keep up with the strong demand I have suppliers are key for me to be able to satisfy this demand and having the ability to tap into a larger capability you all have will be critical for me I see my focus has been on utilizing the lots that are on screen okay and final slide from me so what are my expectations from suppliers well I need to continue to be able to utilize call off agreements for both small and large engagements I will be looking to focus on the technologies that I've listed on screen so Peg a documentum and office 365.</t>
+          <t>Long multi-million pound contract assignments - next slide. So, what am I looking forward to? So, I'm looking forward to using the Dallas framework to help me meet the demand I have from my customers for new and enhanced case and content Management Solutions. My experience today has shown me that by us working together and adopting a one-team approach, we're able to keep up with the strong demand I have. Suppliers are key for me to be able to satisfy this demand and having the ability to tap into a larger capability you all have will be critical for me. I see my focus has been on utilizing the lots that are on screen - okay and final slide from me. So, what are my expectations from suppliers? Well, I need to continue to be able to utilize call off agreements for both small and large engagements. I will be looking to focus on the technologies that I've listed on screen - so Peg, a Documentum and Office 365.</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Case and Content Management</t>
+          <t>Supplier Expectations</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>['Dallas framework', 'call off agreements', 'Peg', 'documentum', 'office 365']</t>
+          <t>['Contracts', 'Dallas Framework', 'Case Management', 'Content Management', 'Suppliers']</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -2005,10 +2005,10 @@
         <v>0.7</v>
       </c>
       <c r="G49" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="H49" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="50">
@@ -2017,27 +2017,27 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>and I'm hoping that we'll be able to continue to utilize our very simple engagement process that we have with you all at the moment so thanks very much and I'm also be here for the Q a session later thank you so much Sarah are you are you there I am indeed hello everyone I'm Sarah Keith so I'm the head of learning and talent development in cdio so my role is to make sure that cdio so our digital directorate and hmrc that we have the necessary skills and capability not only for nine but also for the future so what I'll do is just talk to you a little bit about the work that we do what we've done so far and where we're going in the future so as we've already spoken about you've already heard we have academies in cedio that actually help us deliver professional learning for roles so what this is doing is helping everyone get better at the work that they're doing now but we're not just focused on the here and now as I said we're also</t>
+          <t>I'm hoping that we'll be able to continue to utilize our very simple engagement process that we have with you all at the moment. So, thanks very much and I'm also be here for the Q&amp;A session later. Thank you so much Sarah, are you there? I am indeed. Hello everyone, I'm Sarah Keith. So, I'm the head of Learning and Talent Development in CDIO. So, my role is to make sure that CDIO, our digital directorate and HMRC, that we have the necessary skills and capability not only for now but also for the future. So, what I'll do is just talk to you a little bit about the work that we do, what we've done so far and where we're going in the future. So, as we've already spoken about, you've already heard, we have academies in CDIO that actually help us deliver professional learning for roles. So, what this is doing is helping everyone get better at the work that they're doing now, but we're not just focused on the here and now, as I said, we're also focused on the future.</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Learning and Talent</t>
+          <t>Learning &amp; Development</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>['cdio', 'hmrc', 'academies', 'professional learning', 'future']</t>
+          <t>['CDIO', 'HMRC', 'Academies', 'Professional Learning', 'Future']</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F50" t="n">
         <v>0.3</v>
       </c>
       <c r="G50" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="H50" t="n">
         <v>0.2</v>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>planning for the future as well so one of the key things that we're looking at is how do we help our people develop the skills for the future not only in the role that they're in now but how can we help them transform their careers not only for their own personal benefit but also for the benefit of the organization so how can we use take people whose skills might not be needed quite so much in the future and help them create skills that we are going to need and that are going to be in demand so as I mentioned we've got academies that do that for our roles at the moment we have a university in ceio which is part of my job I lead the university and what that does is it provides the wrapper for the academies we support all the academies we also oversee Learning and Development in cdio in general and the university itself as well as a SharePoint site acts as a One-Stop shop for Learning and the university in fact is the result of a previous collaboration with one of our suppliers so we're very very keen to</t>
+          <t>Planning for the future, so one of the key things that we're looking at is how do we help our people develop the skills for the future, not only in the role that they're in now, but how can we help them transform their careers, not only for their own personal benefit, but also for the benefit of the organization. So, how can we use take people whose skills might not be needed quite so much in the future and help them create skills that we are going to need and that are going to be in demand? So, as I mentioned, we've got academies that do that for our roles at the moment. We have a university in CDIO, which is part of my job. I lead the university and what that does is it provides the wrapper for the academies. We support all the academies, we also oversee Learning and Development in CDIO in general and the university itself, as well as a SharePoint site, acts as a One-Stop shop for Learning. The university in fact is the result of a previous collaboration with one of our suppliers. So, we're very, very keen to.</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2059,20 +2059,20 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>['planning', 'future', 'skills', 'transform', 'academies', 'university', 'Learning', 'Development', 'SharePoint', 'One-Stop shop', 'collaboration']</t>
+          <t>['Learning', 'Development', 'Academies', 'University', 'SharePoint']</t>
         </is>
       </c>
       <c r="E51" t="n">
         <v>0.5</v>
       </c>
       <c r="F51" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G51" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="H51" t="n">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="52">
@@ -2081,30 +2081,30 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>work with you on innovative ways in which we can build capability so we've also mentioned their capability schemes this is something that we're looking at at the moment and we're actually developing them and this is really helping us to leverage our existing talent to help our people transform their careers help cdio develop the capability it needs the future so we're looking at intensive courses you know ways in which we can support people to learn whilst also of course not affecting the work that we do because learning is integral to everything that we do learning is where Innovation comes from so as an I.T organization we need to be learning all the time so it's an integral part of our work nevertheless there's also you know that learning training in particular takes time away from work so we've got to balance the two so it's finding innovative ways to do this and that's really what I'm I'm</t>
+          <t>Work with you on innovative ways in which we can build capability. So, we've also mentioned their capability schemes. This is something that we're looking at at the moment and we're actually developing them and this is really helping us to leverage our existing talent to help our people transform their careers. Help CDIO develop the capability it needs for the future. So, we're looking at intensive courses, you know ways in which we can support people to learn whilst also of course not affecting the work that we do, because learning is integral to everything that we do. Learning is where innovation comes from, so as an I.T organization we need to be learning all the time. So, it's an integral part of our work. Nevertheless, there's also, you know, that learning, training in particular, takes time away from work. So, we've got to balance the two. So, it's finding innovative ways to do this and that's really what I'm I'm.</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Building Capability</t>
+          <t>Learning Innovation</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>['talent', 'transformation', 'learning', 'innovation', 'training']</t>
+          <t>['learning', 'innovation', 'talent', 'transformation', 'capability']</t>
         </is>
       </c>
       <c r="E52" t="n">
         <v>0.5</v>
       </c>
       <c r="F52" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G52" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="H52" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="53">
@@ -2113,7 +2113,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>excited about working with suppliers you know our existing suppliers and new suppliers as well to find different ways of doing that and you know we're quite happy to experiment try new things do all sorts of you know pilot new new ways of doing things so if there's anything that occurs if you think you know we'd like to you know that that you've heard that sort of inspires you hopefully makes you think well yes actually that's something that we could help with that's what I'd like to do and as I said you know we're very much open to suggest questions we're really not fixed in terms of what we're doing but what what is absolutely key to what we do is making sure that we have the skills for the future we are creating cdio in in hmrc as a learning organization so as I said learning is really Central and key to what we do so capability build for us I mean it's incredibly important for me because it's</t>
+          <t>I'm excited about working with suppliers - our existing suppliers and new suppliers as well - to find different ways of doing things. We're quite happy to experiment, try new things, and do all sorts of pilot new ways of doing things. So, if there's anything that occurs to you, if you think we'd like to do something that you've heard that inspires you, hopefully makes you think 'Yes, actually that's something that we could help with', that's what I'd like to do. As I said, we're very much open to suggestions and questions. We're really not fixed in terms of what we're doing, but what is absolutely key to what we do is making sure that we have the skills for the future. We are creating CDIO in HMRC as a learning organization, so learning is really central and key to what we do. So, capability building for us is incredibly important, because it's central.</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2123,20 +2123,20 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>['suppliers', 'experiment', 'pilot', 'questions', 'CDIO']</t>
+          <t>['suppliers', 'experimentation', 'piloting', 'learning', 'CDIO']</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F53" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G53" t="n">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="H53" t="n">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="54">
@@ -2145,7 +2145,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>it's as you can tell I'm very passionate about it it's my job I love Learning and Development I love supporting people to learn but more than that you know making sure the organization has the skills it needs so please you know get your thinking caps on because we really really do encourage any ideas all ideas welcome I will be around for questions later on as well so if you've got any any questions about the work that we're doing now if you'd like to hear any more about any of that then please do do let me know thank you very much thank you and thanks to all the speakers that joined us from online and for keeping to time as well we were a bit concerned about that but I'm happy to welcome for the path so hopefully you'll have picked up from the presentations that were made by the previous speakers that there's a bit of a thread running through the way those stakeholders will consume services so in Lot 2 as we described before we've got a devsecops approach to the delivery of build services and when we talk Dave</t>
+          <t>It's as you can tell I'm very passionate about it. It's my job. I love Learning and Development. I love supporting people to learn, but more than that, you know, making sure the organization has the skills it needs. So please, you know, get your thinking caps on because we really, really do encourage any ideas. All ideas welcome. I will be around for questions later on as well, so if you've got any questions about the work that we're doing now, if you'd like to hear any more about any of that, then please do let me know. Thank you very much. Thank you and thanks to all the speakers that joined us from online and for keeping to time as well. We were a bit concerned about that, but I'm happy to welcome for the path. So hopefully you'll have picked up from the presentations that were made by the previous speakers that there's a bit of a thread running through the way those stakeholders will consume services. So in Lot 2, as we described before, we've got a devsecops approach to the delivery of build services and when we talk Dave.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2155,7 +2155,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>['Learning', 'Development', 'Organization', 'Skills', 'Ideas']</t>
+          <t>['devsecops', 'build services', 'stakeholders']</t>
         </is>
       </c>
       <c r="E54" t="n">
@@ -2165,10 +2165,10 @@
         <v>0.5</v>
       </c>
       <c r="G54" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="H54" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="55">
@@ -2177,7 +2177,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>SEC UPS what we mean is that the same teams that will build the services will ultimately run the services so that then means that there's got to be a clear delineation with those services that already exist in lot 3 and the running of those services so different modes of operation so there will be different types of contracts that drop into those lots you'll have also seen from David Cooper's part of the presentation a lot for is focused on those configurable platforms and products and whilst David specifically mentioned those that are appropriate to case management delivery Group which are things like pegger and documentum and the Microsoft Office 365 platforms the eagle-eyed amongst you will have seen at least nine technologies that were mentioned during the course of the presentation they represent the technologies that we have today it's not an exhaustive list we may adopt new technologies tomorrow but when it comes to thinking about bidding for lot 4. that break between lot 4A and 4B there's</t>
+          <t>SEC UPS what we mean is that the same teams that will build the services will ultimately run the services, so that then means that there's got to be a clear delineation with those services that already exist in lot 3 and the running of those services. So different modes of operation, so there will be different types of contracts that drop into those lots. You'll have also seen from David Cooper's part of the presentation, a lot for is focused on those configurable platforms and products, and whilst David specifically mentioned those that are appropriate to case management delivery Group, which are things like pegger and documentum and the Microsoft Office 365 platforms, the eagle-eyed amongst you will have seen at least nine technologies that were mentioned during the course of the presentation. They represent the technologies that we have today, it's not an exhaustive list, we may adopt new technologies tomorrow, but when it comes to thinking about bidding for lot 4, that break between lot 4A and 4B there's got to be a clear delineation between those two lots.</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2187,17 +2187,17 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>['SEC', 'UPS', 'teams', 'services', 'contracts', 'configurable', 'platforms', 'products', 'case management', 'documentum', 'Microsoft Office 365', 'technologies']</t>
+          <t>['SEC', 'UPS', 'case management', 'Microsoft Office 365', 'lot 4']</t>
         </is>
       </c>
       <c r="E55" t="n">
         <v>0.5</v>
       </c>
       <c r="F55" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G55" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H55" t="n">
         <v>0.2</v>
@@ -2209,7 +2209,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>going to be something really interesting that comes out in the invitation to Tender stage of this in order to get on lot 4A you would have to have capability in at least six of those nine name Technologies and for lot 4B in two of those nine name Technologies so again Lower barrier for entry to smes in that part of the last one and Sarah talked well about the the need for us to continue to grow our own capability and to use those academies focused on the Technologies to build that skill and capability what we haven't talked about in an awful lot of depth so far is the content of lot one and that's deliberately we've left it until this point because lot one is actually focused to a great extent on helping to build that intelligent client capability that you've heard referred to repeatedly throughout the course of the presentations today it's something that we genuinely want to build within the organization because we're moving from a situation in which essentially</t>
+          <t>Going to be something really interesting that comes out in the invitation to Tender stage of this. In order to get on Lot 4A, you would have to have capability in at least six of those nine named Technologies, and for Lot 4B in two of those nine named Technologies. So again, lower barrier for entry to SMEs in that part of the last one. Sarah talked well about the need for us to continue to grow our own capability and to use those academies focused on the Technologies to build that skill and capability. What we haven't talked about in an awful lot of depth so far is the content of Lot One, and that's deliberately. We've left it until this point because Lot One is actually focused to a great extent on helping to build that intelligent client capability that you've heard referred to repeatedly throughout the course of the presentations today. It's something that we genuinely want to build within the organization because we're moving from a situation in which essentially...</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2219,7 +2219,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>['Tender', 'Lot 4A', 'Lot 4B', 'SMEs', 'Academies', 'Technologies', 'Content', 'Organization']</t>
+          <t>['Tender', 'Lot 4A', 'Lot 4B', 'SMES', 'Academies', 'Technologies', 'Lot One']</t>
         </is>
       </c>
       <c r="E56" t="n">
@@ -2241,17 +2241,17 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>everything has been done for a long period of time by a group of outsourced suppliers and whilst we do have significant capability in the organization we do need to build that further so that we can validate and test the things that were being told by suppliers on an ongoing basis so part of the approach to building that intelligent client capability is to have a group of suppliers who can act as a council which will provide advice to Tom skellage as the C team do lead and also take on specific tasks and challenges in terms of trying to accelerate our transformation because what we want to do over the course of the next three to eight years really is to move towards an estate where predominantly it is configurable platforms and products so the quicker we can accelerate that the quicker we can get things into the cloud with those configurable platforms the quicker our overheads reduce and we have a better cost proposition overall</t>
+          <t>Everything has been done for a long period of time by a group of outsourced suppliers, and whilst we do have significant capability in the organization, we do need to build that further so that we can validate and test the things that were being told by suppliers on an ongoing basis. So, part of the approach to building that intelligent client capability is to have a group of suppliers who can act as a council which will provide advice to Tom Skellage as the C team do lead, and also take on specific tasks and challenges in terms of trying to accelerate our transformation. Because what we want to do over the course of the next three to eight years really is to move towards an estate where predominantly it is configurable platforms and products. So, the quicker we can accelerate that, the quicker we can get things into the cloud with those configurable platforms, the quicker our overheads reduce and we have a better cost proposition overall.</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Intelligent Client</t>
+          <t>Accelerating Transformation</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>['outsourced suppliers', 'validate', 'test', 'council', 'Tom skellage', 'configurable platforms']</t>
+          <t>['outsourced suppliers', 'intelligent client', 'configurable platforms', 'cloud', 'overheads']</t>
         </is>
       </c>
       <c r="E57" t="n">
@@ -2261,7 +2261,7 @@
         <v>0.8</v>
       </c>
       <c r="G57" t="n">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="H57" t="n">
         <v>0.2</v>
@@ -2273,17 +2273,17 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>so we need the support of the market certainly in the short term to be able to do that as we're building that capability but also within that you'll start to see some interesting and Innovative things that we're looking to propose so for example the suppliers within that lot may be involved in strategy and architecture design validation and what have you and by the way a copy of these slides will be made available for you to get all of the details of the content of the lot but there'll be things that you won't have seen hmrc or much of UK government do before that we're looking to propose for example facilitated settlers and coder sessions now some of you will be aware of what that is you'll have probably been involved in them but the process here is that a supplier set up a platform takes a problem a business problem with one of our services or Digital Services or systems that are presented by our architecture team and crowdsources an answer so put it out to coders developers configurers around the world to provide</t>
+          <t>So, we need the support of the market certainly in the short term to be able to do that as we're building that capability, but also within that you'll start to see some interesting and innovative things that we're looking to propose. For example, the suppliers within that lot may be involved in strategy and architecture design validation and what have you. By the way, a copy of these slides will be made available for you to get all of the details of the content of the lot, but there'll be things that you won't have seen HMRC or much of UK government do before that we're looking to propose. For example, facilitated settlers and coder sessions. Now, some of you will be aware of what that is, you'll have probably been involved in them, but the process here is that a supplier set up a platform, takes a problem, a business problem with one of our services or digital services or systems that are presented by our architecture team, and crowdsources an answer, so put it out to coders, developers, configurers around the world to provide.</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Innovative Solutions</t>
+          <t>Innovation Proposal</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>['suppliers', 'strategy', 'architecture', 'validation', 'facilitated', 'settlers', 'coder', 'sessions', 'crowdsources']</t>
+          <t>['market', 'suppliers', 'slides', 'HMRC', 'facilitated settlers', 'coder sessions', 'platform']</t>
         </is>
       </c>
       <c r="E58" t="n">
@@ -2293,10 +2293,10 @@
         <v>0.7</v>
       </c>
       <c r="G58" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="H58" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="59">
@@ -2305,27 +2305,27 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>answers to those things and a securitized sanitized with the suppliers taking responsibility for securitizing and sanitizing those answers to come back into hmrc to apply to us in the in our Real World Systems so there's no hmrc data exposure but there will be solutions that can come back and help us to accelerate those types of transformation that could be supported by payments that hmrc could make via the supplier to individual coders Who present solutions that solve problems which again is an interesting thing that's hmrc and much of government hasn't done before I think only gchq has done that so far in the UK but it's becoming bigger in the Dutch government so I would expect it to expand as as time goes on and as we start moving through the slides we start to look at some of the additional features that we'll see and just to carry up before we move into this because this is a cross-government framework and will be accessible by any government Department as well as wider public sector whilst hmrc May well be adopting some of</t>
+          <t>Answers to those things and a securitized, sanitized with the suppliers taking responsibility for securitizing and sanitizing those answers to come back into HMRC to apply to us in our Real World Systems. So, there's no HMRC data exposure, but there will be solutions that can come back and help us to accelerate those types of transformation that could be supported by payments that HMRC could make via the supplier to individual coders who present solutions that solve problems. Which again is an interesting thing that HMRC and much of government hasn't done before. I think only GCHQ has done that so far in the UK, but it's becoming bigger in the Dutch government, so I would expect it to expand as time goes on. And as we start moving through the slides, we start to look at some of the additional features that we'll see. Just to carry up before we move into this, because this is a cross-government framework and will be accessible by any government department as well as wider public sector, whilst HMRC may well be adopting some of it.</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Data Exposure</t>
+          <t>HMRC Solutions</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>['securitizing', 'sanitizing', 'solutions', 'coders', 'gchq', 'Dutch', 'government']</t>
+          <t>['securitizing', 'sanitizing', 'Real World Systems', 'GCHQ', 'cross-government']</t>
         </is>
       </c>
       <c r="E59" t="n">
         <v>0.5</v>
       </c>
       <c r="F59" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G59" t="n">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="H59" t="n">
         <v>0.2</v>
@@ -2337,17 +2337,17 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>these things it's not going to be a requirement for the other government departments who are involved to adopt them they'll have to make their own choices as to whether or not they do but some of those things will involve competition being a default for any non-commodetized service tailored governance being in place that can help us to really rapidly get to Market wherever possible tailored calloff contract models again depending on the size of the requirements and the the length of the engagement we can create tailored contract models for that standardized and complementary kpi models we actually have a work stream going on right now in which we're starting to create a standardized view of what it means to be a supplier to hmrc in the Dallas environment in the future so you can expect that to be part of the things you will see if you're appointed to the framework and of course the core social value needs that need to be aligned to for any requirements over 10 million pounds now there needs to be that social value impact that's included and one of the</t>
+          <t>These things, it's not going to be a requirement for the other government departments who are involved to adopt them. They'll have to make their own choices as to whether or not they do, but some of those things will involve competition being a default for any non-commodetized service, tailored governance being in place that can help us to really rapidly get to Market wherever possible, tailored calloff contract models (again depending on the size of the requirements and the length of the engagement) we can create tailored contract models for that, standardized and complementary KPI models. We actually have a work stream going on right now in which we're starting to create a standardized view of what it means to be a supplier to HMRC in the Dallas environment in the future, so you can expect that to be part of the things you will see if you're appointed to the framework. And of course, the core social value needs that need to be aligned to for any requirements over 10 million pounds - now there needs to be that social value impact that's included.</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>HMRC Suppliers</t>
+          <t>Government contracts</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>['competition', 'governance', 'contracts', 'KPIs', 'social value']</t>
+          <t>['competition', 'governance', 'KPI', 'social value', 'HMRC']</t>
         </is>
       </c>
       <c r="E60" t="n">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>things we've been really happy to see is the response to this during the tech sourcing program competitions that we put out and it's it's abundantly obvious those organizations who view social value as being for life and not just for Christmas because when we see things like ecosystems being set up and Lead organizations working in a complementary way with those ecosystem Partners to create opportunities in local communities working with those ecosystem Partners to help us to understand how they will impact design Define and deliver right throughout the life cycle of a particular statement of work we can start to see those organizations that really want to have that affect that social impact the trickle-down of the economics both to the SME organizations but also into those local communities where there can be real impact as a result of the things that we do together Us in government and the suppliers cut out the next slide</t>
+          <t>Things we've been really happy to see is the response to this during the tech sourcing program competitions that we put out. It's abundantly obvious those organizations who view social value as being for life and not just for Christmas, because when we see things like ecosystems being set up and Lead organizations working in a complementary way with those ecosystem Partners to create opportunities in local communities, working with those ecosystem Partners to help us to understand how they will impact, design, define and deliver right throughout the life cycle of a particular statement of work, we can start to see those organizations that really want to have that affect that social impact, the trickle-down of the economics both to the SME organizations but also into those local communities where there can be real impact as a result of the things that we do together, us in government and the suppliers. Cut out the next slide.</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2386,10 +2386,10 @@
         <v>0.7</v>
       </c>
       <c r="F61" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="G61" t="n">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="H61" t="n">
         <v>0.2</v>
@@ -2401,7 +2401,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>so in terms of the the fund allocation Lee mentioned at the outset that there's a real opportunity here for us to for suppliers to have a fairly sizable slice of the pie that's available now two billion pounds is an overall forecast is is a big number to start us off with but U.S suppliers are only likely to be interested in investing to the extent that we would want you to invest if you know you are guaranteed to make some money from this so one of the options hmrc plans to include in Lots two and four is the option to direct award on what we're calling a tiered taxi rank basis so what we'll do is create three value levels and in those value levels the suppliers are pointed to that framework a lot will literally take turns of getting work packages allocated to them up to a certain value level we're anticipating at the moment that that figure may be around 40 of the forecast value of the lot but that's not fixed yet but what that means is that there's a</t>
+          <t>So, in terms of the fund allocation, Lee mentioned at the outset that there's a real opportunity here for us to, for suppliers to have a fairly sizable slice of the pie that's available now. Two billion pounds is an overall forecast, is a big number to start us off with, but U.S. suppliers are only likely to be interested in investing to the extent that they are guaranteed to make some money from this. So, one of the options HMRC plans to include in Lots two and four is the option to direct award on what we're calling a tiered taxi rank basis. So, what we'll do is create three value levels and in those value levels the suppliers are pointed to that framework. A lot will literally take turns of getting work packages allocated to them up to a certain value level. We're anticipating at the moment that that figure may be around 40% of the forecast value of the lot, but that's not fixed yet. But what that means is that there's a lot of potential for suppliers to get involved.</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2411,7 +2411,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>['Lee', 'HMRC', 'Taxi Rank', 'Value Levels']</t>
+          <t>['HMRC', 'U.S. suppliers', 'Taxi Rank', 'Two Billion Pounds']</t>
         </is>
       </c>
       <c r="E62" t="n">
@@ -2433,27 +2433,27 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>guaranteed minimum level of Revenue that A supplier should be able to realize from being a lot to and four just by virtue of being there naturally there will also be competition that will make up at least 60 of the activity that exists in those lots too but by us putting skin in the game the idea is that that gets reciprocated by the market you put skin in the game too you bring your 80 and you keep your a team with us and whilst this is clearly a wider government framework one of the things we'll ask suppliers to Warrant as a means of qualifying to be present on the framework is that they can guarantee the capacity and capability to hmrc and that it won't be diluted by engagements elsewhere with the other government departments so I guess there's a big forecasting job to be done for what those sorts of levels might be as other government departments start to adopt the Dallas model as part of their future plans and obviously the mechanism for a continued competition throughout the life of the framework</t>
+          <t>Guaranteed minimum level of Revenue that A supplier should be able to realize from being a lot to and four just by virtue of being there naturally there will also be competition that will make up at least 60% of the activity that exists in those lots too but by us putting skin in the game the idea is that that gets reciprocated by the market. You put skin in the game too, you bring your 80% and you keep your A team with us. Whilst this is clearly a wider government framework, one of the things we'll ask suppliers to Warrant as a means of qualifying to be present on the framework is that they can guarantee the capacity and capability to HMRC and that it won't be diluted by engagements elsewhere with the other government departments. So I guess there's a big forecasting job to be done for what those sorts of levels might be as other government departments start to adopt the Dallas model as part of their future plans and obviously the mechanism for a continued competition throughout the life of the framework.</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Government Framework</t>
+          <t>Government framework</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>['Revenue', 'Competition', 'Capacity', 'Forecasting', 'Engagements']</t>
+          <t>['Revenue', 'Competition', 'HMRC', 'Dallas model']</t>
         </is>
       </c>
       <c r="E63" t="n">
         <v>0.5</v>
       </c>
       <c r="F63" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G63" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H63" t="n">
         <v>0.2</v>
@@ -2465,27 +2465,27 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>we discussed before about the fact that if we're so open in providing information with our pipelines our architectural designs what work packages are going to be coming out three months down the line it should enable a very very rapid turnaround so rather than a big commercial Contracting process essentially we've just put out a statement of requirements you come back to us with your proposal within four weeks and we'll have boots on the ground very quickly afterwards that's that's the intent and the more that we can do that the more we'll be able to respond in an agile way to the emerging situations that develop Jillian referred before to how the covert schemes really created a challenge for hmrc and it's quite heartening to note that when you consider the fact that when the chancellor at the time Rishi sunak stood up and announced that there would be schemes introduced for Coronavirus job retention self in self-employment Income Support schemes the first one of those coronavirus job retention was literally from the ground</t>
+          <t>We discussed before about the fact that if we're so open in providing information with our pipelines, our architectural designs, what work packages are going to be coming out three months down the line, it should enable a very, very rapid turnaround. So, rather than a big commercial Contracting process, essentially we've just put out a statement of requirements; you come back to us with your proposal within four weeks and we'll have boots on the ground very quickly afterwards. That's that's the intent, and the more that we can do that, the more we'll be able to respond in an agile way to the emerging situations that develop. Jillian referred before to how the covert schemes really created a challenge for HMRC, and it's quite heartening to note that when you consider the fact that when the chancellor at the time, Rishi Sunak, stood up and announced that there would be schemes introduced for Coronavirus Job Retention, Self-Employment Income Support schemes, the first one of those coronavirus job retention was literally from the ground up.</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Rapid Turnaround</t>
+          <t>Covid Response</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>['Contracting', 'Statement of Requirements', 'Agile', 'Covert Schemes', 'HMRC']</t>
+          <t>['HMRC', 'Rishi Sunak', 'Coronavirus Job Retention', 'Self-Employment Income Support', 'Agile Response']</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F64" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="G64" t="n">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="H64" t="n">
         <v>0.2</v>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>to delivery four weeks so if we can industrialize that kind of model we can respond to many of the things that are likely to happen over the course of the next months and years particularly as we start to see the focuses shift with a new prime minister and there's certainly going to be a general election before the end of 2024 who knows it may even be sooner and again we could see Focus shifts again so we need to be in a position to respond in an agile way to those to those to those things so in terms of direct Awards we've already mentioned the tiered taxi Rank and it's tiered for a reason now if we have three value tiers it essentially means that no one supplier gets all the big chunky work one and other suppliers get all the the crumbs that get wiped off the table everyone gets a chance to rotate through those through those lists and when we make the awards the way we plan to structure these is that for the highest value taxi rank the supplier</t>
+          <t>To delivery four weeks, so if we can industrialize that kind of model, we can respond to many of the things that are likely to happen over the course of the next months and years, particularly as we start to see the focuses shift with a new prime minister and there's certainly going to be a general election before the end of 2024 - who knows, it may even be sooner - and again we could see focus shifts again. So, we need to be in a position to respond in an agile way to those to those to those things. So, in terms of direct awards, we've already mentioned the tiered taxi rank and it's tiered for a reason. Now, if we have three value tiers, it essentially means that no one supplier gets all the big chunky work, and other suppliers get all the crumbs that get wiped off the table. Everyone gets a chance to rotate through those through those lists and when we make the awards, the way we plan to structure these is that for the highest value taxi rank, the supplier.</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2507,7 +2507,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>['direct awards', 'tiered taxi rank', 'value tiers', 'suppliers', 'awards']</t>
+          <t>['Industrialize', 'Focus Shifts', 'Direct Awards', 'Taxi Rank', 'Rotate']</t>
         </is>
       </c>
       <c r="E65" t="n">
@@ -2529,17 +2529,17 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>placed first in the list will become supplier one in the highest value suppliers Place second will be in first in the medium value and the supplier Place third will be first in the low value and then the rotation will happen on that order so the information's on the slide they're about direct Awards again we'll be circulating these so I don't plan to read them in more detail one thing that's important to point out though is that within procurement legislation there is a a bias a Prejudice shall we say towards competition so where something would normally be within one of the taxi ranks or purchasable through a service catalog hmrc would retain the rate and the option to compete that but the opposite isn't true if something would normally be within the competition sphere we can't turn it into a direct award opportunity so just to make that clear and we've got our next slide</t>
+          <t>Placed first in the list will become supplier one in the highest value suppliers. Place second will be in first in the medium value and the supplier. Place third will be first in the low value and then the rotation will happen on that order. So, the information's on the slide, they're about direct Awards again we'll be circulating these so I don't plan to read them in more detail. One thing that's important to point out though is that within procurement legislation there is a a bias, a Prejudice shall we say, towards competition. So, where something would normally be within one of the taxi ranks or purchasable through a service catalog, HMRC would retain the rate and the option to compete that. But the opposite isn't true, if something would normally be within the competition sphere, we can't turn it into a direct award opportunity. So, just to make that clear and we've got our next slide.</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Direct Awards</t>
+          <t>Procurement Legislation</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>['procurement', 'legislation', 'competition', 'taxi ranks', 'service catalog']</t>
+          <t>['direct awards', 'taxi ranks', 'service catalog', 'competition', 'HMRC']</t>
         </is>
       </c>
       <c r="E66" t="n">
@@ -2561,24 +2561,24 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>many competitions we've already mentioned the extra detail here is that the due diligence that we'll be running to a point suppliers in the first place is going to be critical to us doing that fast turnaround and the mechanisms actually going to going to enable our customer groups and platform teams to deploy those rapid sourcing models and using a lighter touch commercial vehicle so rather than the big 800 page contracts that some of you have seen from us in the past wherever possible we'll be looking to deliver those in six to eight pages of information which just reference either a framework document or a an enduring call off that the suppliers would have as a by virtue of that being appointed to the framework next slide please and those Innovation approaches we talked about rainbow teams you've had mentioned a number of times today and I trailed before the fact that we've had awful trouble working out exactly how we can create a situation in which we can transfer risk while still having suppliers work together and we went back and forth on this for</t>
+          <t>Many competitions we've already mentioned - the extra detail here is that the due diligence that we'll be running to appoint suppliers in the first place is going to be critical to us doing that fast turnaround. And the mechanisms are actually going to enable our customer groups and platform teams to deploy those rapid sourcing models and using a lighter touch commercial vehicle. So, rather than the big 800 page contracts that some of you have seen from us in the past, wherever possible we'll be looking to deliver those in six to eight pages of information which just reference either a framework document or an enduring call off that the suppliers would have as a by virtue of that being appointed to the framework. Next slide please. And those Innovation approaches we talked about - rainbow teams, you've had mentioned a number of times today - and I trailed before the fact that we've had awful trouble working out exactly how we can create a situation in which we can transfer risk while still having suppliers work together and we went back and forth on this for a while.</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Rapid Sourcing</t>
+          <t>Supplier Management</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>['competitions', 'due diligence', 'customer groups', 'platform teams', 'Innovation', 'rainbow teams', 'risk transfer']</t>
+          <t>['Due Diligence', 'Rapid Sourcing', 'Innovation', 'Rainbow Teams', 'Risk Transfer']</t>
         </is>
       </c>
       <c r="E67" t="n">
         <v>0.5</v>
       </c>
       <c r="F67" t="n">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="G67" t="n">
         <v>0.7</v>
@@ -2593,7 +2593,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>weeks and weeks and weeks thinking how do we force suppliers to do this and then one day the light bulb went on and we thought why why are we thinking about forcing suppliers to do anything rather than incentivizing suppliers to do something so what we're planning to develop as part of this process is a contract management mechanism where there will be kpi measurements based upon collaboration with suppliers within the lots that this applies to so predominantly we would look at this being watch two and four but if you imagine a world in which you're assigned to deliver a work package and you have kpis linked to that work package and you can deliver that entirely with yourself or your own supplier team or with your ecosystem and you can get a tick in the Box you can get paid your Milestone payments for all of the things that you've delivered and all of that's fine because it works for hmrc but against those kpis you would never</t>
+          <t>Weeks and weeks and weeks thinking, 'How do we force suppliers to do this?' And then one day, the light bulb went on and we thought, 'Why are we thinking about forcing suppliers to do anything, rather than incentivizing suppliers to do something?' So, what we're planning to develop as part of this process is a contract management mechanism, where there will be KPI measurements based upon collaboration with suppliers within the lots that this applies to. So, predominantly, we would look at this being watch two and four. But if you imagine a world in which you're assigned to deliver a work package and you have KPIs linked to that work package, and you can deliver that entirely with yourself or your own supplier team or with your ecosystem, and you can get a tick in the box, you can get paid your milestone payments for all of the things that you've delivered, and all of that's fine because it works for HMRC, but against those KPIs you would never.</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2603,20 +2603,20 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>['Suppliers', 'KPIs', 'Work Package', 'Ecosystem', 'HMRC']</t>
+          <t>['KPIs', 'Suppliers', 'Incentivizing', 'Work Package', 'Ecosystem']</t>
         </is>
       </c>
       <c r="E68" t="n">
         <v>0.5</v>
       </c>
       <c r="F68" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G68" t="n">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="H68" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="69">
@@ -2625,17 +2625,17 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>score more than 60 percent out of 100 percent if you then brought in individuals from other supplier teams you can start to score 70 or 80 or 90 the extent to which you support other suppliers and their deliveries could take you up to 100 potentially and unlocking those stage points has the potential then to unlock not just the performance incentives of being placed really high in a league table that we will keep which you can then report on to other government departments when you're going through your bidding processes but potentially also unlock Financial incentives too that would make it worth the while of suppliers to involve individuals from other organizations why would we want to do that well part of it is about transferring risk but part of it is about giving us the opportunity to say okay you've taken that risk you've taken the extra King Shilling so to speak so any issues that exists between yourselves and other suppliers within that group are your issues rather than</t>
+          <t>Score more than 60 percent out of 100 percent if you then brought in individuals from other supplier teams you can start to score 70 or 80 or 90. The extent to which you support other suppliers and their deliveries could take you up to 100 potentially, and unlocking those stage points has the potential then to unlock not just the performance incentives of being placed really high in a league table that we will keep, which you can then report on to other government departments when you're going through your bidding processes, but potentially also unlock Financial incentives too that would make it worth the while of suppliers to involve individuals from other organizations. Why would we want to do that? Well, part of it is about transferring risk, but part of it is about giving us the opportunity to say okay, you've taken that risk, you've taken the extra King Shilling so to speak, so any issues that exists between yourselves and other suppliers within that group are your issues rather than ours.</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Supplier Teams</t>
+          <t>Supplier Risk</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>['score', 'supplier', 'deliveries', 'incentives', 'risk']</t>
+          <t>['Suppliers', 'Risk', 'Incentives', 'League Table', 'Government']</t>
         </is>
       </c>
       <c r="E69" t="n">
@@ -2648,7 +2648,7 @@
         <v>0.3</v>
       </c>
       <c r="H69" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="70">
@@ -2657,7 +2657,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>our issues as a consequence of that extra incentivization being part of the agreement but the real benefit for us is the fact that we've come from a world in which we've had a huge amount of dependence on just one or two suppliers we don't ever want to go back there and that's not to say anything about those suppliers who are wonderful suppliers but as an organization it enabled us to fall into bad practice and we want to avoid going back to that bad practice again so by having that bigger group of suppliers who've got that in-depth knowledge of our estate of the services the products the systems it enables us to be able to swap suppliers out more quickly and avoid that dependence that has us locked in for potentially two three four years longer than we could have ever intended to do information sharing we've already talked about so three year plans we'll be providing which are generally going to be linked to the spending review periods that are released by the treasury we'll</t>
+          <t>Our issues are a consequence of that extra incentivization being part of the agreement, but the real benefit for us is the fact that we've come from a world in which we've had a huge amount of dependence on just one or two suppliers. We don't ever want to go back there, and that's not to say anything about those suppliers, who are wonderful suppliers, but as an organization it enabled us to fall into bad practice and we want to avoid going back to that bad practice again. By having that bigger group of suppliers who've got that in-depth knowledge of our estate of the services, the products, the systems, it enables us to be able to swap suppliers out more quickly and avoid that dependence that has us locked in for potentially two, three, four years longer than we could have ever intended to do. Information sharing, we've already talked about. So, three year plans we'll be providing, which are generally going to be linked to the spending review periods that are released by the treasury.</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2689,27 +2689,27 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>be able to provide one-year project plans and wherever possible three-month plans identifying which work packages are going to be released that's predominantly for Lots two and four in lot 3 you will generally because these are Legacy services that are based on run and sometimes modernization they're likely to be longer contracts from the outset until those con those Services would be slated for decommissioning and because of the fact that generally speaking all of the intellectual property is produced for hmrc it becomes hmrc's intellectual property and therefore we would exercise the option to share that intellectual property with all of the suppliers on the framework to enable them to then pick up work that may have been started by another supplier so again that openness of the information sharing will help to underpin what we plan to take forward I mean obviously as suppliers it's entirely on your own heads if you choose to share your own intellectual property but we'll happily share ours with those who are appointed to the framework next slide please</t>
+          <t>Be able to provide one-year project plans and, wherever possible, three-month plans identifying which work packages are going to be released. That's predominantly for Lots two and four in Lot 3. You will generally, because these are Legacy services that are based on run and sometimes modernization, they're likely to be longer contracts from the outset until those services would be slated for decommissioning. And because of the fact that generally speaking all of the intellectual property is produced for HMRC, it becomes HMRC's intellectual property and therefore we would exercise the option to share that intellectual property with all of the suppliers on the framework to enable them to then pick up work that may have been started by another supplier. So again, that openness of the information sharing will help to underpin what we plan to take forward. I mean, obviously, as suppliers it's entirely on your own heads if you choose to share your own intellectual property, but we'll happily share ours with those who are appointed to the framework. Next slide please!</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Project Plans</t>
+          <t>Information Sharing</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>['one-year', 'three-month', 'Legacy services', 'modernization', 'intellectual property', 'information sharing']</t>
+          <t>['intellectual property', 'Legacy services', 'HMRC', 'framework', 'work packages']</t>
         </is>
       </c>
       <c r="E71" t="n">
         <v>0.5</v>
       </c>
       <c r="F71" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G71" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H71" t="n">
         <v>0.2</v>
@@ -2721,7 +2721,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>and of course the SME ecosystem this is really underpinned by a long-standing Target that government wants to spend one pound in every three with smes and we achieved a really positive step forward in the tsp competitions that we did in the first couple of waves in introducing those ecosystems we're looking to build on that with Dallas but also create more opportunities for smes to contract with us directly whenever possible so those the B parts of the lot 2B 4B we're looking to try to reduce the barriers to entry reduce insurance requirements and what have you so they're more attuned to the needs of the smaller organization that still has sufficient scale and capacity to be able to deliver in conjunction with other suppliers on those lots and in terms of financial incentivization models one of the models that we're looking to try and introduce in certain circumstances would be returned on investment-based models which you probably won't have seen from hmrc before so you'll probably be familiar with the concept of concessions contracts within</t>
+          <t>And of course, the SME ecosystem. This is really underpinned by a long-standing target that government wants to spend one pound in every three with SMEs. We achieved a really positive step forward in the TSP competitions that we did in the first couple of waves in introducing those ecosystems. We're looking to build on that with Dallas, but also create more opportunities for SMEs to contract with us directly whenever possible. So, those B parts of the Lot 2B and 4B, we're looking to try to reduce the barriers to entry, reduce insurance requirements, and what have you, so they're more attuned to the needs of the smaller organization that still has sufficient scale and capacity to be able to deliver in conjunction with other suppliers on those lots. And, in terms of financial incentivization models, one of the models that we're looking to try and introduce in certain circumstances would be return on investment-based models, which you probably won't have seen from HMRC before. So, you'll probably be familiar with the concept of concessions contracts within.</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2731,17 +2731,17 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>['SME', 'Target', 'TSP', 'Dallas', 'Barriers', 'Insurance', 'ROI', 'Concessions']</t>
+          <t>['SMEs', 'TSP', 'Dallas', 'Lot 2B', 'Lot 4B', 'HMRC']</t>
         </is>
       </c>
       <c r="E72" t="n">
         <v>0.5</v>
       </c>
       <c r="F72" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G72" t="n">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="H72" t="n">
         <v>0.2</v>
@@ -2753,17 +2753,17 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>the regulations this just really Builds on that to say that we have a requirement you can tell us that you could deliver the requirement for X amounts of money but that x amount of money could be something paid to you in return for delivering the requirement or alternatively you could be paid a smaller amount of money but potentially get a larger reward based on the percentage of the ROI further down the line so it's an opportunity for suppliers to gain more from a revenue point of view on the basis of being able to deliver the outcome that we're looking for so again hopefully for us that's something that will help us to lock in value and avoid having to rework things as we often do today on a time and materials basis gain share options we're looking to introducing some of the lots of mechanism whereby through open book where suppliers are appointed if their profit margins from the framework exceed 25 percent they'll then be a netting approach where there'll be a rebate paid into an innovation Fund in hmrc which</t>
+          <t>The regulations this just really builds on that to say that we have a requirement. You can tell us that you could deliver the requirement for X amounts of money, but that X amount of money could be something paid to you in return for delivering the requirement, or alternatively you could be paid a smaller amount of money but potentially get a larger reward based on the percentage of the ROI further down the line. So it's an opportunity for suppliers to gain more from a revenue point of view on the basis of being able to deliver the outcome that we're looking for. So again, hopefully for us, that's something that will help us to lock in value and avoid having to rework things as we often do today on a time and materials basis. Gain share options, we're looking to introducing some of the lots of mechanism whereby through open book, where suppliers are appointed, if their profit margins from the framework exceed 25 percent, they'll then be a netting approach where there'll be a rebate paid into an innovation fund in HMRC.</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Gain Share Options</t>
+          <t>Gain Sharing</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>['regulations', 'requirement', 'ROI', 'reward', 'value', 'time and materials']</t>
+          <t>['Regulations', 'Requirements', 'ROI', 'Time and Materials', 'Gain Sharing', 'Open Book']</t>
         </is>
       </c>
       <c r="E73" t="n">
@@ -2773,7 +2773,7 @@
         <v>0.7</v>
       </c>
       <c r="G73" t="n">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="H73" t="n">
         <v>0.2</v>
@@ -2785,27 +2785,27 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>will actually fund some of the activities that take place in lot one such as those facilitated citizen coder sessions that I talked about before so again there's an opportunity not just to have that remittance but to earn some of it back potentially too and the minimum workshare commitment we've already mentioned and more detail of that will be released when we issue the invitation to Tender and I'm sure the the team who are going to take us through next step Shannon and Miriam we'll talk in detail about what dates are the key dates to look out for when it comes to the release of those materials I think that may be my final slide so I'm going to hand over to Mike note to take us through the next part of the session ably assisted by Shannon and Miriam but you can introduce yourselves hello I'm Shannon wood and I'm a Dallas we're extreme lead so we've been with the project since initiation around April</t>
+          <t>Will actually fund some of the activities that take place in Lot One, such as those facilitated Citizen Coder sessions that I talked about before. So, again, there's an opportunity not just to have that remittance, but to earn some of it back potentially too. The minimum workshare commitment we've already mentioned, and more detail of that will be released when we issue the invitation to Tender. I'm sure the team who are going to take us through the next step, Shannon and Miriam, will talk in detail about what dates are the key dates to look out for when it comes to the release of those materials. I think that may be my final slide, so I'm going to hand over to Mike to take us through the next part of the session, ably assisted by Shannon and Miriam, but you can introduce yourselves. Hello, I'm Shannon Wood and I'm a Dallas. We're Extreme Lead, so we've been with the project since initiation around April.</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Citizen Coder</t>
+          <t>Project Initiation</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>['remittance', 'workshare', 'invitation', 'Tender', 'dates']</t>
+          <t>['remittance', 'workshare', 'invitation to tender', 'Shannon Wood', 'Miriam', 'Mike']</t>
         </is>
       </c>
       <c r="E74" t="n">
         <v>0.5</v>
       </c>
       <c r="F74" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G74" t="n">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="H74" t="n">
         <v>0.2</v>
@@ -2817,27 +2817,27 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>I'm Miriam lorok same role as Shannon also working on the Dallas team with hmrc thank you Mr Happy I'll try and Shout out loud hopefully you can hear me so ccs are leading this this framework but we are heavily supported by hmrc and hmrc teams here which is why we're trying to show it as a joint incentive here and a joint program going forward we we are dependent on the help and support we are running at PACE it is a large program and there is a lot of work to do so we're trying to push through and working today together collaboratively to get there you know we just move on to the next slide if that's okay so as I said we're ccsr are running the framework it will follow the normal process find a tender service will be put out there and we'll be seeking from multiple suppliers for each lot as you see here in this room and online there are a lot of people interested in this framework so yeah I think it is is key and I'll</t>
+          <t>I'm Miriam lorok, same role as Shannon, also working on the Dallas team with hmrc. Thank you Mr. Happy, I'll try and shout out loud, hopefully you can hear me. So, ccs are leading this this framework, but we are heavily supported by hmrc and hmrc teams here, which is why we're trying to show it as a joint incentive here and a joint program going forward. We we are dependent on the help and support. We are running at PACE, it is a large program and there is a lot of work to do, so we're trying to push through and working today together collaboratively to get there. You know we just move on to the next slide if that's okay. So, as I said, we're ccsr are running the framework, it will follow the normal process, find a tender service will be put out there and we'll be seeking from multiple suppliers for each lot. As you see here in this room and online, there are a lot of people interested in this framework, so yeah I think it is is key and I'll.</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>CCS Framework</t>
+          <t>Framework Development</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>['Miriam', 'Shannon', 'Dallas', 'HMRC', 'PACE', 'Tender', 'Suppliers']</t>
+          <t>['hmrc', 'ccs', 'tender', 'PACE', 'Dallas']</t>
         </is>
       </c>
       <c r="E75" t="n">
         <v>0.5</v>
       </c>
       <c r="F75" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="G75" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="H75" t="n">
         <v>0.2</v>
@@ -2849,17 +2849,17 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>go through a procurement do's and don'ts later but you know it is going to be very very important to get and answer the questions that are put out there when when the tender set out the framework is for four years and we're putting a value of about four and a half billion as our anticipated value at this point in time you know and to what we know that hmrc are going to be delivering and what we're talking to other customers around and other customers being on this call as well we know they're they're here they're really interested and really want to work with us to to help and get use of this we know people have got similar problems that hmrc have across central government this is a potential solution for them to deliver against those problems as Phil has said lots to B and 4B are structured to be attractive more attractive to smes CCS driver reporter will be used to deliver this tender and please from my sourcing teams and policy</t>
+          <t>Go through a procurement do's and don'ts later, but you know it is going to be very, very important to get and answer the questions that are put out there when the tender set out the framework is for four years and we're putting a value of about four and a half billion as our anticipated value at this point in time. You know and to what we know that HMRC are going to be delivering and what we're talking to other customers around and other customers being on this call as well, we know they're they're here they're really interested and really want to work with us to to help and get use of this. We know people have got similar problems that HMRC have across central government, this is a potential solution for them to deliver against those problems. As Phil has said, lots to B and 4B are structured to be attractive, more attractive to SMEs. CCS driver reporter will be used to deliver this tender and please from my sourcing teams and policy.</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Procurement Process</t>
+          <t>Procurement process</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>['procurement', 'tender', 'framework', 'value', 'hmrc', 'customers', 'solution', 'smes', 'CCS']</t>
+          <t>['procurement', 'tender', 'HMRC', 'SMES', 'CCS']</t>
         </is>
       </c>
       <c r="E76" t="n">
@@ -2869,7 +2869,7 @@
         <v>0.8</v>
       </c>
       <c r="G76" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="H76" t="n">
         <v>0.2</v>
@@ -2881,17 +2881,17 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>teams Karma reduction plans will be a key element of this to to be to be put onto the either through the at SQ stage so please start pushing those getting those ready ready to be presented back and if you need to know any more detail about that please go to the CCS website to to look at that and as Phil said this presentation will be put onto the CCS website on the Dallas Page so please look at look at that as well as Mike said but this is a fine attender service we're using flight attend the service and it'll be a restricted procedure so first we'll have the SQ that will come out with this is due to come out on the 6th of October and you'll have about 30 days to respond it'll be a combination of pass fail and quality questions that are backwards looking looking at your past experiences you're gonna get our steps in stepping up and down on this and so as you can see the invitation to Tender will be released following that we're looking at</t>
+          <t>Teams' Karma reduction plans will be a key element of this. To be put onto the SQ stage, so please start pushing those, getting those ready to be presented back. If you need to know any more detail about that, please go to the CCS website to look at that. As Phil said, this presentation will be put onto the CCS website on the Dallas Page, so please look at that as well. As Mike said, this is a fine attendee service we're using. Flight attendee service and it'll be a restricted procedure. So first, we'll have the SQ that will come out with this. It is due to come out on the 6th of October and you'll have about 30 days to respond. It'll be a combination of pass/fail and quality questions that are backwards looking, looking at your past experiences. You're gonna get our steps in stepping up and down on this. So, as you can see, the invitation to Tender will be released following that. We're looking at it.</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Karma reduction</t>
+          <t>Karma Reduction</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>['teams', 'SQ', 'CCS', 'Dallas', 'flight attend', 'Tender']</t>
+          <t>['Karma', 'SQ', 'CCS', 'Dallas', 'Flight Attendee', 'Pass/Fail', 'Quality Questions']</t>
         </is>
       </c>
       <c r="E77" t="n">
@@ -2901,7 +2901,7 @@
         <v>0.8</v>
       </c>
       <c r="G77" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="H77" t="n">
         <v>0.2</v>
@@ -2913,7 +2913,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>release in approximately February 2023 and so whereas as Miriam said the SQ will be backwards looking questions based on your experience the ITT will provide forward-looking questions so that could include case studies scenarios and face-to-face presentations and so you'll have approximately six weeks to respond to the tender and we expect our internal governance to be completed around September 2023 following that outcome letters will be issued and suppliers will be awarded to the framework shortly afterwards okay so the do's and don'ts of procurement housekeeping look I I don't really want to say choose to suck eggs but we do see time and time again suppliers not completing the documentation correctly and then complaining that they don't get onto the Frameworks you know this is going to be competitive there is going to be only a few places available on each of the Lots so please read all the guidance to the tender all the documentation perhaps any public</t>
+          <t>Release in approximately February 2023 and so, whereas, as Miriam said, the SQ will be backwards looking questions based on your experience, the ITT will provide forward-looking questions, so that could include case studies, scenarios, and face-to-face presentations. And so, you'll have approximately six weeks to respond to the tender and we expect our internal governance to be completed around September 2023. Following that outcome, letters will be issued and suppliers will be awarded to the framework shortly afterwards. Okay, so the do's and don'ts of procurement housekeeping. Look, I don't really want to say 'choose to suck eggs', but we do see time and time again suppliers not completing the documentation correctly and then complaining that they don't get onto the Frameworks. You know, this is going to be competitive, there is going to be only a few places available on each of the Lots, so please read all the guidance to the tender, all the documentation, perhaps any public.</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2923,7 +2923,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>['tender', 'framework', 'documentation', 'guidance', 'competitive']</t>
+          <t>['tender', 'framework', 'governance', 'documentation', 'suppliers']</t>
         </is>
       </c>
       <c r="E78" t="n">
@@ -2945,17 +2945,17 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>published clarification questions will be putting those through the relevant rival system send all related contracts via the messaging function on on Bravo so we can keep a track and keep managing that clarification questions we'll go through at the end of where we're going to put those questions between now and when release but but please put those clarification questions in early for it for us and we can give you that information and keep up to date with the published clarification questions and responses going through okay please don't do anything the last minute allow plenty of time to get yourself ready prepared and supported for for your response cross reference without the responses across your tender what we see so often is misalignment of the information yeah please do a final QA check it helps us better quality responses are easier for us to read include attachments where there have</t>
+          <t>Published clarification questions will be putting those through the relevant rival system. Send all related contracts via the messaging function on Bravo, so we can keep a track and keep managing that clarification questions. We'll go through at the end of where we're going to put those questions between now and when release, but please put those clarification questions in early for us and we can give you that information and keep up to date with the published clarification questions and responses going through. Okay, please don't do anything last minute. Allow plenty of time to get yourself ready, prepared and supported for your response. Cross reference without the responses across your tender. What we see so often is misalignment of the information. Yeah, please do a final QA check. It helps us; better quality responses are easier for us to read. Include attachments where there have.</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Clarification Questions</t>
+          <t>Tender response</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>['published', 'rival', 'Bravo', 'QA', 'attachments']</t>
+          <t>['clarification', 'rival system', 'messaging', 'QA check', 'attachments']</t>
         </is>
       </c>
       <c r="E79" t="n">
@@ -2968,7 +2968,7 @@
         <v>0.7</v>
       </c>
       <c r="H79" t="n">
-        <v>0.9</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="80">
@@ -2977,17 +2977,17 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>been specifically requested sorry don't include attachments where they have been not requested yeah you'll be clear the questions will be clear we'll try and make it clear that you can't add things but please check and check again and state the cubs named customer references details that are confidential we will adhere to those confidentially confidentiality markings on those okay all mandatory questions and questions relevant to your bid need to be answered the questions and within the character limits so please pay attention to that there is a set reason that we put them there for that for those lengths we're looking for the information to be relevant in that area so please make sure you read that area all mandatory fields and tables to be completed you know we're not clear what what we're having there yet but you know if you have any questions when that comes out make sure you respond back to us</t>
+          <t>Been specifically requested - sorry, don't include attachments where they have not been requested. Yeah, you'll be clear - the questions will be clear, we'll try and make it clear that you can't add things, but please check and check again and state the customer references details that are confidential - we will adhere to those confidentially, confidentiality markings on those. Okay, all mandatory questions and questions relevant to your bid need to be answered within the character limits, so please pay attention to that. There is a set reason that we put them there for that for those lengths - we're looking for the information to be relevant in that area, so please make sure you read that area. All mandatory fields and tables to be completed - you know we're not clear what we're having there yet, but you know if you have any questions when that comes out, make sure you respond back to us.</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Bid Requirements</t>
+          <t>Bid requirements</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>['attachments', 'questions', 'mandatory', 'confidentiality', 'character limits']</t>
+          <t>['attachments', 'questions', 'confidentiality', 'character limits', 'mandatory fields']</t>
         </is>
       </c>
       <c r="E80" t="n">
@@ -3009,27 +3009,27 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>we'll make sure they're all relevant for you to put in and we'll give you the details and instructions how to complete those so yes sir please marketing we don't want to hear the marketing responses we want to make sure that there is relevant detail in able to support your responses that's that's clear and concise and then check just a final check your organization details are accurate any T's disease you're uncertain with please ask the questions make sure your legal teams are engaged with those you cannot include any attachments so where we've asked for attachments please include those where you haven't where we haven't please do not but be please check and be clear about that the character character count limits will be imposed so if you run short they won't be used and won't be put in or sorry if you run over those they won't be counted in your overall response we'll cut it off at the limit</t>
+          <t>We'll make sure they're all relevant for you to put in and we'll give you the details and instructions how to complete those. So yes sir, please marketing. We don't want to hear the marketing responses, we want to make sure that there is relevant detail in able to support your responses. That's that's clear and concise. And then check, just a final check, your organization details are accurate. Any T's disease you're uncertain with, please ask the questions. Make sure your legal teams are engaged with those. You cannot include any attachments, so where we've asked for attachments please include those. Where we haven't, please do not, but be please check and be clear about that. The character count limits will be imposed, so if you run short they won't be used and won't be put in or sorry if you run over those they won't be counted in your overall response. We'll cut it off at the limit.</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Marketing Responses</t>
+          <t>Organization Details</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>['marketing', 'detail', 'organization', 'legal', 'attachments', 'character count']</t>
+          <t>['marketing', 'responses', 'details', 'attachments', 'character count']</t>
         </is>
       </c>
       <c r="E81" t="n">
         <v>0.5</v>
       </c>
       <c r="F81" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="G81" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="H81" t="n">
         <v>0.2</v>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>that we've set okay thanks again and so we've included in the Packer provisional timeline so as we've got seven different Lots in the framework we've split it into two different phases so phase one will include Lots 2A 2B 3 and 5. and as I said the SQ will be issued on the 6th of October and we're going to issue with the slide pack afterwards so if you don't get your photo in now you can look at it afterwards and and then we look thing for phase two to be launched next summer yeah and we're going to talk about the market engagement two sessions that we're going to be running as a follow-on to this event and so today is their first Market engagement session we're also looking to do our one-to-one sessions as you can see on the screen they'll be face to face and they'll be allocated on a first Confessor basis please remember that you'll be allocated one slot and there won't be opportunities to change their date or</t>
+          <t>That we've set, okay? Thanks again, and so we've included in the Packer provisional timeline. So, as we've got seven different Lots in the framework, we've split it into two different phases. So, phase one will include Lots 2A, 2B, 3, and 5. And, as I said, the SQ will be issued on the 6th of October, and we're going to issue with the slide pack afterwards. So, if you don't get your photo in now, you can look at it afterwards. And then we look thing for phase two to be launched next summer, yeah? And we're going to talk about the market engagement two sessions that we're going to be running as a follow-on to this event. And so, today is their first Market engagement session. We're also looking to do our one-to-one sessions, as you can see on the screen. They'll be face to face, and they'll be allocated on a first Confessor basis. Please remember that you'll be allocated one slot, and there won't be opportunities to change their date or time.</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3051,17 +3051,17 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>['Packer', 'Lots', 'SQ', 'Market Engagement', 'one-to-one sessions']</t>
+          <t>['Packer', 'Timeline', 'Lots', 'SQ', 'Slide Pack', 'Market Engagement', 'One-to-One Sessions']</t>
         </is>
       </c>
       <c r="E82" t="n">
         <v>0.5</v>
       </c>
       <c r="F82" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="G82" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="H82" t="n">
         <v>0.2</v>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>time if that allocated slot and we're going to collate all the questions and answers and from those sessions and we'll anonymize and publish those following the event the sessions will be held in Birmingham and if you're allocated a slot on a day that's affected by rail strikes then you will have the option to dial in virtually the team from ccs and hmrc will be there in person so you can come in person if you wish to and as you can see there's just a reminder at the bottom the dates for the slots for wave one is the week commenced in the 26th of September so last week in September and that includes Lots 2A 2B 3 and 5. we'll issue more information on the slots for Wave 2 next year foreign 's already hinted at after the SQ has been released or all questions or clarification questions will be directed through the CCS Bravo e portal prior to that we've got at the end of the presentation you'll see a few Dallas email addresses that you can use to</t>
+          <t>Time, if that allocated slot, and we're going to collate all the questions and answers from those sessions and we'll anonymize and publish those following the event. The sessions will be held in Birmingham and if you're allocated a slot on a day that's affected by rail strikes then you will have the option to dial in virtually. The team from CCS and HMRC will be there in person, so you can come in person if you wish to. As you can see, there's just a reminder at the bottom: the dates for the slots for Wave One is the week commencing in the 26th of September (so last week in September) and that includes Lots 2A, 2B, 3 and 5. We'll issue more information on the slots for Wave 2 next year, as Foreign has already hinted at, after the SQ has been released. Or, all questions or clarification questions will be directed through the CCS Bravo e portal. Prior to that, we've got at the end of the presentation a few Dallas email addresses that you can use to contact us.</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3083,7 +3083,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>['time', 'slot', 'questions', 'answers', 'Birmingham', 'rail strikes', 'CCS', 'HMRC', 'person', 'Wave 1', 'Wave 2', 'SQ', 'clarification']</t>
+          <t>['CCS', 'HMRC', 'rail strikes', 'Wave One', 'Wave 2', 'SQ', 'Dallas']</t>
         </is>
       </c>
       <c r="E83" t="n">
@@ -3093,10 +3093,10 @@
         <v>0.7</v>
       </c>
       <c r="G83" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="H83" t="n">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="84">
@@ -3105,7 +3105,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>contact us or we've also got a registration form for the market engagement event where you'll have some space to ask questions and obviously in the sessions as well and as Shannon said they will all be released they'll be collated anonymized and released as part of the as part of the tender process for the public and so lastly if you do want to register for a face-to-face one-to-one session you can use the link on the screen or you can scan the QR code you can also use that form to ask any questions that you may have and we'd welcome some feedback too the QR code will be on at the end of the presentation if you need to take a photo of it then just numbers at Birmingham we're using CCS offices in Birmingham so there will be limited numbers of supplier attendees per supplier three so so just three three supplies for each of the sessions okay</t>
+          <t>Contact us, or we've also got a registration form for the market engagement event where you'll have some space to ask questions, and obviously in the sessions as well. And, as Shannon said, they will all be released; they'll be collated, anonymized, and released as part of the tender process for the public. Lastly, if you do want to register for a face-to-face one-to-one session, you can use the link on the screen or you can scan the QR code. You can also use that form to ask any questions that you may have, and we'd welcome some feedback too. The QR code will be on at the end of the presentation if you need to take a photo of it; then just numbers at Birmingham, we're using CCS offices in Birmingham, so there will be limited numbers of supplier attendees per supplier - three, so just three supplies for each of the sessions, okay?</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3115,17 +3115,17 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>['contact', 'registration', 'questions', 'tender', 'feedback']</t>
+          <t>['contact', 'registration', 'questions', 'tender', 'QR code', 'Birmingham']</t>
         </is>
       </c>
       <c r="E84" t="n">
         <v>0.5</v>
       </c>
       <c r="F84" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G84" t="n">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="H84" t="n">
         <v>0.8</v>
@@ -3137,17 +3137,17 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>thank you thanks so much for that presentation Phil I don't know if you want to come up to field any questions that we have we're now moving on to question and answer session we have quite a few on slido at the minute actually quite a few have been answered as the as the presentations have gone on so so I'll sort of maybe take this opportunity to go through a very popular one that may or may not be controversial but I'll ask it anyway it says as Philip said yet another framework are you saying that none of the existing Frameworks to supply these project skills and roles are exist already including the new DSP essentially why why do we need this one on top of what we already have sorry Ali could you sorry</t>
+          <t>Thank you, thanks so much for that presentation, Phil. I don't know if you want to come up to field any questions that we have. We're now moving on to the question and answer session. We have quite a few on Slido at the minute, actually quite a few have been answered as the presentations have gone on, so I'll sort of maybe take this opportunity to go through a very popular one that may or may not be controversial, but I'll ask it anyway. It says, "As Philip said, yet another framework - are you saying that none of the existing frameworks to supply these project skills and roles exist already, including the new DSP? Essentially, why do we need this one on top of what we already have?" Sorry, Ali, could you... sorry?</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Project Skills</t>
+          <t>Project Frameworks</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>['Framework', 'DSP', 'Skills', 'Roles']</t>
+          <t>['Frameworks', 'Project Skills', 'Roles', 'DSP', 'Controversial']</t>
         </is>
       </c>
       <c r="E85" t="n">
@@ -3157,7 +3157,7 @@
         <v>0.2</v>
       </c>
       <c r="G85" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="H85" t="n">
         <v>0.8</v>
@@ -3169,27 +3169,27 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>yeah it's a really good question I'm sure Michael have a perspective on this too but essentially what we're not saying as a result of this framework is that there are not some excellent Frameworks already in existence with ccs what those Frameworks don't do however is allow us to achieve some of the things we want to achieve as a result of putting Dallas in place so we talked about ongoing competitive tension we talked about information sharing we talked about the opportunities for very rapid competition we can only really do those things in the the setting of having a framework that has a smaller number of suppliers on each of the Lots where those suppliers are become familiar and develop Partnerships with us in a very rapid period of time so that they can understand how we do business and by virtue of those things enable us to have those quick competition turnarounds in four to six weeks to respond with agility to the things that develop so whilst there are some exceptional Frameworks in place that covers some of these things they don't do them in quite</t>
+          <t>Yeah, it's a really good question. I'm sure Michael have a perspective on this too, but essentially what we're not saying as a result of this framework is that there are not some excellent Frameworks already in existence with CCS. What those Frameworks don't do, however, is allow us to achieve some of the things we want to achieve as a result of putting Dallas in place. So, we talked about ongoing competitive tension, we talked about information sharing, we talked about the opportunities for very rapid competition. We can only really do those things in the setting of having a framework that has a smaller number of suppliers on each of the Lots, where those suppliers become familiar and develop Partnerships with us in a very rapid period of time, so that they can understand how we do business and by virtue of those things enable us to have those quick competition turnarounds in four to six weeks to respond with agility to the things that develop. So, whilst there are some exceptional Frameworks in place that covers some of these things, they don't do them in quite the same way.</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Dallas Framework</t>
+          <t>Competition Framework</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>['Michael', 'competitive tension', 'information sharing', 'Partnerships', 'agility']</t>
+          <t>['Competition', 'Framework', 'CCS', 'Dallas', 'Partnerships']</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F86" t="n">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="G86" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="H86" t="n">
         <v>0.2</v>
@@ -3201,17 +3201,17 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>the way we need to move forward within hmrc and there are a number of other departments as Mike mentioned before that are in precisely the same boat and are looking to use some of the principles that we're trying to introduce here but Mike did you want to adjust on that yeah just to add to that that you know part of the early days of this program we we challenged each other hmrc and CCS around what Frameworks could align and how could we align those Frameworks and and make their work for what hmrc were wanting to deliver and wanted to get out of it and what we come to is that actually there is no perfect scenario for us and this actually helps us and when we talk to other customers this is also an effective mechanism to help them as well I think just to add as well that hmrc has always been quite aware of the fact that we're a bit of a canary in a coal mine on this particular one because if some of the principles and mechanisms that we're looking to introduce actually work well and have the utility to start to scale across other government</t>
+          <t>The way we need to move forward within HMRC, and there are a number of other departments as Mike mentioned before, that are in precisely the same boat and are looking to use some of the principles that we're trying to introduce here. But Mike, did you want to adjust on that? Yeah, just to add to that, that you know, part of the early days of this program, we challenged each other, HMRC and CCS, around what Frameworks could align and how could we align those Frameworks and make them work for what HMRC were wanting to deliver and wanted to get out of it. And what we come to is that actually there is no perfect scenario for us, and this actually helps us. And when we talk to other customers, this is also an effective mechanism to help them as well. I think just to add as well that HMRC has always been quite aware of the fact that we're a bit of a canary in a coal mine on this particular one, because if some of the principles and mechanisms that we're looking to introduce actually work well and have the utility to start to scale across other government.</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>HMR &amp; CCS</t>
+          <t>HMRC Scaling</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>['hmrc', 'ccs', 'frameworks', 'program', 'customers', 'government']</t>
+          <t>['HMRC', 'CCS', 'Frameworks', 'Scaling', 'Government']</t>
         </is>
       </c>
       <c r="E87" t="n">
@@ -3221,10 +3221,10 @@
         <v>0.7</v>
       </c>
       <c r="G87" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="H87" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="88">
@@ -3233,27 +3233,27 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>departments there are things here that could become much more commonplace within CCS Frameworks of the future and there's already deliberations happening in relation to tech services four I understand to start to think about how that could be shaped with some of the principles that we're looking to introduce here yes definitely new regulations coming in next year for us as well maybe help move things along so again we're thinking of you know thinking of models that help our customers going forward thanks Mike thanks are there any questions in the room anybody in the room have a question Julia we have a question we just need the mic so that those online can also hear as well so yeah if right down in the front here Julia could you just as you ask me a question if you could at least your name in which organization did you raise your hand so Juliet thank you let's see can you mentioned that</t>
+          <t>Departments, there are things here that could become much more commonplace within CCS Frameworks of the future, and there's already deliberations happening in relation to tech services four. I understand to start to think about how that could be shaped with some of the principles that we're looking to introduce here. Yes, definitely new regulations coming in next year for us as well, maybe help move things along. So, again, we're thinking of, you know, thinking of models that help our customers going forward. Thanks, Mike. Thanks. Are there any questions in the room? Anybody in the room have a question? Julia, we have a question. We just need the mic so that those online can also hear as well. So, yeah, if right down in the front here, Julia, could you just as you ask me a question if you could at least your name in which organization did you raise your hand? So, Juliet, thank you. Let's see, can you mentioned that?</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>CCS Frameworks</t>
+          <t>Tech Services</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>['departments', 'tech services', 'regulations', 'models', 'customers']</t>
+          <t>['CCS Frameworks', 'Regulations', 'Models', 'Customers']</t>
         </is>
       </c>
       <c r="E88" t="n">
         <v>0.5</v>
       </c>
       <c r="F88" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G88" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="H88" t="n">
         <v>0.8</v>
@@ -3265,27 +3265,27 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>so we can expand a little but obviously the the ITT packs aren't going to be going out until February so there's still some more development to be done and some of that development will actually happen as a consequence of some of the conversations that we have in Birmingham at the end of the month because as has been mentioned we don't want to close the book on the art of the possible if there's something that can genuinely help us proposition that we have here but the essentially what we were thinking about is that in lot 2A and 4A where we have larger suppliers we would set a mechanism whereby if the profit margin that was generated from the framework exceeded 25 then in bandings above 25 percent it would be possible to remit a percentage of the excess profit above 25 into Innovation funds and those Innovation funds would then enable us to fund things like the facilitated citizen coder sessions or potentially prototyping activity that may come into</t>
+          <t>So, we can expand a little, but obviously the ITT packs aren't going to be going out until February, so there's still some more development to be done. And some of that development will actually happen as a consequence of some of the conversations that we have in Birmingham at the end of the month, because, as has been mentioned, we don't want to close the book on the art of the possible if there's something that can genuinely help us proposition that we have here. But essentially what we were thinking about is that in Lot 2A and 4A, where we have larger suppliers, we would set a mechanism whereby if the profit margin that was generated from the framework exceeded 25%, then in bandings above 25%, it would be possible to remit a percentage of the excess profit above 25% into Innovation funds. And those Innovation funds would then enable us to fund things like the facilitated citizen coder sessions or potentially prototyping activity that may come into play.</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Innovation Funds</t>
+          <t>Innovation funds</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>['ITT', 'profit margin', 'framework', 'bandings', 'Innovation funds', 'facilitated citizen coder']</t>
+          <t>['ITT packs', 'Birmingham', 'Lot 2A', 'Lot 4A', 'Innovation funds']</t>
         </is>
       </c>
       <c r="E89" t="n">
         <v>0.5</v>
       </c>
       <c r="F89" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G89" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H89" t="n">
         <v>0.2</v>
@@ -3297,17 +3297,17 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>the the area of lot one so that's that's the broad principle that we're looking to apply but the exact bandings and what the values are on there we haven't settled on yet another question here thanks Holly thanks so much Chris Farthing advice Cloud if an SME was to apply directly for the lots of relevant for can they also still apply for the supply chain ones as well as in going going alongside with the big boys absolute PS yeah there's also some some advantage in that I would I would suggest because it enables greater opportunity to flex across different lots for some views possible so we're definitely Keen to encourage encourage that the only restriction that we're actually making is that you cannot Supply on both lot 4A and 4B as the same lead supplier and lot 2A and 2B so it applies on</t>
+          <t>The broad principle that we're looking to apply is that the area of Lot One. The exact bandings and values haven't been settled on yet. Another question here: if an SME was to apply directly for the lots relevant for them, can they also still apply for the supply chain ones as well as going alongside with the big boys? Absolutely! There's also some advantage in that, I would suggest, because it enables greater opportunity to flex across different lots for some views possible. We're definitely keen to encourage that. The only restriction that we're actually making is that you cannot supply on both Lot 4A and 4B as the same lead supplier and Lot 2A and 2B, so it applies on.</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>SME applications</t>
+          <t>Supply Chain</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>['SME', 'supply chain', 'lots', 'flexibility']</t>
+          <t>['SME', 'Lot One', 'Bandings', 'Values', 'Supply Chain']</t>
         </is>
       </c>
       <c r="E90" t="n">
@@ -3329,27 +3329,27 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>both of those both of those parts of the framework anymore Julia hi it's Rob Malcolm from dxc I've got a process question if that's okay in terms of the SQ itself the intent of the SQ I assume is to down select the number of supplies to take forward to the ITT could you just describe that process and how many you were expecting to take through to that next phase and then if you could just further expand on how many you supplies to expect to see on each lot at the end of the process many thanks so we may actually be able to get the slide back potentially which identifies how many suppliers were intending to appoint to each of the lots for the SQ phase you are absolutely right it's it's being used to narrow the list down so that it doesn't become too great a an evaluation headache for the department and for CCS because with something this new if we were to end up having to plow through hundreds and</t>
+          <t>Both of those parts of the framework anymore? Julia, hi, it's Rob Malcolm from DXC. I've got a process question, if that's okay. In terms of the SQ itself, the intent of the SQ, I assume, is to down select the number of supplies to take forward to the ITT. Could you just describe that process and how many you were expecting to take through to that next phase? And then, if you could just further expand on how many you supplies to expect to see on each lot at the end of the process? Many thanks. So, we may actually be able to get the slide back potentially, which identifies how many suppliers were intending to appoint to each of the lots for the SQ phase. You are absolutely right, it's it's being used to narrow the list down so that it doesn't become too great a an evaluation headache for the department and for CCS, because with something this new, if we were to end up having to plow through hundreds and...</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Process Question</t>
+          <t>Process question</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>['Rob Malcolm', 'SQ', 'ITT', 'slide', 'CCS']</t>
+          <t>['SQ', 'ITT', 'supplies', 'slide', 'lots', 'CCS']</t>
         </is>
       </c>
       <c r="E91" t="n">
         <v>0.5</v>
       </c>
       <c r="F91" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G91" t="n">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="H91" t="n">
         <v>0.9</v>
@@ -3361,17 +3361,17 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>hundreds of tenders then it could potentially delay us from a timeline point of view and hmrc is very much on the clock with this because we're looking to try and get it in at a time roughly around the expiry of the initial terms of some existing contracts so that that's what's driving some of those decisions but broadly speaking we're looking to down select to double the number of suppliers that we intend to appoint to the framework a lot now there may be one or two variations around that particularly if you end up with unlock one for example the suppliers that are our 10th and 11th on the list if they score identically then we would probably take them through on an identical score but generally we will set the set the level and and cut off everything below that level but broadly speaking we're aiming for double double the figures that you see on the screen there hi Ed development Triad just carry on from Chris's question as an SME we will</t>
+          <t>Hundreds of tenders could potentially delay us from a timeline point of view. HMRC is very much on the clock with this because we're looking to try and get it in at a time roughly around the expiry of the initial terms of some existing contracts. So, that's what's driving some of those decisions. But, broadly speaking, we're looking to down select to double the number of suppliers that we intend to appoint to the framework. There may be one or two variations around that, particularly if you end up with unlock one for example the suppliers that are our 10th and 11th on the list, if they score identically then we would probably take them through on an identical score. But, generally, we will set the set the level and and cut off everything below that level. But, broadly speaking, we're aiming for double double the figures that you see on the screen. Hi Ed development Triad, just carry on from Chris's question, as an SME we will.</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>SME Tenders</t>
+          <t>Supplier Framework</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>['tenders', 'HMRC', 'timeline', 'contracts', 'suppliers', 'framework', 'variations', 'score', 'cut off']</t>
+          <t>['tenders', 'HMRC', 'down select', 'unlock one', 'SME']</t>
         </is>
       </c>
       <c r="E92" t="n">
@@ -3381,7 +3381,7 @@
         <v>0.8</v>
       </c>
       <c r="G92" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="H92" t="n">
         <v>0.2</v>
@@ -3393,7 +3393,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>be able to apply with other Primes in the same lot if that makes sense thanks so just to understand the question then so if there are five primes in lot 2A yes could we join or apply with several primes within the same lot yeah absolutely I mean obviously the there will be conversations and discussions that you will enter into with those primes about the nature of the working agreement that would exist between you but we would want to place no constraint on any supply chain members from operating with with multiple suppliers across those lots so I suppose technically you could end up as a as a supplier for five of the lead suppliers within one of the lots and also as a direct supplier in the B part of the lot which for smes might maximize your opportunity to to generate business but obviously we've talked a lot about capacity we've talked a lot about capability and</t>
+          <t>Be able to apply with other Primes in the same lot if that makes sense. Thanks, so just to understand the question then, so if there are five Primes in Lot 2A, yes, could we join or apply with several Primes within the same lot? Yeah, absolutely. I mean, obviously, there will be conversations and discussions that you will enter into with those Primes about the nature of the working agreement that would exist between you, but we would want to place no constraint on any supply chain members from operating with multiple suppliers across those lots. So, I suppose technically, you could end up as a supplier for five of the lead suppliers within one of the lots and also as a direct supplier in the B part of the lot, which, for SMEs, might maximize your opportunity to generate business, but obviously we've talked a lot about capacity, we've talked a lot about capability and...</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3403,7 +3403,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>['Primes', 'Lot', 'Agreement', 'SMEs', 'Capability']</t>
+          <t>['Primes', 'Lot 2A', 'Supply Chain', 'SMEs', 'Capacity']</t>
         </is>
       </c>
       <c r="E93" t="n">
@@ -3425,27 +3425,27 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>that is important to us and so I think the openness that we're looking to develop in the partnership arrangements with the suppliers would necessitate a situation where we would have to have fairly robust conversations if suppliers were bite enough more than they could chew and likewise I think when we come to qualifying suppliers to be appointed to the Lots we will be looking at Financial standings to just determine whether or not they would be capable of at very least meeting the type of minimum workshare commitments that we would be proposing for the lot thanks I will take another question that came in on online there's a question about will there be any situation where you may still procure via other Frameworks such as dos or gcloud so I think the quick answer to that is we we wouldn't want to constrain ourselves so whatever options are available we'll do an analysis a commercial analysis and</t>
+          <t>That is important to us, and so I think the openness that we're looking to develop in the partnership arrangements with the suppliers would necessitate a situation where we would have to have fairly robust conversations if suppliers were 'bite' enough more than they could chew. And likewise, I think when we come to qualifying suppliers to be appointed to the Lots, we will be looking at Financial standings to just determine whether or not they would be capable of at very least meeting the type of minimum workshare commitments that we would be proposing for the lot. Thanks. I will take another question that came in online. There's a question about will there be any situation where you may still procure via other Frameworks such as DOS or GCloud? So I think the quick answer to that is we wouldn't want to constrain ourselves, so whatever options are available we'll do a commercial analysis.</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Procurement Frameworks</t>
+          <t>Procurement Process</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>['suppliers', 'Financial standings', 'minimum workshare commitments', 'dos', 'gcloud']</t>
+          <t>['Suppliers', 'Financial standings', 'Frameworks', 'Commercial analysis']</t>
         </is>
       </c>
       <c r="E94" t="n">
         <v>0.5</v>
       </c>
       <c r="F94" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G94" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H94" t="n">
         <v>0.2</v>
@@ -3457,7 +3457,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>determine what the best route to Market is from a strategic point of view for hmrc it would make sense for us wherever possible to put as much work through the Dallas framework as possible and there's no loss to CCS from that either because obviously being a CCS framework it attracts the levy so whenever we spend through this becomes a virtuous circle for all of government in terms of spend under management but as things start to move forward you may start to see the other forays into the market that hmrc has made in things like data and sap start to unify under this type of approach in future iterations too another one from online Can hmrc facilitate introductions or contact sharing for a larger primes and interested smes Mike do you want to take that yeah so CCs is kindly volunteered to facilitate those arrangements okay</t>
+          <t>Determine what the best route to Market is from a strategic point of view for HMRC. It would make sense for us, wherever possible, to put as much work through the Dallas framework as possible and there's no loss to CCS from that either, because obviously being a CCS framework it attracts the levy, so whenever we spend through this becomes a virtuous circle for all of government in terms of spend under management. But as things start to move forward, you may start to see the other forays into the market that HMRC has made in things like data and SAP start to unify under this type of approach in future iterations too. Another one from online: Can HMRC facilitate introductions or contact sharing for larger primes and interested SMEs? Mike, do you want to take that? Yeah, so CCS has kindly volunteered to facilitate those arrangements. Okay.</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3467,7 +3467,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>['HMRC', 'Dallas', 'CCS', 'Data', 'SAP', 'PRIME', 'SME']</t>
+          <t>['HMRC', 'Market', 'Dallas', 'CCS', 'Data', 'SAP', 'Levy', 'Government', 'Primes', 'SMES']</t>
         </is>
       </c>
       <c r="E95" t="n">
@@ -3477,10 +3477,10 @@
         <v>0.7</v>
       </c>
       <c r="G95" t="n">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="H95" t="n">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="96">
@@ -3489,27 +3489,27 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>thanks [Music] could you please list the distinct nine Technologies so the nine Technologies are on the slide deck which is okay CCS website but I'm Testament memory now but the Pega systems Microsoft Dynamics Microsoft Power Platform Office 365 apps Kong document nice and sap yes so well done thank you there's a question at the back hello there Chris Gallagher confluent I'm looking at the annual values and the number of suppliers the primes are still going to have to be fairly large I would argue because they are they're large annual values right will you be spelling out what a good Prime will look like I'm not saying names but what good would look like if you see what I mean because I think that would be extremely useful thank you interestingly the I mentioned before about the work stream that we've just set up and Rich may want to talk a little bit more about this in</t>
+          <t>Thanks [Music]. Could you please list the distinct nine Technologies? So, the nine Technologies are on the slide deck, which is okay CCS website, but I'm Testament memory now. But the Pega systems, Microsoft Dynamics, Microsoft Power Platform, Office 365 apps, Kong document nice, and SAP, yes. So, well done. Thank you. There's a question at the back. Hello there, Chris Gallagher, Confluent. I'm looking at the annual values and the number of suppliers. The primes are still going to have to be fairly large, I would argue, because they are they're large annual values, right? Will you be spelling out what a good Prime will look like? I'm not saying names, but what good would look like, if you see what I mean, because I think that would be extremely useful. Thank you. Interestingly, the I mentioned before about the work stream that we've just set up, and Rich may want to talk a little bit more about this in.</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Nine Technologies</t>
+          <t>Technology Suppliers</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>['CCS', 'Testament', 'Memory', 'Pega', 'Microsoft Dynamics', 'Power Platform', 'Office 365', 'Kong', 'Document', 'SAP']</t>
+          <t>['Technology', 'Suppliers', 'Prime', 'Annual Values', 'Work Stream']</t>
         </is>
       </c>
       <c r="E96" t="n">
         <v>0.5</v>
       </c>
       <c r="F96" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G96" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="H96" t="n">
         <v>0.8</v>
@@ -3521,7 +3521,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>a moment but we've just set up a work stream looking at a a broad brush picture of what we're looking for from suppliers both in terms of the characteristics of the supplier the capacity their capability their ability to work in partnership with us their ability to collaborate with other suppliers and the types of activities they would be expected to deliver deliver and the standard kpi sets that would apply to all of the suppliers in certain lots that that is happening as we speak so hopefully that will address an awful lot of the the content of the question there but I'm happy to hand over to sorry Rick thank you smiling advice card again to mind this is going to be services-based procurement isn't it you're not looking for the supplier to actually Supply the technology as well are you no it's it's purely Services based and I mean obviously it was it was covered in the presentation that over time there will</t>
+          <t>A moment, but we've just set up a work stream looking at a broad brush picture of what we're looking for from suppliers, both in terms of the characteristics of the supplier, the capacity, their capability, their ability to work in partnership with us, their ability to collaborate with other suppliers, and the types of activities they would be expected to deliver and the standard KPI sets that would apply to all of the suppliers in certain lots. That is happening as we speak, so hopefully that will address an awful lot of the content of the question there, but I'm happy to hand over to Rick. Thank you. Smiling advice card again to mind. This is going to be services-based procurement, isn't it? You're not looking for the supplier to actually supply the technology as well, are you? No, it's purely services-based and I mean, obviously it was covered in the presentation that over time there will be.</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3531,20 +3531,20 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>['Services', 'Capability', 'Partnership', 'Collaboration', 'KPI']</t>
+          <t>['services-based', 'KPI sets', 'supplier characteristics', 'capacity', 'capability', 'partnership', 'collaboration', 'technology']</t>
         </is>
       </c>
       <c r="E97" t="n">
         <v>0.5</v>
       </c>
       <c r="F97" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G97" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H97" t="n">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="98">
@@ -3553,7 +3553,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>be a shift away from coding toward configuration so those technologies will already exist as either platform as a service or software as a service and then the services will be work packages involved in configuring those services for specific use cases thanks I'll take one from from online how will hmrc integrate social value in such a large and long framework I think that's a to be concluded so there will definitely be detailed information when it comes to the the ITT stage what we've done on this in the past though is we've focused on four action themes generally which are to do with well-being societal impact equality and we've previously looked at covert recovery and particularly the impact on local communities when it comes to code recovery but that's less of a a challenge now so we may just major on on three of those areas rather than rather than four moving forward but</t>
+          <t>Be a shift away from coding toward configuration, so those technologies will already exist as either platform as a service or software as a service, and then the services will be work packages involved in configuring those services for specific use cases. Thanks, I'll take one from online: How will HMRC integrate social value in such a large and long framework? I think that's a to be concluded, so there will definitely be detailed information when it comes to the ITT stage. What we've done on this in the past though is we've focused on four action themes generally, which are to do with well-being, societal impact, equality, and we've previously looked at covert recovery and particularly the impact on local communities when it comes to code recovery, but that's less of a challenge now, so we may just major on three of those areas rather than four moving forward, but...</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>['social value', 'framework', 'ITT stage', 'well-being', 'societal impact', 'equality']</t>
+          <t>['social value', 'framework', 'ITT stage', 'action themes', 'covert recovery']</t>
         </is>
       </c>
       <c r="E98" t="n">
@@ -3585,17 +3585,17 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>certainly when it comes to sustainability and carbon reduction it's already been trailed in the presentation around how the carbon reduction plans need to be made available I understand that it's going to be a requirement of the SQ phase that those carbon reduction plans will be put on suppliers websites with a link provided in the SQ return so just to trail that well in advance as well as producing the plan it needs to be present on your website when you submit the SQ great what is hmrc's appetite to offshoring is this seen as part of the future mix so it's a good question and it came up repeatedly during the tsp procurements that we did I think the short answer is that we wouldn't want to constrain ourselves when it comes to opportunities but there is and is all has always been a small P political issue when it comes to offshoring particularly at a time when from a financial point of view an economic point of view</t>
+          <t>Certainly, when it comes to sustainability and carbon reduction, it's already been trailed in the presentation around how the carbon reduction plans need to be made available. I understand that it's going to be a requirement of the SQ phase that those carbon reduction plans will be put on suppliers' websites, with a link provided in the SQ return. So, just to trail that well in advance, as well as producing the plan, it needs to be present on your website when you submit the SQ. Great! What is HMRC's appetite to offshoring? Is this seen as part of the future mix? So, it's a good question and it came up repeatedly during the TSP procurements that we did. I think the short answer is that we wouldn't want to constrain ourselves when it comes to opportunities, but there is - and has always been - a small political issue when it comes to offshoring, particularly at a time when, from a financial point of view and an economic point of view, an offshoring approach is attractive.</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Offshoring Appetite</t>
+          <t>Offshoring HMRC</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>['Sustainability', 'Carbon Reduction', 'HMRC', 'Offshoring', 'TSP']</t>
+          <t>['sustainability', 'carbon reduction', 'HMRC', 'offshoring', 'TSP']</t>
         </is>
       </c>
       <c r="E99" t="n">
@@ -3617,7 +3617,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>there's there are struggles within the country there's the potential for the effect of inflation and energy cost Rises and what have you to affect employment so the small P political side of things is the question of whether or not it would be right for us to Offshore certain things at a time when there may be a threat to employment in the UK so we always have to balance those things out under any circumstances we do not offshore data so all data is in the UK but we we wouldn't say no never to other things but it would have to be taken on a case-by-case basis so and I will just say Brooke for other customers they may wish to have offshore in so you know we're not going to exclude it at the framework level it's whether it's used and utilized within the call-off level that's going to be relevant thanks we have a question about are there any mandated certifications or accreditations that all suppliers need to have ISO for instance</t>
+          <t>There's there are struggles within the country. There's the potential for the effect of inflation and energy cost rises and what have you to affect employment. So, the small political side of things is the question of whether or not it would be right for us to offshore certain things at a time when there may be a threat to employment in the UK. So, we always have to balance those things out. Under any circumstances, we do not offshore data, so all data is in the UK. But, we wouldn't say no never to other things, but it would have to be taken on a case-by-case basis. So, and I will just say, for other customers, they may wish to have offshore in. So, you know, we're not going to exclude it at the framework level. It's whether it's used and utilized within the call-off level that's going to be relevant. Thanks. We have a question about are there any mandated certifications or accreditations that all suppliers need to have, ISO for instance?</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3627,7 +3627,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>['employment', 'inflation', 'energy cost', 'UK', 'offshore', 'data', 'certifications', 'accreditations', 'ISO']</t>
+          <t>['employment', 'inflation', 'energy cost', 'offshoring', 'certifications', 'accreditations']</t>
         </is>
       </c>
       <c r="E100" t="n">
@@ -3640,7 +3640,7 @@
         <v>0.7</v>
       </c>
       <c r="H100" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="101">
@@ -3649,7 +3649,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>yes we're working we're working through all of those and making sure we got the right accreditations the right levels with their cyber security cyber Essentials whatever it is we'll make sure that's clear about what it is we're asking for but we will need to make to make sure that they are the recognized bodies that are all grows those accreditations and just to to expand on that that the pack we mentioned before what it means to supply to hmrc pack essentially will start to lay out some of that detail too around what accreditations would be essential to work with hmrc specific to the framework when you think about Lot 4 and the fact that that is focused on specific strategic Technologies our expectation would be that for the technologies that you report for wanting to supply you would be accredited to at least silver status with the technology vendor we have one in the back and then we'll come to you so yeah a bit of a boost guide question I guess Phil but what's</t>
+          <t>Yes, we're working. We're working through all of those and making sure we got the right accreditations, the right levels with their cyber security, cyber Essentials, whatever it is, we'll make sure that's clear about what it is we're asking for, but we will need to make to make sure that they are the recognized bodies that are all grows those accreditations. And just to to expand on that, that the pack we mentioned before, what it means to supply to HMRC pack, essentially will start to lay out some of that detail too around what accreditations would be essential to work with HMRC specific to the framework. When you think about Lot 4 and the fact that that is focused on specific strategic Technologies, our expectation would be that for the technologies that you report for wanting to supply you would be accredited to at least silver status with the technology vendor. We have one in the back and then we'll come to you. So yeah, a bit of a boost guide question I guess Phil, but what's?</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>['Cyber Security', 'Accreditations', 'HMRC', 'Lot 4', 'Silver Status']</t>
+          <t>['accreditations', 'HMRC', 'Lot 4', 'silver status', 'technology vendor']</t>
         </is>
       </c>
       <c r="E101" t="n">
@@ -3681,30 +3681,30 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>the percentage ratio of the money being spent going to be to large-scale programs as opposed to smaller ones on the top 2B do you think out of 150 million it was all spent so at the moment it's impossible for us to state that with any certainty but broadly speaking what we're looking to do is allocate on the basis of work packages and the way things stand work packages with a value in excess of a million pounds will go into the a part of the lot less than a million pounds will go into the B part of the lot and there'll be figures below a million pounds for the B part of the lot that will then make up the the levels for all the tiers for the taxi rank allocation of work go ahead hi Phil it's David Hunt from Lidos for tsp there was a sort of Drop Dead date that was the expiry of the Aspire and other contracts in the June time frame this year you mentioned this is time</t>
+          <t>The percentage ratio of the money being spent going to be to large-scale programs as opposed to smaller ones on the top 2B - do you think out of 150 million it was all spent? So, at the moment, it's impossible for us to state that with any certainty, but broadly speaking, what we're looking to do is allocate on the basis of work packages. And the way things stand, work packages with a value in excess of a million pounds will go into the A part of the lot, less than a million pounds will go into the B part of the lot, and there'll be figures below a million pounds for the B part of the lot that will then make up the levels for all the tiers for the taxi rank allocation of work. Go ahead, Hi Phil, it's David Hunt from Lidos for TSP. There was a sort of Drop Dead date that was the expiry of the Aspire and other contracts in the June time frame this year - you mentioned this is time?</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Taxi Rank Allocation</t>
+          <t>Taxi Allocation</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>['money', 'programs', 'work packages', 'million pounds', 'taxi rank']</t>
+          <t>['Money', 'Work Packages', 'Taxi Rank', 'Drop Dead Date']</t>
         </is>
       </c>
       <c r="E102" t="n">
         <v>0.5</v>
       </c>
       <c r="F102" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="G102" t="n">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="H102" t="n">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="103">
@@ -3713,30 +3713,30 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>constrained or time pressured what are the time constraints that are causing you to stick to this particular times table that you've offered now well you're right it's more time pressured and time constrained with Dallas but we do have of the contracts that we let under tsp as as Lee referenced earlier on we always knew that a lot of them would be stepping stone contracts because we wouldn't be at a state of maturity to enable us to move to the type of operating model but of those contracts I believe 19 of the 32 contracts that we've seen immediately within scope of Dallas will expire between September 2023 and January 2025 so consequently as those initial terms expire we'll be looking as early as possible to move them into this structure thanks will suppliers be expected to provide people to work on the customer site or is remote working allowed so we've switched to virtually all remote working within hmrc now following</t>
+          <t>Constrained or time pressured? What are the time constraints that are causing you to stick to this particular times table that you've offered now? Well, you're right, it's more time pressured and time constrained with Dallas, but we do have of the contracts that we let under TSP, as Lee referenced earlier on, we always knew that a lot of them would be stepping stone contracts because we wouldn't be at a state of maturity to enable us to move to the type of operating model. But of those contracts, I believe 19 of the 32 contracts that we've seen immediately within scope of Dallas will expire between September 2023 and January 2025. So, consequently, as those initial terms expire, we'll be looking as early as possible to move them into this structure. Thanks. Will suppliers be expected to provide people to work on the customer site, or is remote working allowed? We've switched to virtually all remote working within HMRC now following.</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>HMRC Contracts</t>
+          <t>Time constraints</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>['constrained', 'time', 'pressure', 'Dallas', 'contracts']</t>
+          <t>['time', 'contracts', 'remote working', 'HMRC', 'Dallas']</t>
         </is>
       </c>
       <c r="E103" t="n">
         <v>0.5</v>
       </c>
       <c r="F103" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="G103" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="H103" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="104">
@@ -3745,27 +3745,27 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>covid and we we don't anticipate that changing markedly but obviously there will be requirements at times to attend in person and and they would be detailed in the the statements of work and call offs that are generated okay thank you but there's one in the room hi Clive Friedman from log point my question is not so much about the framework but more about the drivers so in your presentation you talk I saw at least 1500 contractors and I'm sure there's many multiples more in hmrc what would good look like as a result of this in terms of the contractors given that the contractors also have the corporate memory of hmrc and the objective is to move in-house what would be the position of looking at those contractors as potentials for assisting in whether it be SME or into Indie primes to tap well certainly for anyone who wanted to bed we wouldn't discourage contacting</t>
+          <t>Covid and we don't anticipate that changing markedly, but obviously there will be requirements at times to attend in person and they would be detailed in the statements of work and call offs that are generated. Okay, thank you. But there's one in the room. Hi Clive Friedman from Log Point. My question is not so much about the framework, but more about the drivers. So, in your presentation you talk I saw at least 1500 contractors and I'm sure there's many multiples more in HMRC. What would good look like as a result of this in terms of the contractors? Given that the contractors also have the corporate memory of HMRC and the objective is to move in-house, what would be the position of looking at those contractors as potentials for assisting in whether it be SME or into Indie primes to tap? Well, certainly for anyone who wanted to, we wouldn't discourage contacting.</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>HMRC Contractors</t>
+          <t>HMRC contractors</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>['covid', 'contractors', 'SME', 'Indie primes']</t>
+          <t>['covid', 'contractors', 'HMRC', 'SME', 'Indie primes']</t>
         </is>
       </c>
       <c r="E104" t="n">
         <v>0.5</v>
       </c>
       <c r="F104" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G104" t="n">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="H104" t="n">
         <v>0.8</v>
@@ -3777,7 +3777,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>the organizations that are in hmrc operating today because an Institutional memory may well be useful in helping you to create bids and subsequently to deliver services I think ultimately in terms of what good would look like and what we're trying to achieve it's very much about that shift towards intelligent clients and again I'll give Rich the opportunity to come in on that one possibly yes I think that this part about moving to intelligent clients and but I think the framework is about really shifting to outcome pieces of work being able to contract for outcomes and taking smaller more self-contained piece of work within that ecosystem of Partners on the framework which which is part of that journey and being able to separate the work and deliver work in small in small chunks is is really part of delivering that strategy for hmrc so retaining that knowledge the intelligent client knowledge in-house but having that ecosystem of Partners to deliver those outcomes for us through a a flexible framework</t>
+          <t>The organizations that are in HMRC operating today because an Institutional memory may well be useful in helping you to create bids and subsequently to deliver services. I think ultimately, in terms of what good would look like and what we're trying to achieve, it's very much about that shift towards intelligent clients and again I'll give Rich the opportunity to come in on that one possibly. Yes, I think that this part about moving to intelligent clients and, but I think the framework is about really shifting to outcome pieces of work, being able to contract for outcomes and taking smaller, more self-contained pieces of work within that ecosystem of Partners on the framework, which is part of that journey and being able to separate the work and deliver work in small chunks is really part of delivering that strategy for HMRC. So, retaining that knowledge, the intelligent client knowledge in-house, but having that ecosystem of Partners to deliver those outcomes for us through a flexible framework.</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3787,20 +3787,20 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>['hmrc', 'Institutional memory', 'bids', 'services', 'outcomes', 'ecosystem', 'Partners', 'framework', 'knowledge']</t>
+          <t>['HMRC', 'Outcomes', 'Partners', 'Framework', 'Knowledge']</t>
         </is>
       </c>
       <c r="E105" t="n">
         <v>0.5</v>
       </c>
       <c r="F105" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G105" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H105" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="106">
@@ -3809,30 +3809,30 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>and I think our cdio dalgia it's been on record as effectively saying about how we as an organization need to balance better how we work with the market so whilst the intelligent client improves on our side of the house there would be more opportunities for us to put things out to the market that we currently do today largely using contingent labor or in some case of resource-based contracts with suppliers rather than outcome-based ones that we're looking to move towards here I'm very conscious by the way that there's been very few technical questions and we've got Jillian and Rich and Dean sat waiting with baited breath for any technical questions so if you do have them I don't this probably doesn't qualify as a technical questions of apologies but it was mentioned that there will be open book requirements can you please expand on this it's a standard within all government contracts that generally we would require suppliers to submit to open</t>
+          <t>And I think our CDIO dalgia it's been on record as effectively saying about how we as an organization need to balance better how we work with the market. So, whilst the intelligent client improves on our side of the house, there would be more opportunities for us to put things out to the market that we currently do today largely using contingent labor or in some cases of resource-based contracts with suppliers rather than outcome-based ones that we're looking to move towards here. I'm very conscious by the way that there's been very few technical questions and we've got Jillian, Rich, and Dean sat waiting with baited breath for any technical questions. So, if you do have them, I don't this probably doesn't qualify as a technical question, of apologies, but it was mentioned that there will be open book requirements. Can you please expand on this? It's a standard within all government contracts that generally we would require suppliers to submit to open book.</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Government Contracts</t>
+          <t>Open Book</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>['cdio', 'intelligent client', 'contingent labor', 'resource-based contracts', 'outcome-based']</t>
+          <t>['CDIO', 'Intelligent Client', 'Contingent Labor', 'Resource-Based Contracts', 'Outcome-Based Contracts']</t>
         </is>
       </c>
       <c r="E106" t="n">
         <v>0.5</v>
       </c>
       <c r="F106" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G106" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H106" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="107">
@@ -3841,7 +3841,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>book costing and for us to have open book reviews periodically that we can commission it's not a given that we will commission them but that we could commission I think in the Lots where we would be looking at gain share as a means of funding Innovation it would be more likely that we would assert that right perhaps more frequently but yeah it would be as as it is in other government contracts where we get that level of detail to enable us to understand the impact that Dallas Activity is having on the the bottom line for your organization thank you is there a detailed list of services or Pipeline and how they map to each of the Lots this may help suppliers prioritize the most appropriate Lots so what we have at the moment is a list of contracts that are directly within the scope of Dallas and we're in the process through a work stream of building exactly that details of the the</t>
+          <t>Book costing, and for us to have open book reviews periodically that we can commission, it's not a given that we will commission them, but that we could commission. I think in the Lots where we would be looking at gain share as a means of funding Innovation, it would be more likely that we would assert that right perhaps more frequently, but yeah it would be as it is in other government contracts where we get that level of detail to enable us to understand the impact that Dallas Activity is having on the bottom line for your organization. Thank you. Is there a detailed list of services or Pipeline and how they map to each of the Lots? This may help suppliers prioritize the most appropriate Lots. So, what we have at the moment is a list of contracts that are directly within the scope of Dallas, and we're in the process through a work stream of building exactly that details of the...</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3851,7 +3851,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>['book', 'costing', 'open', 'reviews', 'commission']</t>
+          <t>['book costing', 'open book reviews', 'gain share', 'government contracts', 'Dallas Activity']</t>
         </is>
       </c>
       <c r="E107" t="n">
@@ -3873,24 +3873,24 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>types of work packages that will exist and how they map to to the various Lots within the framework so that will be made available at the ITT stage this is good morning my name's Robbie I'm from cloud Source I'll ask a certainly cool question for lot four you thanks for like naming the technologies that you want suppliers to provide I'm curious though to try and differentiate my organization whether we bid in lot 2B or in lot 4B lot to be a lot lot twos about digital services so what what outcomes are you looking to generate in lot for so the difference fundamentally is that in Lot 2 the the digital build services that will be aligned to the digital delivery centers to borders and trade and for Enterprise Integration will be largely done on a</t>
+          <t>Types of work packages that will exist and how they map to the various Lots within the framework will be made available at the ITT stage. This is good morning, my name's Robbie. I'm from Cloud Source. I'll ask a certainly cool question for Lot Four. You thanks for like naming the technologies that you want suppliers to provide. I'm curious though to try and differentiate my organization whether we bid in Lot 2B or in Lot 4B. Lot 2 is about digital services, so what outcomes are you looking to generate in Lot 4? So the difference fundamentally is that in Lot 2, the digital build services that will be aligned to the Digital Delivery Centers to Borders and Trade and for Enterprise Integration will be largely done on a.</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Lot 4B</t>
+          <t>Digital Services</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>['Lot 2B', 'Lot 4B', 'digital services', 'digital delivery centers', 'borders and trade', 'Enterprise Integration']</t>
+          <t>['Lot 2', 'Lot 4', 'Digital Services', 'Digital Delivery Centers', 'Borders and Trade', 'Enterprise Integration']</t>
         </is>
       </c>
       <c r="E108" t="n">
         <v>0.5</v>
       </c>
       <c r="F108" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="G108" t="n">
         <v>0.7</v>
@@ -3905,17 +3905,17 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>devsecops Model but using code of codable technology so things like scalar and Java and and some of the various other technologies that Jillian mentioned in her presentation the difference with Lot 4 is that it's all focused on configurable technology and so anything that comes into that sphere of being a configurable product or platform either from the list that we've provided earlier or get added to later on will automatically slot into Lot 4 and be configured rather than coded thank you another one from online how does the low code no code platform strategy affect how current Digital Services that are bespoke or code developed in the future will that change so rich do you wanna so I think if from from Tom's Video the future is to move to a a much more of a platform based architecture</t>
+          <t>DevSecOps model, but using code of codable technology, so things like scalar and Java and some of the various other technologies that Jillian mentioned in her presentation. The difference with Lot 4 is that it's all focused on configurable technology, and so anything that comes into that sphere of being a configurable product or platform, either from the list that we've provided earlier or get added to later on, will automatically slot into Lot 4 and be configured rather than coded. Thank you. Another one from online: How does the low code no code platform strategy affect how current Digital Services that are bespoke or code developed in the future? Will that change? So, Rich, do you wanna...? I think, if from from Tom's Video, the future is to move to a much more of a platform based architecture.</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Low Code Platform</t>
+          <t>Low Code Platforms</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>['devsecops', 'codable', 'scalar', 'Java', 'configurable', 'platform', 'architecture']</t>
+          <t>['DevSecOps', 'Codable Technology', 'Lot 4', 'Configurable Technology', 'Digital Services']</t>
         </is>
       </c>
       <c r="E109" t="n">
@@ -3928,7 +3928,7 @@
         <v>0.7</v>
       </c>
       <c r="H109" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="110">
@@ -3937,7 +3937,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>building on top of that primarily you're trying to use low code and no code Solutions as much as possible but I think as as this was was trailed up front this is part of a longer journey to move from from a lot of Legacy systems so we're going to be shifting that architecture over a period of time so that will that will be part of the digital Journey that hmrc goes on ideally we'll we'll introduce more and more of those Loco Technologies as we go along but we have to understand where we're starting from and need to build on that so so it allows us to evolve to that state of over over the next few years I think from a commercial perspective as well just to build on that you'll notice from the annual values that have been cited on the screen in front of you that there is more money currently focused on the digital development side of things than there is on the configurable side of things what will happen over time is that we will start to see a shift of money and potentially it might be iteration two or whatever the successor for Dallas becomes we'll start to see money more</t>
+          <t>Building on top of that, primarily you're trying to use low code and no code solutions as much as possible. But I think, as this was trailed up front, this is part of a longer journey to move from a lot of legacy systems, so we're going to be shifting that architecture over a period of time. So that will be part of the digital journey that HMRC goes on. Ideally, we'll introduce more and more of those low code technologies as we go along, but we have to understand where we're starting from and need to build on that, so it allows us to evolve to that state over the next few years. I think, from a commercial perspective, as well, just to build on that, you'll notice from the annual values that have been cited on the screen in front of you that there is more money currently focused on the digital development side of things than there is on the configurable side of things. What will happen over time is that we will start to see a shift of money and, potentially, it might be iteration two or whatever the successor for Dallas becomes, we'll start to see money more and more.</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3947,20 +3947,20 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>['low code', 'no code', 'Legacy systems', 'Loco Technologies', 'commercial perspective', 'digital development']</t>
+          <t>['low code', 'no code', 'legacy systems', 'digital development', 'configurable side']</t>
         </is>
       </c>
       <c r="E110" t="n">
         <v>0.5</v>
       </c>
       <c r="F110" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G110" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H110" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="111">
@@ -3969,17 +3969,17 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>money shift into the configurable platforms than we see today but within the life cycle of this framework and possibly even within the life cycle of its successor we're not going to get away from doing scholar and Java stack coding deployed on our multi-channel digital tax platform those services will still exist it's just that more there'll be a greater preponderance into Lot 4 over time foreign okay well Pega documentum development work be a part of this framework absolutely yes is there a specified security clearance per lot so it's not specified per lot it's more specified on the basis of the type of work that's being done so generally any work that involves use of live data requires SC clearance where there's no live data involved unless there's something specific that requires it to be have a higher security classification generally bpss is sufficient</t>
+          <t>Money shift into the configurable platforms than we see today, but within the life cycle of this framework and possibly even within the life cycle of its successor, we're not going to get away from doing scholar and Java stack coding deployed on our multi-channel digital tax platform. Those services will still exist; it's just that more there'll be a greater preponderance into Lot 4 over time. Foreign? Okay. Well, Pega documentum development work be a part of this framework? Absolutely, yes. Is there a specified security clearance per lot? So it's not specified per lot; it's more specified on the basis of the type of work that's being done. So generally any work that involves use of live data requires SC clearance, where there's no live data involved unless there's something specific that requires it to be have a higher security classification generally bpss is sufficient.</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Digital Tax Platform</t>
+          <t>Software Development</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>['money', 'Java', 'Lot 4', 'Pega', 'Documentum', 'SC clearance', 'BPSS']</t>
+          <t>['Software', 'Development', 'Security', 'Clearance', 'Platforms']</t>
         </is>
       </c>
       <c r="E111" t="n">
@@ -3992,7 +3992,7 @@
         <v>0.7</v>
       </c>
       <c r="H111" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="112">
@@ -4001,7 +4001,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>to say again that your framework level dependent hmrc may call it off in their in their call off contracts other customers May utilize and ask for different things so it's it's going to be as and when required the school off can you confirm the criteria to be used to assess a supplier as an SME what if the organization grows beyond this definition during the framework period So the appointment is made at the start of the framework and so the supplier would remain on the framework within that lot for the period of the framework in terms of the definition of SMA cabinet office has a specific definition which relates to the amount of employees and the turnover but it's specific to its operation as a worldwide entity so for example an organization may be an SME according to the numbers but if they have an overseas parent they can't be an SME technically because</t>
+          <t>To say again that your framework level dependent HMRC may call it off in their in their call off contracts. Other customers may utilize and ask for different things, so it's it's going to be as and when required. The school off can you confirm the criteria to be used to assess a supplier as an SME? What if the organization grows beyond this definition during the framework period? So the appointment is made at the start of the framework and so the supplier would remain on the framework within that lot for the period of the framework. In terms of the definition of SMA, Cabinet Office has a specific definition which relates to the amount of employees and the turnover, but it's specific to its operation as a worldwide entity. So, for example, an organization may be an SME according to the numbers, but if they have an overseas parent they can't be an SME technically because they.</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -4011,7 +4011,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>['hmrc', 'call off contracts', 'SME', 'cabinet office', 'overseas parent']</t>
+          <t>['HMRC', 'Call Off Contracts', 'SME', 'Cabinet Office', 'Overseas Parent']</t>
         </is>
       </c>
       <c r="E112" t="n">
@@ -4033,7 +4033,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>the parent can provide company guarantees or access to wider market capitalization here we go Julia well it's for the people online so that they can hear you as well so it's David I'm from Lidos again to what extent are the is the SQ going to be set against hmrc's criteria as opposed to the criteria that may reflect other departments requirements at the moment and I'm sure Michael come in if I get any of this wrong but at the moment we're jointly developing the SQ with ccs so that there will be a flavor for both so hmrc's requirements will come into that but ccs are also having a major input into that content but as Shannon and Miriam mentioned before our anticipation is that the SQ process is very much around looking backwards what are the skills capabilities experiences of you having</t>
+          <t>The parent can provide company guarantees or access to wider market capitalization. Here we go, Julia. Well, it's for the people online so that they can hear you as well. So it's David, I'm from Lidos again. To what extent are the SQ going to be set against HMRC's criteria as opposed to the criteria that may reflect other departments' requirements at the moment? And I'm sure Michael will come in if I get any of this wrong, but at the moment we're jointly developing the SQ with CCS, so that there will be a flavor for both. So HMRC's requirements will come into that, but CCS are also having a major input into that content. But, as Shannon and Miriam mentioned before, our anticipation is that the SQ process is very much around looking backwards - what are the skills, capabilities, experiences of you having?</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -4043,7 +4043,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>['company', 'guarantees', 'market', 'capitalization', 'HMRC', 'CCS']</t>
+          <t>['HMRC', 'CCS', 'Skills', 'Capabilities', 'Experiences']</t>
         </is>
       </c>
       <c r="E113" t="n">
@@ -4065,7 +4065,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>delivered in organizations of a similar size and scale to hmrc in this kind of operation where there would be supplier collaboration greater information sharing all of those things were looking to test based on your experiences in the past and then when we get to ITT phase it's very much going to be about what are you going to do for us today and the Monty Python one of the Romans done for us lately kind of sense and the needs will be very similar whether it's hmrc or another department they'll be very similar around what the criteria we're setting at the SQ level so it is CCS are leading that input from from Phil and the team plus our other knowledge of what's going on there because I think that's a follow-up question Julia of course yes yeah we we recognize that it is but we think we'll be we'll work through enough that we'll get a a good balance which will work for the framework</t>
+          <t>Delivered in organizations of a similar size and scale to HMRC in this kind of operation, where there would be supplier collaboration, greater information sharing, all of those things were looking to test based on your experiences in the past. And then when we get to ITT phase, it's very much going to be about what are you going to do for us today - the Monty Python 'What have the Romans done for us lately?' kind of sense. And the needs will be very similar whether it's HMRC or another department; they'll be very similar around what the criteria we're setting at the SQ level. So it is CCS are leading that input from Phil and the team, plus our other knowledge of what's going on there. Because I think that's a follow-up question, Julia - of course, yes. We recognize that it is, but we think we'll be we'll work through enough that we'll get a good balance which will work for the framework.</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -4075,7 +4075,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>['Supplier', 'Collaboration', 'Information', 'Sharing', 'ITT']</t>
+          <t>['HMRC', 'ITT', 'SQ Level', 'CCS', 'Phil', 'Julia']</t>
         </is>
       </c>
       <c r="E114" t="n">
@@ -4088,7 +4088,7 @@
         <v>0.7</v>
       </c>
       <c r="H114" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="115">
@@ -4097,7 +4097,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>someone is asking how many slots are available for the face-to-face one-to-one sessions so we've set aside enough capacity within the week in Birmingham to accommodate around 100 suppliers okay during the course of that week we'll have five five teams available but we can Flex up to six depending on uptake and as Mike mentioned before there's a limit of three representatives for each supplier organization during that week but it's it's an opportunity to to meet us face to face to ask us questions to make suggestions and hopefully we it can be a mutually beneficial Arrangement just to reiterate though any questions that we are asked in that setting we will be capturing and publishing as part of our responsibility to be fair and transparent to all of the bidders thank you is it worthwhile for hmrc to consider large-scale Enterprise Integration Services as a dedicated lot separate to although joined up to product development</t>
+          <t>Someone is asking how many slots are available for the face-to-face one-to-one sessions, so we've set aside enough capacity within the week in Birmingham to accommodate around 100 suppliers. Okay, during the course of that week, we'll have five teams available, but we can flex up to six depending on uptake. And, as Mike mentioned before, there's a limit of three representatives for each supplier organization during that week. But it's an opportunity to meet us face to face, to ask us questions, to make suggestions, and hopefully we it can be a mutually beneficial arrangement. Just to reiterate though, any questions that we are asked in that setting, we will be capturing and publishing as part of our responsibility to be fair and transparent to all of the bidders. Thank you. Is it worthwhile for HMRC to consider large-scale Enterprise Integration Services as a dedicated lot, separate to although joined up to product development?</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -4107,20 +4107,20 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>['HMRC', 'Face-to-Face', 'One-to-One', 'Birmingham', 'Flex', 'Mutually Beneficial']</t>
+          <t>['HMRC', 'Face-to-Face', 'Product Development', 'Transparency', 'Fairness']</t>
         </is>
       </c>
       <c r="E115" t="n">
         <v>0.5</v>
       </c>
       <c r="F115" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G115" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H115" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="116">
@@ -4129,17 +4129,17 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>we have considered that as a commercial approach But ultimately we landed on the fact that our technology journey is very much around working to configurable platforms and products so it becomes more about products than it does about lines of business and about lines of service and that's that's how we decided to structure the the framework I I guess it's there's no wrong answer as to how you would want to structure it but because we want to take that product centered approach in the way that we take the transformation forward it seemed to be the most sensible split could you please confirm the SQ date is it the 6th of October with a 30-day return I.E mid-november yeah yeah the 30-day is statutory we we give 30 days for the return of the SQ okay which clouds are hmrc using and expecting to use will product vendor</t>
+          <t>We have considered that as a commercial approach. But ultimately, we landed on the fact that our technology journey is very much around working to configurable platforms and products, so it becomes more about products than it does about lines of business and about lines of service. And that's how we decided to structure the framework. I guess there's no wrong answer as to how you would want to structure it, but because we want to take that product-centered approach in the way that we take the transformation forward, it seemed to be the most sensible split. Could you please confirm the SQ date? Is it the 6th of October with a 30-day return, i.e. mid-November? Yeah, the 30-day is statutory. We give 30 days for the return of the SQ. Okay, which clouds are HMRC using and expecting to use? Will product vendor?</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Product Centered Approach</t>
+          <t>Product Transformation</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>['commercial approach', 'configurable platforms', 'products', 'lines of business', 'lines of service', 'SQ date', 'clouds', 'hmrc']</t>
+          <t>['commercial approach', 'configurable platforms', 'product-centered approach', 'SQ date', 'HMRC']</t>
         </is>
       </c>
       <c r="E116" t="n">
@@ -4152,7 +4152,7 @@
         <v>0.7</v>
       </c>
       <c r="H116" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="117">
@@ -4161,7 +4161,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>clouds also be used servicenow for example or Pega cloud so today at hmrc in terms of infrastructure as a service predominantly uses AWS and azure but as Tom raised in his presentation we want to over time move more away from iwas into platform as a service and software as a service so that wouldn't necessitate the actual vendor software being served from their side of the firewall into our side of the firewall and then configured on our side of the firewall will there be will bespoke performance certificates be required to prove skills and experience in developments I think is the the way to answer that we will come out with more detail on that but we're working through what that would need to look like when it comes to the the Itt okay and just going back sorry there's a question in the room</t>
+          <t>Clouds can also be used for ServiceNow, for example, or Pega Cloud. So, today at HMRC, in terms of Infrastructure as a Service, predominantly uses AWS and Azure. But, as Tom raised in his presentation, we want to over time move more away from IWAS into Platform as a Service and Software as a Service. So, that wouldn't necessitate the actual vendor software being served from their side of the firewall into our side of the firewall and then configured on our side of the firewall. Will there be bespoke performance certificates be required to prove skills and experience in developments? I think that's the way to answer that. We will come out with more detail on that, but we're working through what that would need to look like when it comes to the ITT. Okay, and just going back, sorry, there's a question in the room?</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -4171,17 +4171,17 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>['cloud', 'servicenow', 'Pega', 'AWS', 'azure']</t>
+          <t>['clouds', 'ServiceNow', 'Pega Cloud', 'HMRC', 'IWAS', 'Platform as a Service', 'Software as a Service', 'firewall']</t>
         </is>
       </c>
       <c r="E117" t="n">
         <v>0.5</v>
       </c>
       <c r="F117" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G117" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="H117" t="n">
         <v>0.8</v>
@@ -4193,12 +4193,12 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>you just triggered a question in my head here so Sarah talked about the university that you have in cdia which I think is you know really fundamental to build your skills yet I don't see a budget allocation to that particular task is is there a budget associated with building that out and where would it fit within the Lots so there isn't a a single specified budget as such today you'll have noticed from the the last instructor Slide the expanded one that had detail on it I think there's about 15 million pounds allocated in total two lot five which again is a forecast on what we think we will spend but the way that spend is taken up is largely through commissioning by individual parts of the cdio organization who will commission a particular Academy to suit their needs so for example David Cooper is the primary user of Pega resources so David May commission the creation of a Pega Academy on an ongoing basis and it makes</t>
+          <t>You just triggered a question in my head here, so Sarah talked about the university that you have in CDIA, which I think is really fundamental to build your skills yet I don't see a budget allocation to that particular task. Is there a budget associated with building that out and where would it fit within the Lots? So there isn't a single specified budget as such today. You'll have noticed from the last instructor slide, the expanded one that had detail on it. I think there's about 15 million pounds allocated in total to Lot 5, which again is a forecast on what we think we will spend. But the way that spend is taken up is largely through commissioning by individual parts of the CDIO organization who will commission a particular Academy to suit their needs. So for example, David Cooper is the primary user of Pega resources, so David may commission the creation of a Pega Academy on an ongoing basis and it makes sense.</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>CDIO Academy</t>
+          <t>CDIO budget</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -4216,7 +4216,7 @@
         <v>0.7</v>
       </c>
       <c r="H118" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="119">
@@ -4225,7 +4225,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>sense for us in some ways to almost industrialize that as a process so that as one the next one comes through so that we have that constant throughput of Staff because we know we lose them out of the door as quickly as we've trained them because we can't pay them enough but that industrialization of that process means we'll get to retain more of them potentially just because they love us because we're fantastic people to work but the the volume will start to shape the market too over time as we have more and more skilled individuals in those in those areas so whilst I wouldn't say there's a fixed budget we're forecasting that there's about 15 million pounds that will be allocated to the the technology skills academies and the production of the the 12-week cross training course as that would result in a nano degree so as our existing staff start to move away from Legacy Technologies they can be trained on the Strategic technologies that are being introduced into the business</t>
+          <t>Sense for us in some ways to almost industrialize that as a process, so that as one the next one comes through, so that we have that constant throughput of Staff because we know we lose them out of the door as quickly as we've trained them because we can't pay them enough, but that industrialization of that process means we'll get to retain more of them potentially just because they love us because we're fantastic people to work with. But the volume will start to shape the market too over time, as we have more and more skilled individuals in those areas. So, whilst I wouldn't say there's a fixed budget, we're forecasting that there's about 15 million pounds that will be allocated to the technology skills academies and the production of the 12-week cross training course, as that would result in a nano degree. So, as our existing staff start to move away from Legacy Technologies, they can be trained on the Strategic technologies that are being introduced into the business.</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -4235,7 +4235,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>['Staff', 'Industrialization', 'Training', 'Legacy Technologies', 'Strategic Technologies']</t>
+          <t>['Industrialization', 'Staff', 'Legacy Technologies', 'Strategic Technologies', 'Nano Degree']</t>
         </is>
       </c>
       <c r="E119" t="n">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>hopefully that answers it I think so of course did you want to come in about to come in did you want to come in on that Sarah it's going to say I mean we we obviously do a lot of work on a business as usual basis as well so this isn't just about you know creating capability or learning opportunities for new stuff but this is about existing staff as well about really utilizing the talent that we already have in cdio because yes we are a fantastic place to work and I think we're making it even better you know we've we've got a great learning and career development offer now in cdio and it's really about building that out so that you know it is about then retaining more of our internal talent but also really leverage in our talent as well I think we have Sarah thank you thank you Sarah there's a question in the room hi it's Natalie Gray from</t>
+          <t>Hopefully that answers it. I think so, of course. Did you want to come in? About to come in? Did you want to come in on that, Sarah? It's going to say I mean we, we obviously do a lot of work on a business as usual basis as well, so this isn't just about you know creating capability or learning opportunities for new stuff, but this is about existing staff as well, about really utilizing the talent that we already have in CDIO. Because yes, we are a fantastic place to work and I think we're making it even better. You know, we've we've got a great learning and career development offer now in CDIO and it's really about building that out so that you know it is about then retaining more of our internal talent, but also really leverage in our talent as well. I think we have Sarah. Thank you, thank you Sarah. There's a question in the room. Hi, it's Natalie Gray from...</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -4267,17 +4267,17 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>['talent', 'retention', 'learning', 'career', 'development']</t>
+          <t>['talent', 'retention', 'CDIO', 'learning', 'career']</t>
         </is>
       </c>
       <c r="E120" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F120" t="n">
         <v>0.3</v>
       </c>
       <c r="G120" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="H120" t="n">
         <v>0.2</v>
@@ -4289,7 +4289,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>co-durance here I was just wondering more about the one-to-one sessions in Birmingham just wondering like how long are they and do suppliers that have made the effort to come and see you in Birmingham get more points or yeah just wondering how it works can I just follow on because we have a couple questions online related so you can take them all together so where there's a question about whether there's an agenda for the face-to-face and whether the market engagement days are multi-supplier or individual supplier meetings so if you could take those so the events will be individual one-to-one so each supplier will individually be able to meet with a joint team from ccs and hmrc during those Market engagement sessions there will be no points allocated to attending face-to-face I think we would struggle to get that one past the lawyers but the the opportunity that there will be no agenda because it's an opportunity for you as suppliers to have digested everything that you've heard today reviewed the packs and come to us with any further questions that you</t>
+          <t>I was just wondering more about the one-to-one sessions in Birmingham. How long are they and do suppliers that have made the effort to come and see you in Birmingham get more points? Can I just follow on because we have a couple questions online related? So, is there an agenda for the face-to-face and are the market engagement days multi-supplier or individual supplier meetings? The events will be individual one-to-one, so each supplier will individually be able to meet with a joint team from CCS and HMRC during those Market engagement sessions. There will be no points allocated to attending face-to-face, but the opportunity that there will be no agenda because it's an opportunity for you as suppliers to have digested everything that you've heard today, reviewed the packs and come to us with any further questions that you've had.</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -4299,17 +4299,17 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>['one-to-one', 'Birmingham', 'points', 'agenda', 'multi-supplier']</t>
+          <t>['one-to-one', 'Birmingham', 'CCS', 'HMRC', 'Market Engagement']</t>
         </is>
       </c>
       <c r="E121" t="n">
         <v>0.5</v>
       </c>
       <c r="F121" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G121" t="n">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="H121" t="n">
         <v>0.8</v>
@@ -4321,17 +4321,17 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>might have one of the things that we found throughout tsp is that some of these events have been naturally limited I guess in the questions that have been asked and sometimes that's just about a bit of uncertainty as to how far to go with a question when you've got competitor organizations in the room with you so having the opportunity to ask that in an anonymized setting where nobody knows who's asked what question when it gets published we anticipated would give us greater opportunity to have more open dialogue in terms of the timing we're planning to allocate 45 minutes to each supplier for those face-to-face sessions does that cover all of the aspects of I think so I great all right let's see how are you thinking about content expertise versus Raw DDOT skills as you award lots for example Customs borders requires specialist knowledge to build good services</t>
+          <t>Might have one of the things that we found throughout TSP is that some of these events have been naturally limited, I guess, in the questions that have been asked and sometimes that's just about a bit of uncertainty as to how far to go with a question when you've got competitor organizations in the room with you. So, having the opportunity to ask that in an anonymized setting, where nobody knows who's asked what question when it gets published, we anticipated would give us greater opportunity to have more open dialogue. In terms of the timing, we're planning to allocate 45 minutes to each supplier for those face-to-face sessions. Does that cover all of the aspects of I think so? I great. All right, let's see. How are you thinking about content expertise versus raw DDOT skills as you award lots? For example, Customs Borders requires specialist knowledge to build good services.</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>TSP Events</t>
+          <t>Supplier Sessions</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>['Competitor Organizations', 'Anonymized Setting', '45 Minutes', 'Content Expertise', 'Raw DDOT Skills']</t>
+          <t>['TSP', 'Anonymized Setting', 'Content Expertise', 'Raw DDOT Skills', 'Customs Borders']</t>
         </is>
       </c>
       <c r="E122" t="n">
@@ -4344,7 +4344,7 @@
         <v>0.7</v>
       </c>
       <c r="H122" t="n">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="123">
@@ -4353,17 +4353,17 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>I guess that's probably one more for Jillian and Dean to perhaps take between them foreign yeah someone can help with that so we need people who understand the technologies that we're building in we need people with the skills for example and obviously is sort of Bas and that sort of thing and Technical Architects the Customs knowledge because there are two sorts of technicals in our world the Customs knowledge comes from our selves so we have a a pool what we call it a large pool but a pool of subject matter experts we have a depth of knowledge inside cdio borders and trade so this is what I really mean by it's that combination of internals and externals you know at the end of it I mean partners that we work with become subject matter experts in that narrow field but we wouldn't expect you to come with deep knowledge of CPC code 2783 for</t>
+          <t>I guess that's probably one more for Jillian and Dean to perhaps take between them foreign yeah someone can help with that so we need people who understand the technologies that we're building in. We need people with the skills for example and obviously is sort of Bas and that sort of thing and Technical Architects. The Customs knowledge because there are two sorts of technicals in our world the Customs knowledge comes from our selves so we have a a pool what we call it a large pool but a pool of subject matter experts. We have a depth of knowledge inside cdio borders and trade so this is what I really mean by it's that combination of internals and externals you know at the end of it I mean partners that we work with become subject matter experts in that narrow field but we wouldn't expect you to come with deep knowledge of CPC code 2783 for.</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Technical Architects</t>
+          <t>Customs Knowledge</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>['Jillian', 'Dean', 'Bas', 'Customs', 'CPC code 2783']</t>
+          <t>['Jillian', 'Dean', 'Bas', 'Technical Architects', 'Customs Knowledge']</t>
         </is>
       </c>
       <c r="E123" t="n">
@@ -4385,17 +4385,17 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>example okay that's not going to happen there only are a handful of people in the entire world well that we could have at access to does that help I think so yes thanks Dean Jillian was there anything you would like to add there same as Dean from a digital platform point of view I mean obviously we do more than just the borders and trade program we've got multiple programs and platform team and again you know we've just transitioned from a number of suppliers still who didn't come in with deep hmrc knowledge but we have the intelligent client Leo within the digital platform team who are the hmrc permanent staff as well as the subject matter experts from the business that were with us in programs and projects that we deliver excellent and I think just to expand that a little bit further because of the fact that this is going to be a cross-government framework it'll be up to each department that uses the framework to Define for themselves where the boundary lies between what they want related to content and ddat</t>
+          <t>Example, okay that's not going to happen. There only are a handful of people in the entire world, well that we could have at access to. Does that help? I think so, yes. Thanks, Dean Jillian. Was there anything you would like to add? Same as Dean, from a digital platform point of view, I mean obviously we do more than just the borders and trade program. We've got multiple programs and platform team and again, you know, we've just transitioned from a number of suppliers still who didn't come in with deep hmrc knowledge, but we have the intelligent client Leo within the digital platform team who are the hmrc permanent staff as well as the subject matter experts from the business that were with us in programs and projects that we deliver. Excellent, and I think just to expand that a little bit further, because of the fact that this is going to be a cross-government framework, it'll be up to each department that uses the framework to define for themselves where the boundary lies between what they want related to content and ddat.</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Digital Platform</t>
+          <t>Cross-Government Framework</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>['hmrc', 'borders', 'trade', 'programs', 'platform', 'suppliers', 'intelligent', 'client', 'Leo', 'subject', 'matter', 'experts']</t>
+          <t>['hmrc', 'digital platform', 'content', 'ddat', 'framework']</t>
         </is>
       </c>
       <c r="E124" t="n">
@@ -4417,30 +4417,30 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>you have one down in the front what framework terms are going to be used for the contract framework Public Service public sector contracts what they'd be based on right so the the framework itself is being developed from the the cabinet's office public sector I.T Services contract and it will be augmented with specific content based on the things that we've discussed today now some things are at this moment open to discussion as to how they land and I think Michael will be able to say a little bit more on that but so when we land it it'll be clear as to what information sits at the framework level what sits within a department-specific service specification and what sits within a a call off contract potentially even an enduring call-off contract for the suppliers appointed that we can then start to commission statements of work from</t>
+          <t>You have one down in the front. What framework terms are going to be used for the contract framework? Public Service public sector contracts - what they'd be based on? Right, so the framework itself is being developed from the Cabinet's Office Public Sector I.T Services contract, and it will be augmented with specific content based on the things that we've discussed today. Now, some things are at this moment open to discussion as to how they land, and I think Michael will be able to say a little bit more on that. But so, when we land it, it'll be clear as to what information sits at the framework level, what sits within a department-specific service specification, and what sits within a call-off contract, potentially even an enduring call-off contract for the suppliers appointed, that we can then start to commission statements of work from.</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Public Service Contracts</t>
+          <t>Contract Framework</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>['framework', 'Public Service', 'public sector', 'contracts', "cabinet's office"]</t>
+          <t>['Public Service', 'Public Sector', "Cabinet's Office", 'I.T Services', 'Michael']</t>
         </is>
       </c>
       <c r="E125" t="n">
         <v>0.5</v>
       </c>
       <c r="F125" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G125" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H125" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="126">
@@ -4449,7 +4449,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>I think we're getting into more of a you know horses for courses scenario within ccs and making sure that we have the right contract for the right Lots so we are looking at that and making sure that we have the right terms with each to support each of the types of activity that are going on so I'm not going to say now it's going to be one because because it may be different types as we have in tier three so just it will be what we think and when we go through what will support the framework other customers and suppliers best organizations it will be issued with the ITT with the Itt yeah they'll go out in the acting not with the SQ no they'll go out with the Itt which is normal thank you another question going back to the cloud question for a minute so given that there's an expectation to broaden Beyond AWS in azira what is hmrc's strategic and Technology posture on multi-cloud</t>
+          <t>I think we're getting into more of a "you know" horses for courses scenario within CCS and making sure that we have the right contract for the right Lots so we are looking at that and making sure that we have the right terms with each to support each of the types of activity that are going on. So, I'm not going to say now it's going to be one because because it may be different types as we have in tier three. So, just it will be what we think and when we go through what will support the framework other customers and suppliers best organizations it will be issued with the ITT with the ITT, yeah they'll go out in the acting not with the SQ. No, they'll go out with the ITT which is normal. Thank you. Another question going back to the cloud question for a minute. So, given that there's an expectation to broaden Beyond AWS in Azira, what is HMRC's strategic and Technology posture on multi-cloud?</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -4459,7 +4459,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>['Cloud', 'Multi-Cloud', 'Strategy', 'Technology', 'Posture']</t>
+          <t>['Cloud', 'HMRC', 'AWS', 'Azira', 'Multi-Cloud']</t>
         </is>
       </c>
       <c r="E126" t="n">
@@ -4472,7 +4472,7 @@
         <v>0.7</v>
       </c>
       <c r="H126" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="127">
@@ -4481,7 +4481,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>so I think as Tom covered in his video the shift to the shift to a platforms and services trying to consume them as services so particularly software as a service and platform as a service will will it inevitably mean that and and consuming them in a way you know in a working from that vend from the core product and only customizing as required is will inevitably end up with multiple Solutions being provided across that so so as Phil talked about we have we already have infrastructure a lot of our infrastructures on cloud services but as we adopt more more of a platform-based architecture that will will lead to the adoption of more cloud services from different software providers thank you as more departments join the framework will they all share the same time or will each customer have their own so it will be for each customer to Define for themselves how what they want</t>
+          <t>So, I think, as Tom covered in his video, the shift to a platforms and services, trying to consume them as services, so particularly software as a service and platform as a service, will inevitably mean that consuming them in a way, you know, in a working from that vend from the core product and only customizing as required, is will inevitably end up with multiple Solutions being provided across that. So, as Phil talked about, we have we already have infrastructure a lot of our infrastructures on cloud services, but as we adopt more of a platform-based architecture, that will lead to the adoption of more cloud services from different software providers. Thank you. As more departments join the framework, will they all share the same time or will each customer have their own? So, it will be for each customer to define for themselves how what they want?</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -4513,27 +4513,27 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>to adopt in relation to that yes it would be a call of specific and how they want to apply it or if they want to apply it it's not going to be dictated across the framework this could be a key principle of the call up that hmrc are using and just to look back around on that question about the framework because obviously there's some uncertainty there we're running this as a restricted process specifically because we wanted to release this in waves because if we release the entire thing to the markets at once it will diminish the quality of what we are able to get back from the market so so consequently rather than having to those who might be interested in applying to be on five Lots at once you wouldn't want to stretch your A-Team so thinly in such a short space of time but what that also enables us to do is to release the specific elements of that wave at the time of the wave now when the it the first ITT goes out we will have details that cover the</t>
+          <t>To adopt in relation to that, yes it would be a call of specific and how they want to apply it, or if they want to apply it, it's not going to be dictated across the framework. This could be a key principle of the call up that HMRC are using, and just to look back around on that question about the framework, because obviously there's some uncertainty there. We're running this as a restricted process specifically because we wanted to release this in waves, because if we release the entire thing to the markets at once it will diminish the quality of what we are able to get back from the market. So, consequently, rather than having those who might be interested in applying to be on five lots at once, you wouldn't want to stretch your A-Team so thinly in such a short space of time. But what that also enables us to do is to release the specific elements of that wave at the time of the wave. Now, when the ITT goes out, we will have details that cover the.</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>HMRC Framework</t>
+          <t>HMRC Process</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>['restricted process', 'ITT', 'A-Team', 'wave', 'Lots']</t>
+          <t>['restricted process', 'wave release', 'ITT', 'A-Team']</t>
         </is>
       </c>
       <c r="E128" t="n">
         <v>0.5</v>
       </c>
       <c r="F128" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="G128" t="n">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="H128" t="n">
         <v>0.2</v>
@@ -4545,17 +4545,17 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>entire framework from end to end and then the ITT for wave one will be specific around the services that we'll be consuming in that wave and then similarly for wave two but the actual the legal side of the documents the the contractual Vehicles the framework the call of contracts they will be released as part of the ATT issuance for wave one yeah we we couldn't do that on open and that's where we one of the reasons we upped the touristry from codeurance and one of the themes this morning has been about operating on outcomes based contracts and supplies having skin in the game would those be don't understand correctly working on fixed price terms so again there are a number of commercial models that we could use for outcome-based contracts we're not necessarily tied to fixed price but as well as fixed price you we could</t>
+          <t>Entire framework from end to end, and then the ITT for wave one will be specific around the services that we'll be consuming in that wave, and then similarly for wave two. But the actual legal side of the documents, the contractual vehicles, the framework, the call of contracts, they will be released as part of the ATT issuance for wave one. Yeah, we we couldn't do that on open, and that's where we one of the reasons we upped the touristry from codeurance. And one of the themes this morning has been about operating on outcomes based contracts and supplies having skin in the game. Would those be, don't understand correctly, working on fixed price terms? So again, there are a number of commercial models that we could use for outcome-based contracts, we're not necessarily tied to fixed price, but as well as fixed price, you, we could.</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Outcome-based contracts</t>
+          <t>Contracts &amp; Outcomes</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>['end-to-end', 'ITT', 'framework', 'legal', 'contractual', 'Vehicles', 'ATT', 'codeurance', 'outcomes', 'skin in the game', 'fixed price']</t>
+          <t>['Contracts', 'Outcomes', 'ITT', 'ATT', 'Codeurance', 'Fixed Price']</t>
         </is>
       </c>
       <c r="E129" t="n">
@@ -4568,7 +4568,7 @@
         <v>0.7</v>
       </c>
       <c r="H129" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="130">
@@ -4577,17 +4577,17 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>have models that are based on part fixed and part variable velocity incentivization models or or return on investment models so we plan as part of the hmrc specific elements of that to provide information to the markets as to the types of commercial models we would be looking to use with the options then available for us to put in place on a case-by-case basis just back up again back up to the framework level we're going to give the customers the option to use whatever is right for the project and for them at that point in time that they call off the work any more in the room no okay I think we'll we'll just take maybe one or two more questions maybe one from online once more to see if there's any in the room because they think we're sort of getting close to time now I think which one shall I pick here how will you ensure that the sqs and ITT</t>
+          <t>Have models that are based on part fixed and part variable velocity incentivization models or return on investment models. So, we plan as part of the HMRC specific elements of that to provide information to the markets as to the types of commercial models we would be looking to use with the options then available for us to put in place on a case-by-case basis. Just back up again, back up to the framework level. We're going to give the customers the option to use whatever is right for the project and for them at that point in time that they call off the work. Any more in the room? No? Okay, I think we'll take maybe one or two more questions, maybe one from online once more to see if there's any in the room because they think we're sort of getting close to time now. I think which one shall I pick here? How will you ensure that the SQS and ITT?</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Commercial Models</t>
+          <t>Commercial models</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>['models', 'velocity', 'incentivization', 'investment', 'hmrc', 'framework', 'customers', 'project', 'sqs', 'ITT']</t>
+          <t>['HMRC', 'Framework', 'Customers', 'SQS', 'ITT']</t>
         </is>
       </c>
       <c r="E130" t="n">
@@ -4600,7 +4600,7 @@
         <v>0.7</v>
       </c>
       <c r="H130" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="131">
@@ -4609,24 +4609,24 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>don't unintentionally end up a bias on the score for large incumbent suppliers of hmrc those who participated in the processes that we followed under Tech sourcing program Tech Services Program will remember the the steps that we took to level the playing field to the extent that actually it was quite a a pleasant surprise to see new suppliers enter the HMR hmrc stable so hopefully with that experience it will be evident to the market that we're not specifically wedded to any specific supplier any specific incumbent also the fact that we have framework Lots in which there are multiple opportunities to get onto the framework would in itself indicate that even if incumbent suppliers were to be successful throughout the process it's not just going to be the incumbent suppliers who are going to be on the lot and it's certainly not just incumbent suppliers that will be allocated work through that lot either on the taxi rank</t>
+          <t>Don't unintentionally end up with a bias on the score for large incumbent suppliers of HMRC. Those who participated in the processes that we followed under the Tech Sourcing Program and Tech Services Program will remember the steps that we took to level the playing field. To the extent that it was quite a pleasant surprise to see new suppliers enter the HMRC stable, so hopefully with that experience it will be evident to the market that we're not specifically wedded to any specific supplier or any specific incumbent. Also, the fact that we have framework Lots in which there are multiple opportunities to get onto the framework would in itself indicate that even if incumbent suppliers were to be successful throughout the process, it's not just going to be the incumbent suppliers who are going to be on the Lot, and it's certainly not just incumbent suppliers that will be allocated work through that Lot either on the taxi rank.</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>HMR Hmrc Suppliers</t>
+          <t>HMRC Suppliers</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>['HMR', 'Hmrc', 'Suppliers', 'Tech Sourcing', 'Tech Services']</t>
+          <t>['HMRC', 'Suppliers', 'Tech Sourcing Program', 'Tech Services Program', 'Framework Lots']</t>
         </is>
       </c>
       <c r="E131" t="n">
         <v>0.5</v>
       </c>
       <c r="F131" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="G131" t="n">
         <v>0.7</v>
@@ -4641,17 +4641,17 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>basis or through through competition so wherever possible we'll be looking to to level the playing field using those same mechanisms that we used in Tech sourcing program but one of the things that's important to say as well because this is a framework and not a contract we can't go into the specifics of exactly what that would mean when it comes to assessing transition costs and the 2p implications because we just don't know what they are now where we're procuring for a framework rather than for a contract and when we start to put in place call-offs there will potentially be some of those call-offs where there are 2p implications and transition cost implications and we will start to provide information on those on a case-by-case basis but you could expect that it would follow the same sort of process that we've done in tsp where transition cost wouldn't be taken into account as part of the the scoring of the bid and yes CCS running those and setting out the Esq and supporting the ITT</t>
+          <t>Basis or through competition, so wherever possible we'll be looking to level the playing field using the same mechanisms that we used in the Tech Sourcing Program. But one of the things that's important to say is that, because this is a framework and not a contract, we can't go into the specifics of exactly what that would mean when it comes to assessing transition costs and the 2p implications. Because we just don't know what they are now, where we're procuring for a framework rather than for a contract. And when we start to put in place call-offs, there will potentially be some of those call-offs where there are 2p implications and transition cost implications. And we will start to provide information on those on a case-by-case basis. But you could expect that it would follow the same sort of process that we've done in TSP, where transition cost wouldn't be taken into account as part of the scoring of the bid. And yes, CCS running those and setting out the Esq and supporting the ITT.</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Transition Costs</t>
+          <t>Procurement Framework</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>['Tech', 'Sourcing', 'Program', 'Framework', 'Contract']</t>
+          <t>['transition costs', '2p implications', 'Tech Sourcing Program', 'CCS', 'Esq', 'ITT']</t>
         </is>
       </c>
       <c r="E132" t="n">
@@ -4673,17 +4673,17 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>aspect we will take the bias out of that and look at trying to get that Level Playing Field response we have no understanding of what's happening when we have an understanding but no detail around who the key suppliers are that that they need to keep or want to keep we'll just pull that back and use it and buy it so you I think interestingly as well when we do the evaluations the way we set up the evaluation teams that are often represented of some different parts of the organization so where you might have a supplier that could perhaps create some kind of unconscious bias for one evaluator in one part of the business about wanting to keep them that would absolutely be leveled off by the fact that there are multiple evaluators from multiple parts of the business you may have nothing to do with with that supplier so it's in some ways it's it's self-policing but it's also moderated as well by the commercial team to ensure any traces of bias are removed from the process however unconscious those traces of bias</t>
+          <t>Aspect, we will take the bias out of that and look at trying to get that Level Playing Field response. We have no understanding of what's happening when we have an understanding but no detail around who the key suppliers are that that they need to keep or want to keep. We'll just pull that back and use it and buy it. So, you I think interestingly as well, when we do the evaluations, the way we set up the evaluation teams that are often represented of some different parts of the organization. So, where you might have a supplier that could perhaps create some kind of unconscious bias for one evaluator in one part of the business about wanting to keep them, that would absolutely be leveled off by the fact that there are multiple evaluators from multiple parts of the business you may have nothing to do with with that supplier. So, it's in some ways it's it's self-policing but it's also moderated as well by the commercial team to ensure any traces of bias are removed from the process, however unconscious those traces of bias are.</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Level Playing Field</t>
+          <t>Supplier Evaluation</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>['bias', 'suppliers', 'evaluation', 'unconscious bias', 'commercial team']</t>
+          <t>['bias', 'supplier', 'evaluation', 'unconscious', 'commercial']</t>
         </is>
       </c>
       <c r="E133" t="n">
@@ -4705,17 +4705,17 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>may be I will be able to answer the rest of the slider questions later on yes we're going to take those away and we'll create a spreadsheet with answers to all the questions and put them on the CCS website along with the the presentation deck I think I'll just take I'll take two more because one of them has been asked three times and then another one I think is is a bit more interesting so when working remotely as just mentioned would there be a need to do so at secret classification I guess Julian and Dean may be able to provide a bit more information on this but generally not we don't do very much at secret classification but there are odd occasions where we do have certain interfaces with mod and one or two other organizations where that might happen but yeah it would be definitely trailed and enough time given for</t>
+          <t>May be I will be able to answer the rest of the slider questions later on. Yes, we're going to take those away and we'll create a spreadsheet with answers to all the questions and put them on the CCS website along with the presentation deck. I think I'll just take I'll take two more because one of them has been asked three times and then another one I think is is a bit more interesting. So, when working remotely as just mentioned, would there be a need to do so at secret classification? I guess Julian and Dean may be able to provide a bit more information on this, but generally not. We don't do very much at secret classification, but there are odd occasions where we do have certain interfaces with MOD and one or two other organizations where that might happen, but yeah it would be definitely trailed and enough time given for it.</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Working remotely</t>
+          <t>Remote Working</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>['secret classification', 'mod', 'spreadsheet', 'presentation deck']</t>
+          <t>['classification', 'MOD', 'spreadsheet', 'presentation']</t>
         </is>
       </c>
       <c r="E134" t="n">
@@ -4728,7 +4728,7 @@
         <v>0.7</v>
       </c>
       <c r="H134" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="135">
@@ -4737,7 +4737,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>suppliers to be able to get the accreditations necessary to operate at that level but I guess so that the cross cross-government piece is exactly the same book level and the requirement of the customer there as when needed Jillian or Dean did or Rich I agree Phil no I agree it would depend on the project if something came into that nature and we would give the supplier plenty of warning that that was happening but that's not the norm for what we do certainly in the digital platform team yeah or sensitive stuff we normally use as data isn't it really Jillian sorry didn't I cause across you then yeah yeah it it is I mean there's occasional bits and pieces with us there's certainly some secret data there are some secret elements like risking you know of goods for obvious reasons but again it would be with prior knowledge we wouldn't need the organization to be classified as that you know that we deal with it would be</t>
+          <t>Suppliers need to be able to get the accreditations necessary to operate at that level. I guess the cross-government piece is exactly the same book level and the requirement of the customer there as when needed. Jillian or Dean did or Rich, I agree. Phil, no I agree. It would depend on the project if something came into that nature and we would give the supplier plenty of warning that that was happening, but that's not the norm for what we do, certainly in the digital platform team. Yeah, or sensitive stuff we normally use as data, isn't it really, Jillian? Sorry, didn't I cause across you then? Yeah, yeah it it is. I mean there's occasional bits and pieces with us, there's certainly some secret data, there are some secret elements like risking you know of goods for obvious reasons, but again it would be with prior knowledge we wouldn't need the organization to be classified as that, you know that we deal with it would be with prior knowledge.</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -4747,7 +4747,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>['suppliers', 'accreditations', 'cross-government', 'customer', 'digital platform', 'secret data']</t>
+          <t>['accreditations', 'cross-government', 'customer', 'digital platform', 'secret data', 'secret elements']</t>
         </is>
       </c>
       <c r="E135" t="n">
@@ -4760,7 +4760,7 @@
         <v>0.7</v>
       </c>
       <c r="H135" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="136">
@@ -4769,17 +4769,17 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>an individual level we'd give a lot of notice about that and there's not a lot there is some but not a great deal foreign thanks Dean I think I'll take a final question here how much rating on prices will there be and how will pricing be scored in Itt so to be finalized we're still working on my level of detail and we'll work out how what's what's the importance of pricing across the pieces and work out how we can get the the best commercial value into into the framework early on to help all of our customers get even better commercial value going forward I mean just to expand on The hmrc View on that we we certainly have a perspective that as Lee set out at the beginning the capacity capability and competition are more of the key features for us rather than price specifically</t>
+          <t>An individual level, we'd give a lot of notice about that and there's not a lot there is some, but not a great deal. Foreign, thanks Dean. I think I'll take a final question here: How much rating on prices will there be and how will pricing be scored in Itt? So, to be finalized, we're still working on my level of detail and we'll work out how, what's the importance of pricing across the pieces and work out how we can get the best commercial value into the framework early on to help all of our customers get even better commercial value going forward. I mean, just to expand on The hmrc View on that, we certainly have a perspective that, as Lee set out at the beginning, the capacity, capability and competition are more of the key features for us rather than price specifically.</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Pricing Scoring</t>
+          <t>Pricing Framework</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>['notice', 'rating', 'prices', 'commercial value', 'hmrc view']</t>
+          <t>['pricing', 'framework', 'commercial value', 'capacity', 'capability', 'competition']</t>
         </is>
       </c>
       <c r="E136" t="n">
@@ -4792,7 +4792,7 @@
         <v>0.7</v>
       </c>
       <c r="H136" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="137">
@@ -4801,27 +4801,27 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>but clearly price is important and given the economic pressures that exist now we understand that it's it's going to be a challenge when bits are put in to maintain that competitiveness of pricing for the headline rate cards that that get produced but we will be looking to get the the highest quality solutions to to meet our needs at the the best possible price whilst recognizing that the cheapest isn't always the best great I'll just pause for any final from the room questions comments no one bar left on the microphone so okay great you have promised there are more on slido that we I just just don't think we have enough time to get to everything but you guys will review those questions and provide the answers so rest assured that even if you didn't get to ask it or have it answered now they will be answered and addressed</t>
+          <t>But, clearly, price is important and given the economic pressures that exist now, we understand that it's going to be a challenge when bits are put in to maintain that competitiveness of pricing for the headline rate cards that get produced. But, we will be looking to get the highest quality solutions to meet our needs at the best possible price, whilst recognizing that the cheapest isn't always the best. Great. I'll just pause for any final questions or comments from the room. No one bar left on the microphone, so okay great. You have promised there are more on Slido that we just don't think we have enough time to get to everything, but you guys will review those questions and provide the answers. So, rest assured that even if you didn't get to ask it or have it answered now, they will be answered and addressed.</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Price competitiveness</t>
+          <t>Pricing Solutions</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>['price', 'economic pressures', 'quality', 'cheapest']</t>
+          <t>['economic pressures', 'price', 'quality', 'competitiveness', 'Slido']</t>
         </is>
       </c>
       <c r="E137" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F137" t="n">
         <v>0.3</v>
       </c>
       <c r="G137" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="H137" t="n">
         <v>0.2</v>
@@ -4833,27 +4833,27 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>I just want to I guess take a little bit of time to say thank you lee it looks like you're up to say thank you first yeah so just to wrap up I just want to say thanks to Tech UK first of all for hosting and facilitating thank you for all of the speakers I hope you found that informative I've certainly learned some things about Dallas and hmrc from the last couple of hours I hope you all did as well and and most of all thank you all for attending both the people that have come in today as well as those online from all of the questions and thanks so much for the people to answering those to show a lot of interest and to be honest we're wasting our time like we don't get a lot of interest in this framework it's no good as suppliers don't want to be on it you've seen the next steps there is opportunity we do not have the Monopoly on good ideas we have time between now and October to hear your thoughts and feedback if you've got that there's a number of channels to reach out please take advantage of those</t>
+          <t>I just want to I guess take a little bit of time to say thank you, Lee. It looks like you're up to say thank you first. Yeah, so just to wrap up, I just want to say thanks to Tech UK first of all for hosting and facilitating. Thank you for all of the speakers. I hope you found that informative. I've certainly learned some things about Dallas and HMRC from the last couple of hours. I hope you all did as well. And most of all, thank you all for attending, both the people that have come in today as well as those online from all of the questions. And thanks so much for the people to answering those. To show a lot of interest and to be honest, we're wasting our time. Like, we don't get a lot of interest in this framework. It's no good as suppliers don't want to be on it. You've seen the next steps. There is opportunity. We do not have the Monopoly on good ideas. We have time between now and October to hear your thoughts and feedback. If you've got that, there's a number of channels to reach out. Please take advantage of those.</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Thank You</t>
+          <t>Thanking Attendees</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>['Tech UK', 'Dallas', 'HMRC', 'Suppliers', 'Monopoly', 'October']</t>
+          <t>['Tech UK', 'Dallas', 'HMRC', 'Suppliers', 'Monopoly']</t>
         </is>
       </c>
       <c r="E138" t="n">
         <v>0.8</v>
       </c>
       <c r="F138" t="n">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="G138" t="n">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="H138" t="n">
         <v>0.2</v>
@@ -4865,27 +4865,27 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>one-to-one sessions we've learned from TSP that sometimes these open forums aren't always the best places to to get really good ideas so please if you're interested take up those one-to-one sessions and yeah thanks again for this I think we'll be hanging around for about the next half hour or so so if anybody wants to say hello we will be here and thanks again foreign just the final word of thanks from me for those who have joined us online and for those in the room and have a great day thank you</t>
+          <t>One-to-one sessions, we've learned from TSP that sometimes these open forums aren't always the best places to get really good ideas, so please, if you're interested, take up those one-to-one sessions. Yeah, thanks again for this. I think we'll be hanging around for about the next half hour or so, so if anybody wants to say hello, we will be here. And thanks again for joining us online and for those in the room. Have a great day. Thank you.</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>One-to-one sessions</t>
+          <t>Open forums</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>['TSP', 'open forums', 'ideas', 'one-to-one sessions', 'hello']</t>
+          <t>['one-to-one', 'TSP', 'ideas', 'sessions', 'hello']</t>
         </is>
       </c>
       <c r="E139" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F139" t="n">
         <v>0.2</v>
       </c>
       <c r="G139" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="H139" t="n">
         <v>0.2</v>

</xml_diff>